<commit_message>
Foto Analyses (Fotos vs Illustrations)
</commit_message>
<xml_diff>
--- a/Townes vs Broad.xlsx
+++ b/Townes vs Broad.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robin\Dropbox\Mein PC (Gemeinsamer-PC)\Documents\GitHub\Ichneumonidae\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolevonallmen/Documents/GitHub/Ichneumonidae/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{78A455F9-8CB2-4D43-9AAA-4B8C5209F6B0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED5D163D-B841-634C-9F11-6565857F0A66}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{63889695-902D-49DB-8829-7F5E2426025F}"/>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{81081F8A-FCD8-4DA0-BE37-B9CD844CA9B2}"/>
+    <workbookView xWindow="-200" yWindow="620" windowWidth="18100" windowHeight="14180" activeTab="2" xr2:uid="{63889695-902D-49DB-8829-7F5E2426025F}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" activeTab="2" xr2:uid="{81081F8A-FCD8-4DA0-BE37-B9CD844CA9B2}"/>
   </bookViews>
   <sheets>
     <sheet name="TOWNES" sheetId="1" r:id="rId1"/>
@@ -23,21 +23,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="870" uniqueCount="531">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="886" uniqueCount="546">
   <si>
     <t>Epelaspis</t>
   </si>
@@ -1317,9 +1308,6 @@
     <t>Goedartia</t>
   </si>
   <si>
-    <t>Amblyjppa</t>
-  </si>
-  <si>
     <t>Callajoppa</t>
   </si>
   <si>
@@ -1630,6 +1618,54 @@
   </si>
   <si>
     <t>Specimen</t>
+  </si>
+  <si>
+    <t>ISCHNOJOPPINI</t>
+  </si>
+  <si>
+    <t>Ischnojoppa</t>
+  </si>
+  <si>
+    <t>Compsophorus</t>
+  </si>
+  <si>
+    <t>COMPSOPHORINI</t>
+  </si>
+  <si>
+    <t>CERATOJOPPINI</t>
+  </si>
+  <si>
+    <t>Ceratojoppa</t>
+  </si>
+  <si>
+    <t>CLYPEODROMINI</t>
+  </si>
+  <si>
+    <t>Clypeodromus</t>
+  </si>
+  <si>
+    <t>CTENOCALINI</t>
+  </si>
+  <si>
+    <t>Ctenocalus</t>
+  </si>
+  <si>
+    <t>JOPPOCRYPTINI</t>
+  </si>
+  <si>
+    <t>Eccoptosage</t>
+  </si>
+  <si>
+    <t>Hymenura</t>
+  </si>
+  <si>
+    <t>Oedicephalus</t>
+  </si>
+  <si>
+    <t>Aethioplites</t>
+  </si>
+  <si>
+    <t>in Ichneumoninae key als Tribe</t>
   </si>
 </sst>
 </file>
@@ -1680,7 +1716,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1723,6 +1759,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1736,7 +1784,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1766,6 +1814,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -2082,32 +2132,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3325E525-F9CE-447C-9C7C-9E0C969A72AA}">
   <dimension ref="A1:R96"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="S12" sqref="S12"/>
     </sheetView>
     <sheetView workbookViewId="1">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" customWidth="1"/>
-    <col min="5" max="5" width="17.140625" customWidth="1"/>
-    <col min="6" max="6" width="17.7109375" customWidth="1"/>
-    <col min="7" max="7" width="17.5703125" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" customWidth="1"/>
-    <col min="9" max="9" width="14.7109375" customWidth="1"/>
-    <col min="11" max="12" width="13.42578125" customWidth="1"/>
-    <col min="13" max="13" width="17.5703125" customWidth="1"/>
-    <col min="14" max="15" width="14.7109375" customWidth="1"/>
-    <col min="16" max="16" width="17.140625" customWidth="1"/>
-    <col min="17" max="17" width="14.85546875" customWidth="1"/>
+    <col min="1" max="1" width="14.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5" customWidth="1"/>
+    <col min="3" max="3" width="18.5" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" customWidth="1"/>
+    <col min="5" max="5" width="17.1640625" customWidth="1"/>
+    <col min="6" max="6" width="17.6640625" customWidth="1"/>
+    <col min="7" max="7" width="17.5" customWidth="1"/>
+    <col min="8" max="8" width="14.5" customWidth="1"/>
+    <col min="9" max="9" width="14.6640625" customWidth="1"/>
+    <col min="11" max="12" width="13.5" customWidth="1"/>
+    <col min="13" max="13" width="17.5" customWidth="1"/>
+    <col min="14" max="15" width="14.6640625" customWidth="1"/>
+    <col min="16" max="16" width="17.1640625" customWidth="1"/>
+    <col min="17" max="17" width="14.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>150</v>
       </c>
@@ -2115,7 +2165,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>147</v>
       </c>
@@ -2123,7 +2173,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>145</v>
       </c>
@@ -2131,7 +2181,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>143</v>
       </c>
@@ -2139,7 +2189,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>114</v>
       </c>
@@ -2147,10 +2197,10 @@
         <v>115</v>
       </c>
       <c r="Q5" t="s">
-        <v>529</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
         <v>18</v>
       </c>
@@ -2198,10 +2248,10 @@
         <v>0</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>530</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C7" s="22" t="s">
         <v>0</v>
       </c>
@@ -2243,7 +2293,7 @@
       </c>
       <c r="R7" s="24"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C8" s="22" t="s">
         <v>1</v>
       </c>
@@ -2284,7 +2334,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C9" s="19" t="s">
         <v>2</v>
       </c>
@@ -2323,7 +2373,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C10" s="19" t="s">
         <v>3</v>
       </c>
@@ -2354,7 +2404,7 @@
       <c r="N10" s="12"/>
       <c r="O10" s="12"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C11" s="19" t="s">
         <v>4</v>
       </c>
@@ -2385,7 +2435,7 @@
       <c r="N11" s="12"/>
       <c r="O11" s="12"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C12" s="19" t="s">
         <v>5</v>
       </c>
@@ -2416,7 +2466,7 @@
       <c r="N12" s="12"/>
       <c r="O12" s="12"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C13" s="19" t="s">
         <v>6</v>
       </c>
@@ -2445,7 +2495,7 @@
       <c r="N13" s="12"/>
       <c r="O13" s="12"/>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C14" s="19" t="s">
         <v>7</v>
       </c>
@@ -2470,7 +2520,7 @@
       <c r="N14" s="12"/>
       <c r="O14" s="12"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C15" s="19" t="s">
         <v>8</v>
       </c>
@@ -2495,7 +2545,7 @@
       <c r="N15" s="12"/>
       <c r="O15" s="12"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C16" s="19" t="s">
         <v>9</v>
       </c>
@@ -2518,7 +2568,7 @@
       <c r="N16" s="12"/>
       <c r="O16" s="12"/>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C17" s="12" t="s">
         <v>10</v>
       </c>
@@ -2541,7 +2591,7 @@
       <c r="N17" s="12"/>
       <c r="O17" s="12"/>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C18" s="19" t="s">
         <v>11</v>
       </c>
@@ -2564,7 +2614,7 @@
       <c r="N18" s="12"/>
       <c r="O18" s="12"/>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C19" s="19" t="s">
         <v>12</v>
       </c>
@@ -2585,7 +2635,7 @@
       <c r="N19" s="12"/>
       <c r="O19" s="12"/>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C20" s="19" t="s">
         <v>13</v>
       </c>
@@ -2604,7 +2654,7 @@
       <c r="N20" s="12"/>
       <c r="O20" s="12"/>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C21" s="19" t="s">
         <v>14</v>
       </c>
@@ -2623,7 +2673,7 @@
       <c r="N21" s="12"/>
       <c r="O21" s="12"/>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C22" s="19" t="s">
         <v>15</v>
       </c>
@@ -2640,7 +2690,7 @@
       <c r="N22" s="12"/>
       <c r="O22" s="12"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C23" s="19" t="s">
         <v>16</v>
       </c>
@@ -2657,7 +2707,7 @@
       <c r="N23" s="12"/>
       <c r="O23" s="12"/>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C24" s="22" t="s">
         <v>17</v>
       </c>
@@ -2674,11 +2724,11 @@
       <c r="N24" s="12"/>
       <c r="O24" s="12"/>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>114</v>
       </c>
@@ -2688,7 +2738,7 @@
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B27" s="2" t="s">
         <v>131</v>
       </c>
@@ -2704,7 +2754,7 @@
       <c r="N27" s="4"/>
       <c r="O27" s="4"/>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B28" s="2" t="s">
         <v>139</v>
       </c>
@@ -2720,7 +2770,7 @@
       <c r="N28" s="4"/>
       <c r="O28" s="4"/>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B29" s="7" t="s">
         <v>133</v>
       </c>
@@ -2736,7 +2786,7 @@
       <c r="N29" s="4"/>
       <c r="O29" s="4"/>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B30" s="7" t="s">
         <v>126</v>
       </c>
@@ -2752,7 +2802,7 @@
       <c r="N30" s="4"/>
       <c r="O30" s="4"/>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B31" s="7" t="s">
         <v>127</v>
       </c>
@@ -2768,7 +2818,7 @@
       <c r="N31" s="4"/>
       <c r="O31" s="4"/>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B32" s="2" t="s">
         <v>123</v>
       </c>
@@ -2784,7 +2834,7 @@
       <c r="N32" s="4"/>
       <c r="O32" s="4"/>
     </row>
-    <row r="33" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B33" s="7" t="s">
         <v>128</v>
       </c>
@@ -2803,7 +2853,7 @@
       <c r="N33" s="4"/>
       <c r="O33" s="4"/>
     </row>
-    <row r="34" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B34" s="7" t="s">
         <v>134</v>
       </c>
@@ -2819,7 +2869,7 @@
       <c r="N34" s="4"/>
       <c r="O34" s="4"/>
     </row>
-    <row r="35" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B35" s="9" t="s">
         <v>119</v>
       </c>
@@ -2838,7 +2888,7 @@
       <c r="N35" s="4"/>
       <c r="O35" s="4"/>
     </row>
-    <row r="36" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B36" s="7" t="s">
         <v>124</v>
       </c>
@@ -2854,7 +2904,7 @@
       <c r="N36" s="4"/>
       <c r="O36" s="4"/>
     </row>
-    <row r="37" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B37" s="7" t="s">
         <v>141</v>
       </c>
@@ -2870,7 +2920,7 @@
       <c r="N37" s="4"/>
       <c r="O37" s="4"/>
     </row>
-    <row r="38" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B38" s="9" t="s">
         <v>117</v>
       </c>
@@ -2889,7 +2939,7 @@
       <c r="N38" s="4"/>
       <c r="O38" s="4"/>
     </row>
-    <row r="39" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B39" s="9" t="s">
         <v>118</v>
       </c>
@@ -2908,7 +2958,7 @@
       <c r="N39" s="4"/>
       <c r="O39" s="4"/>
     </row>
-    <row r="40" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B40" s="2" t="s">
         <v>136</v>
       </c>
@@ -2924,7 +2974,7 @@
       <c r="N40" s="4"/>
       <c r="O40" s="4"/>
     </row>
-    <row r="41" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B41" s="9" t="s">
         <v>122</v>
       </c>
@@ -2943,7 +2993,7 @@
       <c r="N41" s="4"/>
       <c r="O41" s="4"/>
     </row>
-    <row r="42" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B42" s="7" t="s">
         <v>129</v>
       </c>
@@ -2959,7 +3009,7 @@
       <c r="N42" s="4"/>
       <c r="O42" s="4"/>
     </row>
-    <row r="43" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B43" s="9" t="s">
         <v>140</v>
       </c>
@@ -2978,7 +3028,7 @@
       <c r="N43" s="4"/>
       <c r="O43" s="4"/>
     </row>
-    <row r="44" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B44" s="7" t="s">
         <v>125</v>
       </c>
@@ -2994,7 +3044,7 @@
       <c r="N44" s="4"/>
       <c r="O44" s="4"/>
     </row>
-    <row r="45" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B45" s="9" t="s">
         <v>120</v>
       </c>
@@ -3004,28 +3054,28 @@
       <c r="F45" s="4"/>
       <c r="G45" s="4"/>
     </row>
-    <row r="46" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B46" s="2" t="s">
         <v>132</v>
       </c>
       <c r="F46" s="4"/>
       <c r="G46" s="26"/>
     </row>
-    <row r="47" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B47" s="7" t="s">
         <v>137</v>
       </c>
       <c r="F47" s="4"/>
       <c r="G47" s="4"/>
     </row>
-    <row r="48" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B48" s="2" t="s">
         <v>130</v>
       </c>
       <c r="F48" s="4"/>
       <c r="G48" s="26"/>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B49" s="9" t="s">
         <v>138</v>
       </c>
@@ -3033,12 +3083,12 @@
         <v>373</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B50" s="2" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B51" s="9" t="s">
         <v>121</v>
       </c>
@@ -3046,7 +3096,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>114</v>
       </c>
@@ -3054,7 +3104,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B54" s="1" t="s">
         <v>18</v>
       </c>
@@ -3104,7 +3154,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C55" s="2" t="s">
         <v>152</v>
       </c>
@@ -3151,7 +3201,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C56" t="s">
         <v>153</v>
       </c>
@@ -3190,7 +3240,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C57" s="5" t="s">
         <v>154</v>
       </c>
@@ -3225,7 +3275,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C58" t="s">
         <v>155</v>
       </c>
@@ -3254,7 +3304,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C59" s="5" t="s">
         <v>156</v>
       </c>
@@ -3283,7 +3333,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C60" t="s">
         <v>157</v>
       </c>
@@ -3312,7 +3362,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C61" t="s">
         <v>158</v>
       </c>
@@ -3341,7 +3391,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C62" s="5" t="s">
         <v>159</v>
       </c>
@@ -3370,7 +3420,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C63" t="s">
         <v>160</v>
       </c>
@@ -3399,7 +3449,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C64" t="s">
         <v>161</v>
       </c>
@@ -3425,7 +3475,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="65" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="65" spans="3:16" x14ac:dyDescent="0.2">
       <c r="C65" t="s">
         <v>162</v>
       </c>
@@ -3451,7 +3501,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="66" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="66" spans="3:16" x14ac:dyDescent="0.2">
       <c r="D66" s="5" t="s">
         <v>175</v>
       </c>
@@ -3471,7 +3521,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="67" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="67" spans="3:16" x14ac:dyDescent="0.2">
       <c r="D67" s="5" t="s">
         <v>176</v>
       </c>
@@ -3491,7 +3541,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="68" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="68" spans="3:16" x14ac:dyDescent="0.2">
       <c r="D68" s="5" t="s">
         <v>177</v>
       </c>
@@ -3511,7 +3561,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="69" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="69" spans="3:16" x14ac:dyDescent="0.2">
       <c r="D69" s="5" t="s">
         <v>178</v>
       </c>
@@ -3528,7 +3578,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="70" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="70" spans="3:16" x14ac:dyDescent="0.2">
       <c r="D70" s="5" t="s">
         <v>179</v>
       </c>
@@ -3545,7 +3595,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="71" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="71" spans="3:16" x14ac:dyDescent="0.2">
       <c r="D71" s="5" t="s">
         <v>180</v>
       </c>
@@ -3562,7 +3612,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="72" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="72" spans="3:16" x14ac:dyDescent="0.2">
       <c r="D72" s="5" t="s">
         <v>181</v>
       </c>
@@ -3576,7 +3626,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="73" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="73" spans="3:16" x14ac:dyDescent="0.2">
       <c r="D73" s="5" t="s">
         <v>182</v>
       </c>
@@ -3587,7 +3637,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="74" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="74" spans="3:16" x14ac:dyDescent="0.2">
       <c r="D74" s="5" t="s">
         <v>183</v>
       </c>
@@ -3598,7 +3648,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="75" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="75" spans="3:16" x14ac:dyDescent="0.2">
       <c r="D75" s="5" t="s">
         <v>184</v>
       </c>
@@ -3609,7 +3659,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="76" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="76" spans="3:16" x14ac:dyDescent="0.2">
       <c r="D76" s="5" t="s">
         <v>185</v>
       </c>
@@ -3620,7 +3670,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="77" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="77" spans="3:16" x14ac:dyDescent="0.2">
       <c r="D77" s="5" t="s">
         <v>186</v>
       </c>
@@ -3631,7 +3681,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="78" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="78" spans="3:16" x14ac:dyDescent="0.2">
       <c r="D78" s="5" t="s">
         <v>187</v>
       </c>
@@ -3639,7 +3689,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="79" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="79" spans="3:16" x14ac:dyDescent="0.2">
       <c r="D79" s="5" t="s">
         <v>188</v>
       </c>
@@ -3647,7 +3697,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="80" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="80" spans="3:16" x14ac:dyDescent="0.2">
       <c r="D80" s="6" t="s">
         <v>189</v>
       </c>
@@ -3655,7 +3705,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="81" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D81" s="5" t="s">
         <v>190</v>
       </c>
@@ -3663,7 +3713,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="82" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D82" s="5" t="s">
         <v>191</v>
       </c>
@@ -3671,7 +3721,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="83" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D83" t="s">
         <v>192</v>
       </c>
@@ -3679,7 +3729,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="84" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D84" s="5" t="s">
         <v>193</v>
       </c>
@@ -3687,7 +3737,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="85" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D85" t="s">
         <v>194</v>
       </c>
@@ -3695,7 +3745,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="86" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D86" s="5" t="s">
         <v>195</v>
       </c>
@@ -3703,7 +3753,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="87" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D87" s="5" t="s">
         <v>196</v>
       </c>
@@ -3711,47 +3761,47 @@
         <v>270</v>
       </c>
     </row>
-    <row r="88" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D88" s="5" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="89" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D89" s="5" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="90" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D90" s="5" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="91" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D91" s="5" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="92" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D92" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="93" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D93" s="5" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="94" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D94" s="5" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="95" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D95" s="5" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="96" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D96" s="5" t="s">
         <v>205</v>
       </c>
@@ -3774,1571 +3824,1571 @@
     </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="e">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
         <v>495</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="8" t="s">
         <v>496</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="8" t="s">
         <v>497</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" s="8" t="s">
         <v>498</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" s="8" t="s">
         <v>499</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" s="8" t="s">
         <v>500</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" s="8" t="s">
         <v>501</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" s="8" t="s">
         <v>502</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" s="8" t="s">
         <v>503</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" s="8" t="s">
         <v>504</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" s="8" t="s">
         <v>505</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="e">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" s="8" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="8" t="s">
         <v>509</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="8" t="s">
         <v>510</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" s="8" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="s">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" s="8" t="s">
         <v>512</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="8" t="s">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" s="8" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="8" t="s">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" s="8" t="s">
         <v>514</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="8" t="s">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" s="8" t="s">
         <v>515</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="8" t="s">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" s="8" t="s">
         <v>516</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="8" t="s">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" s="8" t="s">
         <v>517</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="8" t="s">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" s="8" t="s">
         <v>518</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="8" t="s">
-        <v>519</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" s="8" t="e">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" s="8" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" s="8" t="e">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" s="8" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" s="8" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" s="8" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" s="8" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" s="8" t="s">
-        <v>525</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" s="8" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" s="8" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" s="8" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" s="8" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" s="8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" s="8" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" s="8" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" s="8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" s="8" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" s="8" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" s="8" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" s="8" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" s="8" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" s="8" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" s="8" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" s="8" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" s="8" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" s="8" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" s="8" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" s="8" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" s="8" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" s="8" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" s="8" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" s="8" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" s="8" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" s="8" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" s="8" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" s="8" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" s="8" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" s="8" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" s="8" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" s="8" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" s="8" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" s="8" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" s="8" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" s="8" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" s="8" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" s="8" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74" s="8" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" s="8" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" s="8" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77" s="8" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78" s="8" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79" s="8" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80" s="8" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81" s="8" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A82" s="8" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83" s="8" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A84" s="8" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A85" s="8" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A86" s="8" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A87" s="8" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A88" s="8" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A89" s="8" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A89" s="8" t="s">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A90" s="8" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A90" s="8" t="s">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A91" s="8" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A91" s="8" t="s">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A92" s="8" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A92" s="8" t="s">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A93" s="8" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A93" s="8" t="s">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A94" s="8" t="s">
         <v>442</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A94" s="8" t="s">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A95" s="8" t="s">
         <v>443</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A95" s="8" t="s">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A96" s="8" t="s">
         <v>444</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A96" s="8" t="s">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A97" s="8" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A97" s="8" t="s">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A98" s="8" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A98" s="8" t="s">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A99" s="8" t="s">
         <v>447</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A99" s="8" t="s">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A100" s="8" t="s">
         <v>448</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A100" s="8" t="s">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A101" s="8" t="s">
         <v>449</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A101" s="8" t="s">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A102" s="8" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A102" s="8" t="s">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A103" s="8" t="s">
         <v>451</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A103" s="8" t="s">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A104" s="8" t="s">
         <v>452</v>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A104" s="8" t="s">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A105" s="8" t="s">
         <v>453</v>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A105" s="8" t="s">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A106" s="8" t="s">
         <v>454</v>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A106" s="8" t="s">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A107" s="8" t="s">
         <v>455</v>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A107" s="8" t="s">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A108" s="8" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A108" s="8" t="s">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A109" s="8" t="s">
         <v>457</v>
       </c>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A109" s="8" t="s">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A110" s="8" t="s">
         <v>458</v>
       </c>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A110" s="8" t="s">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A111" s="8" t="s">
         <v>459</v>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A111" s="8" t="s">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A112" s="8" t="s">
         <v>460</v>
       </c>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A112" s="8" t="s">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A113" s="8" t="s">
         <v>461</v>
       </c>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A113" s="8" t="s">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A114" s="8" t="s">
         <v>462</v>
       </c>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A114" s="8" t="s">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A115" s="8" t="s">
         <v>463</v>
       </c>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A115" s="8" t="s">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A116" s="8" t="s">
         <v>464</v>
       </c>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A116" s="8" t="s">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A117" s="8" t="s">
         <v>465</v>
       </c>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A117" s="8" t="s">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A118" s="8" t="s">
         <v>466</v>
       </c>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A118" s="8" t="s">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A119" s="8" t="s">
         <v>467</v>
       </c>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A119" s="8" t="s">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A120" s="8" t="s">
         <v>468</v>
       </c>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A120" s="8" t="s">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A121" s="8" t="s">
         <v>469</v>
       </c>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A121" s="8" t="s">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A122" s="8" t="s">
         <v>470</v>
       </c>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A122" s="8" t="s">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A123" s="8" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A123" s="8" t="s">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A124" s="8" t="s">
         <v>472</v>
       </c>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A124" s="8" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A125" s="8" t="e">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A126" s="8" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A127" s="8" t="s">
         <v>477</v>
       </c>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A127" s="8" t="s">
+    <row r="128" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A128" s="8" t="s">
         <v>478</v>
       </c>
     </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A128" s="8" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A129" s="8" t="e">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A130" s="8" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A131" s="8" t="e">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A132" s="8" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A133" s="8" t="s">
         <v>482</v>
       </c>
     </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A133" s="8" t="s">
+    <row r="134" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A134" s="8" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A134" s="8" t="s">
+    <row r="135" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A135" s="8" t="s">
         <v>484</v>
       </c>
     </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A135" s="8" t="s">
+    <row r="136" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A136" s="8" t="s">
         <v>485</v>
       </c>
     </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A136" s="8" t="s">
+    <row r="137" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A137" s="8" t="s">
         <v>486</v>
       </c>
     </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A137" s="8" t="s">
+    <row r="138" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A138" s="8" t="s">
         <v>487</v>
       </c>
     </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A138" s="8" t="s">
+    <row r="139" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A139" s="8" t="s">
         <v>488</v>
       </c>
     </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A139" s="8" t="s">
+    <row r="140" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A140" s="8" t="s">
         <v>489</v>
       </c>
     </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A140" s="8" t="s">
+    <row r="141" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A141" s="8" t="s">
         <v>490</v>
       </c>
     </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A141" s="8" t="s">
+    <row r="142" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A142" s="8" t="s">
         <v>491</v>
       </c>
     </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A142" s="8" t="s">
+    <row r="143" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A143" s="8" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A143" s="8" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A144" s="8" t="e">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A145" s="8" t="e">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A146" s="8" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A147" s="8" t="e">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A148" s="8" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A149" s="8" t="e">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A150" s="8" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A151" s="8" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A152" s="8" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A152" s="8" t="s">
+    <row r="153" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A153" s="8" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A153" s="8" t="s">
+    <row r="154" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A154" s="8" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A154" s="8" t="s">
+    <row r="155" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A155" s="8" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A155" s="8" t="s">
+    <row r="156" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A156" s="8" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A156" s="8" t="s">
+    <row r="157" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A157" s="8" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A157" s="8" t="s">
+    <row r="158" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A158" s="8" t="s">
         <v>433</v>
       </c>
     </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A158" s="8" t="s">
+    <row r="159" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A159" s="8" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A159" s="8" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A160" s="8" t="e">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A161" s="8" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A162" s="8" t="s">
         <v>474</v>
       </c>
     </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A162" s="8" t="s">
+    <row r="163" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A163" s="8" t="s">
         <v>475</v>
       </c>
     </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A163" s="8" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A164" s="8" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A165" s="8" t="e">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A166" s="8" t="e">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A167" s="8" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A168" s="8" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A169" s="8" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A170" s="8" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A171" s="8" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A172" s="8" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A173" s="8" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A174" s="8" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A175" s="8" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A176" s="8" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A177" s="8" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A178" s="8" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A179" s="8" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A180" s="8" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A181" s="8" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A182" s="8" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A183" s="8" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A184" s="8" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A185" s="8" t="e">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A186" s="8" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A187" s="8" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A188" s="8" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A189" s="8" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A190" s="8" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A191" s="8" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A192" s="8" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A193" s="8" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A194" s="8" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A195" s="8" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A196" s="8" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A197" s="8" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A198" s="8" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A199" s="8" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A200" s="8" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A201" s="8" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A202" s="8" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="203" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A203" s="8" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="204" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A204" s="8" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="205" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A205" s="8" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="206" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A206" s="8" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="207" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A207" s="8" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="208" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A208" s="8" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="209" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A209" s="8" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="210" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A210" s="8" t="e">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="211" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A211" s="8" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="212" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A212" s="8" t="e">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="213" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A213" s="8" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="214" spans="1:1" x14ac:dyDescent="0.25">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="214" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A214" s="8" t="e">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="215" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A215" s="8" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="216" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A216" s="8" t="e">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="217" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A217" s="8" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="218" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A218" s="4"/>
     </row>
-    <row r="219" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A219" s="4"/>
     </row>
-    <row r="220" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A220" s="4"/>
     </row>
-    <row r="221" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A221" s="4"/>
     </row>
-    <row r="222" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A222" s="4"/>
     </row>
-    <row r="223" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A223" s="4"/>
     </row>
-    <row r="224" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A224" s="4"/>
     </row>
-    <row r="225" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A225" s="4"/>
     </row>
-    <row r="226" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A226" s="4"/>
     </row>
-    <row r="227" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A227" s="4"/>
     </row>
-    <row r="228" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A228" s="4"/>
     </row>
-    <row r="229" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A229" s="4"/>
     </row>
-    <row r="230" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A230" s="4"/>
     </row>
-    <row r="231" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A231" s="4"/>
     </row>
-    <row r="232" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A232" s="4"/>
     </row>
-    <row r="233" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A233" s="4"/>
     </row>
-    <row r="234" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A234" s="4"/>
     </row>
-    <row r="235" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A235" s="4"/>
     </row>
-    <row r="236" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A236" s="4"/>
     </row>
-    <row r="237" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A237" s="4"/>
     </row>
-    <row r="238" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A238" s="4"/>
     </row>
-    <row r="239" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A239" s="4"/>
     </row>
-    <row r="240" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A240" s="4"/>
     </row>
-    <row r="241" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A241" s="4"/>
     </row>
-    <row r="242" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A242" s="4"/>
     </row>
-    <row r="243" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A243" s="4"/>
     </row>
-    <row r="244" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A244" s="4"/>
     </row>
-    <row r="245" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A245" s="4"/>
     </row>
-    <row r="246" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A246" s="4"/>
     </row>
-    <row r="247" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A247" s="4"/>
     </row>
-    <row r="248" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A248" s="4"/>
     </row>
-    <row r="249" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A249" s="4"/>
     </row>
-    <row r="250" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A250" s="4"/>
     </row>
-    <row r="251" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A251" s="4"/>
     </row>
-    <row r="252" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A252" s="4"/>
     </row>
-    <row r="253" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A253" s="4"/>
     </row>
-    <row r="254" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A254" s="4"/>
     </row>
-    <row r="255" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A255" s="4"/>
     </row>
-    <row r="256" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A256" s="4"/>
     </row>
-    <row r="257" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A257" s="4"/>
     </row>
-    <row r="258" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A258" s="4"/>
     </row>
-    <row r="259" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A259" s="4"/>
     </row>
-    <row r="260" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A260" s="4"/>
     </row>
-    <row r="261" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A261" s="4"/>
     </row>
-    <row r="262" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A262" s="4"/>
     </row>
-    <row r="263" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A263" s="4"/>
     </row>
-    <row r="264" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A264" s="4"/>
     </row>
-    <row r="265" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A265" s="4"/>
     </row>
-    <row r="266" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A266" s="4"/>
     </row>
-    <row r="267" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A267" s="4"/>
     </row>
-    <row r="268" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A268" s="4"/>
     </row>
-    <row r="269" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A269" s="4"/>
     </row>
-    <row r="270" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A270" s="4"/>
     </row>
-    <row r="271" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A271" s="4"/>
     </row>
-    <row r="272" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A272" s="4"/>
     </row>
-    <row r="273" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A273" s="4"/>
     </row>
-    <row r="274" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A274" s="4"/>
     </row>
-    <row r="275" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A275" s="4"/>
     </row>
-    <row r="276" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A276" s="4"/>
     </row>
-    <row r="277" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A277" s="4"/>
     </row>
-    <row r="278" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A278" s="4"/>
     </row>
-    <row r="279" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A279" s="4"/>
     </row>
-    <row r="280" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A280" s="4"/>
     </row>
-    <row r="281" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A281" s="4"/>
     </row>
-    <row r="282" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A282" s="4"/>
     </row>
-    <row r="283" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A283" s="4"/>
     </row>
-    <row r="284" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A284" s="4"/>
     </row>
-    <row r="285" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A285" s="4"/>
     </row>
-    <row r="286" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A286" s="4"/>
     </row>
-    <row r="287" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A287" s="4"/>
     </row>
-    <row r="288" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A288" s="4"/>
     </row>
-    <row r="289" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A289" s="4"/>
     </row>
-    <row r="290" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A290" s="4"/>
     </row>
-    <row r="291" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A291" s="4"/>
     </row>
-    <row r="292" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A292" s="4"/>
     </row>
-    <row r="293" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A293" s="4"/>
     </row>
-    <row r="294" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A294" s="4"/>
     </row>
-    <row r="295" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A295" s="4"/>
     </row>
-    <row r="296" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A296" s="4"/>
     </row>
-    <row r="297" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A297" s="4"/>
     </row>
-    <row r="298" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A298" s="4"/>
     </row>
-    <row r="299" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A299" s="4"/>
     </row>
-    <row r="300" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A300" s="4"/>
     </row>
-    <row r="301" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A301" s="4"/>
     </row>
-    <row r="302" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A302" s="4"/>
     </row>
-    <row r="303" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A303" s="4"/>
     </row>
-    <row r="304" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A304" s="4"/>
     </row>
-    <row r="305" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A305" s="4"/>
     </row>
-    <row r="306" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A306" s="4"/>
     </row>
-    <row r="307" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A307" s="4"/>
     </row>
-    <row r="308" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A308" s="4"/>
     </row>
-    <row r="309" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A309" s="4"/>
     </row>
-    <row r="310" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A310" s="4"/>
     </row>
-    <row r="311" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A311" s="4"/>
     </row>
-    <row r="312" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A312" s="4"/>
     </row>
-    <row r="313" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A313" s="4"/>
     </row>
-    <row r="314" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A314" s="4"/>
     </row>
-    <row r="315" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A315" s="4"/>
     </row>
-    <row r="316" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A316" s="4"/>
     </row>
-    <row r="317" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A317" s="4"/>
     </row>
-    <row r="318" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A318" s="4"/>
     </row>
-    <row r="319" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A319" s="4"/>
     </row>
-    <row r="320" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A320" s="4"/>
     </row>
-    <row r="321" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A321" s="4"/>
     </row>
-    <row r="322" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A322" s="4"/>
     </row>
-    <row r="323" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A323" s="4"/>
     </row>
-    <row r="324" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A324" s="4"/>
     </row>
-    <row r="325" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A325" s="4"/>
     </row>
-    <row r="326" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A326" s="4"/>
     </row>
-    <row r="327" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A327" s="4"/>
     </row>
-    <row r="328" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A328" s="4"/>
     </row>
-    <row r="329" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A329" s="4"/>
     </row>
-    <row r="330" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A330" s="4"/>
     </row>
-    <row r="331" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A331" s="4"/>
     </row>
-    <row r="332" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A332" s="4"/>
     </row>
-    <row r="333" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A333" s="4"/>
     </row>
-    <row r="334" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A334" s="4"/>
     </row>
-    <row r="335" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A335" s="4"/>
     </row>
-    <row r="336" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A336" s="4"/>
     </row>
-    <row r="337" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A337" s="4"/>
     </row>
-    <row r="338" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A338" s="4"/>
     </row>
-    <row r="339" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A339" s="4"/>
     </row>
-    <row r="340" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A340" s="4"/>
     </row>
-    <row r="341" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A341" s="4"/>
     </row>
-    <row r="342" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A342" s="4"/>
     </row>
-    <row r="343" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A343" s="4"/>
     </row>
-    <row r="344" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A344" s="4"/>
     </row>
-    <row r="345" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A345" s="4"/>
     </row>
-    <row r="346" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A346" s="4"/>
     </row>
-    <row r="347" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A347" s="4"/>
     </row>
-    <row r="348" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A348" s="4"/>
     </row>
-    <row r="349" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A349" s="4"/>
     </row>
-    <row r="350" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A350" s="4"/>
     </row>
-    <row r="351" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A351" s="4"/>
     </row>
-    <row r="352" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A352" s="4"/>
     </row>
-    <row r="353" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A353" s="4"/>
     </row>
-    <row r="354" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A354" s="4"/>
     </row>
-    <row r="355" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A355" s="4"/>
     </row>
-    <row r="356" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A356" s="4"/>
     </row>
-    <row r="357" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A357" s="4"/>
     </row>
-    <row r="358" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A358" s="4"/>
     </row>
-    <row r="359" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A359" s="4"/>
     </row>
-    <row r="360" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A360" s="4"/>
     </row>
-    <row r="361" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A361" s="4"/>
     </row>
-    <row r="362" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A362" s="4"/>
     </row>
-    <row r="363" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A363" s="4"/>
     </row>
-    <row r="364" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A364" s="4"/>
     </row>
-    <row r="365" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A365" s="4"/>
     </row>
-    <row r="366" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A366" s="4"/>
     </row>
-    <row r="367" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A367" s="4"/>
     </row>
-    <row r="368" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A368" s="4"/>
     </row>
-    <row r="369" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A369" s="4"/>
     </row>
-    <row r="370" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A370" s="4"/>
     </row>
-    <row r="371" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A371" s="4"/>
     </row>
-    <row r="372" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A372" s="4"/>
     </row>
-    <row r="373" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A373" s="4"/>
     </row>
-    <row r="374" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A374" s="4"/>
     </row>
-    <row r="375" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A375" s="4"/>
     </row>
-    <row r="376" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A376" s="4"/>
     </row>
-    <row r="377" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A377" s="4"/>
     </row>
   </sheetData>
@@ -5348,31 +5398,31 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EED08F7F-A003-4C3B-8646-FC85C271AAFB}">
-  <dimension ref="A1:N162"/>
+  <dimension ref="A1:Q162"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A25" sqref="A1:K1048576"/>
+    <sheetView tabSelected="1" topLeftCell="G41" workbookViewId="0">
+      <selection activeCell="L57" sqref="L57"/>
     </sheetView>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="1">
-      <selection activeCell="B97" sqref="B97"/>
+    <sheetView tabSelected="1" topLeftCell="B42" workbookViewId="1">
+      <selection activeCell="I61" sqref="I61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="15"/>
-    <col min="2" max="2" width="18.5703125" style="12" customWidth="1"/>
-    <col min="3" max="3" width="19.140625" style="12" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" style="12" customWidth="1"/>
-    <col min="5" max="5" width="20.28515625" style="12" customWidth="1"/>
+    <col min="1" max="1" width="11.5" style="15"/>
+    <col min="2" max="2" width="18.5" style="12" customWidth="1"/>
+    <col min="3" max="3" width="19.1640625" style="12" customWidth="1"/>
+    <col min="4" max="4" width="16.5" style="12" customWidth="1"/>
+    <col min="5" max="5" width="20.33203125" style="12" customWidth="1"/>
     <col min="6" max="6" width="21" style="12" customWidth="1"/>
-    <col min="7" max="7" width="17.140625" style="12" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" style="12"/>
-    <col min="9" max="9" width="15.42578125" style="12" customWidth="1"/>
-    <col min="10" max="10" width="16.140625" style="12" customWidth="1"/>
-    <col min="11" max="11" width="17.140625" style="12" customWidth="1"/>
+    <col min="7" max="7" width="17.1640625" style="12" customWidth="1"/>
+    <col min="8" max="8" width="11.5" style="12"/>
+    <col min="9" max="9" width="15.5" style="12" customWidth="1"/>
+    <col min="10" max="10" width="16.1640625" style="12" customWidth="1"/>
+    <col min="11" max="11" width="17.1640625" style="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
         <v>150</v>
       </c>
@@ -5380,7 +5430,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="s">
         <v>147</v>
       </c>
@@ -5388,7 +5438,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
         <v>145</v>
       </c>
@@ -5396,7 +5446,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="15" t="s">
         <v>143</v>
       </c>
@@ -5404,12 +5454,12 @@
         <v>355</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B6" s="12" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="15" t="s">
         <v>143</v>
       </c>
@@ -5417,30 +5467,33 @@
         <v>356</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B11" s="12" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="29" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B16" s="12" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B16" s="11" t="s">
         <v>386</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C16" s="12" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B18" s="12" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" s="15" t="s">
         <v>143</v>
       </c>
@@ -5448,20 +5501,20 @@
         <v>358</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B20" s="11" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="M23" s="4"/>
       <c r="N23" s="4"/>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="M24" s="4"/>
       <c r="N24" s="4"/>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" s="15" t="s">
         <v>143</v>
       </c>
@@ -5469,15 +5522,15 @@
         <v>359</v>
       </c>
       <c r="C25" s="12" t="s">
+        <v>522</v>
+      </c>
+      <c r="D25" s="12" t="s">
         <v>523</v>
-      </c>
-      <c r="D25" s="12" t="s">
-        <v>524</v>
       </c>
       <c r="M25" s="4"/>
       <c r="N25" s="4"/>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B26" s="15" t="s">
         <v>114</v>
       </c>
@@ -5488,10 +5541,13 @@
         <v>374</v>
       </c>
       <c r="E26" s="18"/>
+      <c r="G26" s="8" t="s">
+        <v>521</v>
+      </c>
       <c r="M26" s="4"/>
       <c r="N26" s="10"/>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="C27" s="14" t="s">
         <v>131</v>
       </c>
@@ -5501,10 +5557,11 @@
       <c r="E27" s="18" t="s">
         <v>381</v>
       </c>
+      <c r="G27" s="8"/>
       <c r="M27" s="4"/>
       <c r="N27" s="10"/>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="C28" s="14" t="s">
         <v>139</v>
       </c>
@@ -5514,10 +5571,11 @@
       <c r="E28" s="18" t="s">
         <v>379</v>
       </c>
+      <c r="G28"/>
       <c r="M28" s="4"/>
       <c r="N28" s="10"/>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="C29" s="14" t="s">
         <v>365</v>
       </c>
@@ -5530,7 +5588,7 @@
       <c r="M29" s="4"/>
       <c r="N29" s="10"/>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="C30" s="14" t="s">
         <v>126</v>
       </c>
@@ -5543,7 +5601,7 @@
       <c r="M30" s="4"/>
       <c r="N30" s="10"/>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="C31" s="14" t="s">
         <v>366</v>
       </c>
@@ -5556,7 +5614,7 @@
       <c r="M31" s="4"/>
       <c r="N31" s="10"/>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="C32" s="14" t="s">
         <v>123</v>
       </c>
@@ -5569,7 +5627,7 @@
       <c r="M32" s="4"/>
       <c r="N32" s="10"/>
     </row>
-    <row r="33" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C33" s="14" t="s">
         <v>367</v>
       </c>
@@ -5580,7 +5638,7 @@
       <c r="M33" s="4"/>
       <c r="N33" s="10"/>
     </row>
-    <row r="34" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C34" s="14" t="s">
         <v>368</v>
       </c>
@@ -5593,7 +5651,7 @@
       <c r="M34" s="4"/>
       <c r="N34" s="10"/>
     </row>
-    <row r="35" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C35" s="14" t="s">
         <v>124</v>
       </c>
@@ -5606,7 +5664,7 @@
       <c r="M35" s="4"/>
       <c r="N35" s="10"/>
     </row>
-    <row r="36" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C36" s="14" t="s">
         <v>369</v>
       </c>
@@ -5619,7 +5677,7 @@
       <c r="M36" s="4"/>
       <c r="N36" s="10"/>
     </row>
-    <row r="37" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C37" s="14" t="s">
         <v>136</v>
       </c>
@@ -5630,7 +5688,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="38" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C38" s="14" t="s">
         <v>370</v>
       </c>
@@ -5641,7 +5699,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="39" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C39" s="14" t="s">
         <v>371</v>
       </c>
@@ -5650,7 +5708,7 @@
       </c>
       <c r="E39" s="18"/>
     </row>
-    <row r="40" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C40" s="14" t="s">
         <v>132</v>
       </c>
@@ -5661,7 +5719,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="41" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C41" s="14" t="s">
         <v>372</v>
       </c>
@@ -5672,7 +5730,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="42" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C42" s="14" t="s">
         <v>130</v>
       </c>
@@ -5683,7 +5741,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="43" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C43" s="13" t="s">
         <v>68</v>
       </c>
@@ -5694,7 +5752,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="44" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C44" s="20" t="s">
         <v>135</v>
       </c>
@@ -5705,7 +5763,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="45" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:14" x14ac:dyDescent="0.2">
       <c r="D45" s="10" t="s">
         <v>323</v>
       </c>
@@ -5713,7 +5771,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="46" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:14" x14ac:dyDescent="0.2">
       <c r="D46" s="11" t="s">
         <v>377</v>
       </c>
@@ -5721,7 +5779,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="47" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:14" x14ac:dyDescent="0.2">
       <c r="D47" s="12" t="s">
         <v>354</v>
       </c>
@@ -5729,7 +5787,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="48" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:14" x14ac:dyDescent="0.2">
       <c r="D48" s="12" t="s">
         <v>153</v>
       </c>
@@ -5737,7 +5795,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.2">
       <c r="D49" s="12" t="s">
         <v>162</v>
       </c>
@@ -5745,7 +5803,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.2">
       <c r="D50" s="12" t="s">
         <v>194</v>
       </c>
@@ -5753,7 +5811,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A55" s="15" t="s">
         <v>143</v>
       </c>
@@ -5761,429 +5819,620 @@
         <v>360</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B56" s="15" t="s">
         <v>114</v>
       </c>
       <c r="C56" s="12" t="s">
+        <v>534</v>
+      </c>
+      <c r="D56" s="12" t="s">
+        <v>533</v>
+      </c>
+      <c r="E56" s="12" t="s">
+        <v>536</v>
+      </c>
+      <c r="F56" s="12" t="s">
+        <v>538</v>
+      </c>
+      <c r="G56" s="12" t="s">
         <v>418</v>
       </c>
-      <c r="D56" s="12" t="s">
+      <c r="H56" s="12" t="s">
         <v>420</v>
       </c>
-      <c r="E56" s="12" t="s">
+      <c r="I56" s="12" t="s">
         <v>421</v>
       </c>
-      <c r="F56" s="12" t="s">
+      <c r="J56" s="12" t="s">
         <v>422</v>
       </c>
-      <c r="G56" s="12" t="s">
+      <c r="K56" s="12" t="s">
+        <v>530</v>
+      </c>
+      <c r="L56" s="12" t="s">
+        <v>540</v>
+      </c>
+      <c r="M56" s="12" t="s">
         <v>423</v>
       </c>
-      <c r="H56" s="12" t="s">
+      <c r="N56" s="12" t="s">
         <v>424</v>
       </c>
-      <c r="I56" s="12" t="s">
+      <c r="O56" s="12" t="s">
+        <v>480</v>
+      </c>
+      <c r="P56" s="12" t="s">
+        <v>506</v>
+      </c>
+      <c r="Q56" s="12" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="57" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B57" s="15"/>
+      <c r="C57" s="14" t="s">
+        <v>535</v>
+      </c>
+      <c r="D57" s="14" t="s">
+        <v>532</v>
+      </c>
+      <c r="E57" s="14" t="s">
+        <v>537</v>
+      </c>
+      <c r="F57" s="14" t="s">
+        <v>539</v>
+      </c>
+      <c r="G57" s="14" t="s">
+        <v>419</v>
+      </c>
+      <c r="H57" s="14" t="s">
+        <v>425</v>
+      </c>
+      <c r="I57" s="12" t="s">
+        <v>526</v>
+      </c>
+      <c r="J57" s="30" t="s">
+        <v>473</v>
+      </c>
+      <c r="K57" s="14" t="s">
+        <v>531</v>
+      </c>
+      <c r="L57" s="14" t="s">
+        <v>541</v>
+      </c>
+      <c r="M57" s="12" t="s">
+        <v>476</v>
+      </c>
+      <c r="N57" s="12" t="s">
+        <v>479</v>
+      </c>
+      <c r="O57" s="30" t="s">
         <v>481</v>
       </c>
-      <c r="J56" s="12" t="s">
+      <c r="P57" s="12" t="s">
         <v>507</v>
       </c>
-      <c r="K56" s="12" t="s">
+      <c r="Q57" s="14" t="s">
         <v>520</v>
       </c>
-      <c r="L56" s="8" t="s">
-        <v>522</v>
-      </c>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B57" s="15"/>
-      <c r="C57" s="12" t="s">
-        <v>419</v>
-      </c>
-      <c r="D57" s="12" t="s">
-        <v>425</v>
-      </c>
-      <c r="E57" s="12" t="s">
+    </row>
+    <row r="58" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B58" s="15"/>
+      <c r="I58" s="12" t="s">
         <v>426</v>
       </c>
-      <c r="F57" s="12" t="s">
+      <c r="J58" s="12" t="s">
         <v>474</v>
       </c>
-      <c r="G57" s="12" t="s">
+      <c r="M58" s="14" t="s">
         <v>477</v>
       </c>
-      <c r="H57" s="12" t="s">
-        <v>480</v>
-      </c>
-      <c r="I57" s="12" t="s">
+      <c r="N58" s="14" t="s">
+        <v>543</v>
+      </c>
+      <c r="O58" s="12" t="s">
         <v>482</v>
       </c>
-      <c r="J57" s="12" t="s">
+      <c r="P58" s="12" t="s">
         <v>508</v>
       </c>
-      <c r="K57" s="12" t="s">
-        <v>521</v>
-      </c>
-      <c r="L57" s="8"/>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B58" s="15"/>
-      <c r="E58" s="12" t="s">
+      <c r="Q58" s="12"/>
+    </row>
+    <row r="59" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B59" s="15"/>
+      <c r="I59" s="12" t="s">
         <v>427</v>
       </c>
-      <c r="F58" s="12" t="s">
+      <c r="J59" s="14" t="s">
+        <v>544</v>
+      </c>
+      <c r="M59" s="12" t="s">
+        <v>478</v>
+      </c>
+      <c r="N59" s="12"/>
+      <c r="O59" s="30" t="s">
+        <v>483</v>
+      </c>
+      <c r="P59" s="12" t="s">
+        <v>509</v>
+      </c>
+      <c r="Q59" s="12"/>
+    </row>
+    <row r="60" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B60" s="15"/>
+      <c r="I60" s="12" t="s">
+        <v>428</v>
+      </c>
+      <c r="J60" s="14" t="s">
         <v>475</v>
       </c>
-      <c r="G58" s="12" t="s">
-        <v>478</v>
-      </c>
-      <c r="I58" s="12" t="s">
-        <v>483</v>
-      </c>
-      <c r="J58" s="12" t="s">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B59" s="15"/>
-      <c r="E59" s="12" t="s">
-        <v>428</v>
-      </c>
-      <c r="F59" s="12" t="s">
-        <v>476</v>
-      </c>
-      <c r="G59" s="12" t="s">
-        <v>479</v>
-      </c>
-      <c r="I59" s="12" t="s">
+      <c r="M60" s="12"/>
+      <c r="N60" s="12"/>
+      <c r="O60" s="12" t="s">
         <v>484</v>
       </c>
-      <c r="J59" s="12" t="s">
+      <c r="P60" s="12" t="s">
         <v>510</v>
       </c>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B60" s="15"/>
-      <c r="E60" s="12" t="s">
+      <c r="Q60" s="12"/>
+    </row>
+    <row r="61" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B61" s="15"/>
+      <c r="I61" s="30" t="s">
         <v>429</v>
       </c>
-      <c r="F60" s="12" t="s">
+      <c r="J61" s="12" t="s">
+        <v>435</v>
+      </c>
+      <c r="M61" s="12"/>
+      <c r="N61" s="12"/>
+      <c r="O61" s="12" t="s">
+        <v>485</v>
+      </c>
+      <c r="P61" s="12" t="s">
+        <v>511</v>
+      </c>
+      <c r="Q61" s="12"/>
+    </row>
+    <row r="62" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B62" s="15"/>
+      <c r="I62" s="12" t="s">
+        <v>430</v>
+      </c>
+      <c r="J62" s="30" t="s">
         <v>436</v>
       </c>
-      <c r="I60" s="12" t="s">
-        <v>485</v>
-      </c>
-      <c r="J60" s="12" t="s">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B61" s="15"/>
-      <c r="E61" s="12" t="s">
-        <v>430</v>
-      </c>
-      <c r="F61" s="12" t="s">
+      <c r="M62" s="12"/>
+      <c r="N62" s="12"/>
+      <c r="O62" s="30" t="s">
+        <v>486</v>
+      </c>
+      <c r="P62" s="12" t="s">
+        <v>512</v>
+      </c>
+      <c r="Q62" s="12"/>
+    </row>
+    <row r="63" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B63" s="15"/>
+      <c r="I63" s="12" t="s">
+        <v>431</v>
+      </c>
+      <c r="J63" s="12" t="s">
         <v>437</v>
       </c>
-      <c r="I61" s="12" t="s">
-        <v>486</v>
-      </c>
-      <c r="J61" s="12" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B62" s="15"/>
-      <c r="E62" s="12" t="s">
-        <v>431</v>
-      </c>
-      <c r="F62" s="12" t="s">
+      <c r="M63" s="12"/>
+      <c r="N63" s="12"/>
+      <c r="O63" s="12" t="s">
+        <v>487</v>
+      </c>
+      <c r="P63" s="12" t="s">
+        <v>513</v>
+      </c>
+      <c r="Q63" s="12"/>
+    </row>
+    <row r="64" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B64" s="15"/>
+      <c r="I64" s="12" t="s">
+        <v>432</v>
+      </c>
+      <c r="J64" s="12" t="s">
         <v>438</v>
       </c>
-      <c r="I62" s="12" t="s">
-        <v>487</v>
-      </c>
-      <c r="J62" s="12" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B63" s="15"/>
-      <c r="E63" s="12" t="s">
-        <v>432</v>
-      </c>
-      <c r="F63" s="12" t="s">
+      <c r="M64" s="12"/>
+      <c r="N64" s="12"/>
+      <c r="O64" s="12" t="s">
+        <v>488</v>
+      </c>
+      <c r="P64" s="14" t="s">
+        <v>514</v>
+      </c>
+      <c r="Q64" s="12"/>
+    </row>
+    <row r="65" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B65" s="15"/>
+      <c r="I65" s="12" t="s">
+        <v>433</v>
+      </c>
+      <c r="J65" s="14" t="s">
         <v>439</v>
       </c>
-      <c r="I63" s="12" t="s">
-        <v>488</v>
-      </c>
-      <c r="J63" s="12" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B64" s="15"/>
-      <c r="E64" s="12" t="s">
-        <v>433</v>
-      </c>
-      <c r="F64" s="12" t="s">
+      <c r="M65" s="12"/>
+      <c r="N65" s="12"/>
+      <c r="O65" s="12" t="s">
+        <v>489</v>
+      </c>
+      <c r="P65" s="12" t="s">
+        <v>515</v>
+      </c>
+      <c r="Q65" s="12"/>
+    </row>
+    <row r="66" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B66" s="15"/>
+      <c r="I66" s="12" t="s">
+        <v>434</v>
+      </c>
+      <c r="J66" s="12" t="s">
         <v>440</v>
       </c>
-      <c r="I64" s="12" t="s">
-        <v>489</v>
-      </c>
-      <c r="J64" s="12" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="65" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B65" s="15"/>
-      <c r="E65" s="12" t="s">
-        <v>434</v>
-      </c>
-      <c r="F65" s="12" t="s">
+      <c r="M66" s="12"/>
+      <c r="N66" s="12"/>
+      <c r="O66" s="12" t="s">
+        <v>490</v>
+      </c>
+      <c r="P66" s="12" t="s">
+        <v>516</v>
+      </c>
+      <c r="Q66" s="12"/>
+    </row>
+    <row r="67" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B67" s="15"/>
+      <c r="J67" s="12" t="s">
         <v>441</v>
       </c>
-      <c r="I65" s="12" t="s">
-        <v>490</v>
-      </c>
-      <c r="J65" s="12" t="s">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="66" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B66" s="15"/>
-      <c r="E66" s="12" t="s">
-        <v>435</v>
-      </c>
-      <c r="F66" s="12" t="s">
+      <c r="M67" s="12"/>
+      <c r="N67" s="12"/>
+      <c r="O67" s="12" t="s">
+        <v>491</v>
+      </c>
+      <c r="P67" s="12" t="s">
+        <v>517</v>
+      </c>
+      <c r="Q67" s="12"/>
+    </row>
+    <row r="68" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B68" s="15"/>
+      <c r="J68" s="12" t="s">
         <v>442</v>
       </c>
-      <c r="I66" s="12" t="s">
-        <v>491</v>
-      </c>
-      <c r="J66" s="12" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="67" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B67" s="15"/>
-      <c r="F67" s="12" t="s">
+      <c r="M68" s="12"/>
+      <c r="N68" s="12"/>
+      <c r="O68" s="12" t="s">
+        <v>492</v>
+      </c>
+      <c r="P68" s="12" t="s">
+        <v>518</v>
+      </c>
+      <c r="Q68" s="12"/>
+    </row>
+    <row r="69" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B69" s="15"/>
+      <c r="J69" s="12" t="s">
         <v>443</v>
       </c>
-      <c r="I67" s="12" t="s">
-        <v>492</v>
-      </c>
-      <c r="J67" s="12" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="68" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B68" s="15"/>
-      <c r="F68" s="12" t="s">
+      <c r="M69" s="12"/>
+      <c r="N69" s="12"/>
+      <c r="O69" s="12" t="s">
+        <v>493</v>
+      </c>
+      <c r="P69" s="12"/>
+      <c r="Q69" s="12"/>
+    </row>
+    <row r="70" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B70" s="15"/>
+      <c r="J70" s="12" t="s">
         <v>444</v>
       </c>
-      <c r="I68" s="12" t="s">
-        <v>493</v>
-      </c>
-      <c r="J68" s="12" t="s">
-        <v>519</v>
-      </c>
-    </row>
-    <row r="69" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B69" s="15"/>
-      <c r="F69" s="12" t="s">
+      <c r="M70" s="12"/>
+      <c r="N70" s="12"/>
+      <c r="O70" s="12" t="s">
+        <v>494</v>
+      </c>
+      <c r="P70" s="12"/>
+      <c r="Q70" s="12"/>
+    </row>
+    <row r="71" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="J71" s="12" t="s">
         <v>445</v>
       </c>
-      <c r="I69" s="12" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="70" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B70" s="15"/>
-      <c r="F70" s="12" t="s">
+      <c r="M71" s="12"/>
+      <c r="N71" s="12"/>
+      <c r="O71" s="12" t="s">
+        <v>495</v>
+      </c>
+      <c r="P71" s="12"/>
+      <c r="Q71" s="12"/>
+    </row>
+    <row r="72" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="J72" s="12" t="s">
         <v>446</v>
       </c>
-      <c r="I70" s="12" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="71" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="F71" s="12" t="s">
+      <c r="M72" s="12"/>
+      <c r="N72" s="12"/>
+      <c r="O72" s="12" t="s">
+        <v>496</v>
+      </c>
+      <c r="P72" s="12"/>
+      <c r="Q72" s="12"/>
+    </row>
+    <row r="73" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="J73" s="30" t="s">
         <v>447</v>
       </c>
-      <c r="I71" s="12" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="72" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="F72" s="12" t="s">
+      <c r="M73" s="12"/>
+      <c r="N73" s="12"/>
+      <c r="O73" s="12" t="s">
+        <v>497</v>
+      </c>
+      <c r="P73" s="12"/>
+      <c r="Q73" s="12"/>
+    </row>
+    <row r="74" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="J74" s="12" t="s">
         <v>448</v>
       </c>
-      <c r="I72" s="12" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="73" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="F73" s="12" t="s">
+      <c r="M74" s="12"/>
+      <c r="N74" s="12"/>
+      <c r="O74" s="12" t="s">
+        <v>498</v>
+      </c>
+      <c r="P74" s="12"/>
+      <c r="Q74" s="12"/>
+    </row>
+    <row r="75" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="J75" s="30" t="s">
         <v>449</v>
       </c>
-      <c r="I73" s="12" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="74" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="F74" s="12" t="s">
+      <c r="M75" s="12"/>
+      <c r="N75" s="12"/>
+      <c r="O75" s="12" t="s">
+        <v>499</v>
+      </c>
+      <c r="P75" s="12"/>
+      <c r="Q75" s="12"/>
+    </row>
+    <row r="76" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="J76" s="12" t="s">
         <v>450</v>
       </c>
-      <c r="I74" s="12" t="s">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="75" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="F75" s="12" t="s">
+      <c r="M76" s="12"/>
+      <c r="N76" s="12"/>
+      <c r="O76" s="12" t="s">
+        <v>500</v>
+      </c>
+      <c r="P76" s="12"/>
+      <c r="Q76" s="12"/>
+    </row>
+    <row r="77" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="J77" s="12" t="s">
         <v>451</v>
       </c>
-      <c r="I75" s="12" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="76" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="F76" s="12" t="s">
+      <c r="M77" s="12"/>
+      <c r="N77" s="12"/>
+      <c r="O77" s="12" t="s">
+        <v>501</v>
+      </c>
+      <c r="P77" s="12"/>
+      <c r="Q77" s="12"/>
+    </row>
+    <row r="78" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="J78" s="30" t="s">
         <v>452</v>
       </c>
-      <c r="I76" s="12" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="77" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="F77" s="12" t="s">
+      <c r="M78" s="12"/>
+      <c r="N78" s="12"/>
+      <c r="O78" s="30" t="s">
+        <v>502</v>
+      </c>
+      <c r="P78" s="12"/>
+      <c r="Q78" s="12"/>
+    </row>
+    <row r="79" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="J79" s="14" t="s">
         <v>453</v>
       </c>
-      <c r="I77" s="12" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="78" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="F78" s="12" t="s">
+      <c r="M79" s="12"/>
+      <c r="N79" s="12"/>
+      <c r="O79" s="12" t="s">
+        <v>503</v>
+      </c>
+      <c r="P79" s="12"/>
+      <c r="Q79" s="12"/>
+    </row>
+    <row r="80" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="J80" s="14" t="s">
+        <v>542</v>
+      </c>
+      <c r="M80" s="12"/>
+      <c r="N80" s="12"/>
+      <c r="O80" s="12" t="s">
+        <v>504</v>
+      </c>
+      <c r="P80" s="12"/>
+      <c r="Q80" s="12"/>
+    </row>
+    <row r="81" spans="10:17" x14ac:dyDescent="0.2">
+      <c r="J81" s="14" t="s">
         <v>454</v>
       </c>
-      <c r="I78" s="12" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="79" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="F79" s="12" t="s">
+      <c r="M81" s="12"/>
+      <c r="N81" s="12"/>
+      <c r="O81" s="12" t="s">
+        <v>505</v>
+      </c>
+      <c r="P81" s="12"/>
+      <c r="Q81" s="12"/>
+    </row>
+    <row r="82" spans="10:17" x14ac:dyDescent="0.2">
+      <c r="J82" s="12" t="s">
         <v>455</v>
       </c>
-      <c r="I79" s="12" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="80" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="F80" s="12" t="s">
+      <c r="L82" s="12"/>
+      <c r="M82" s="12"/>
+      <c r="N82" s="12"/>
+      <c r="O82" s="12"/>
+    </row>
+    <row r="83" spans="10:17" x14ac:dyDescent="0.2">
+      <c r="J83" s="12" t="s">
         <v>456</v>
       </c>
-      <c r="I80" s="12" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="81" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F81" s="12" t="s">
+      <c r="L83" s="12"/>
+      <c r="M83" s="12"/>
+      <c r="N83" s="12"/>
+      <c r="O83" s="12"/>
+    </row>
+    <row r="84" spans="10:17" x14ac:dyDescent="0.2">
+      <c r="J84" s="12" t="s">
         <v>457</v>
       </c>
-      <c r="I81" s="12" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="82" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F82" s="12" t="s">
+      <c r="L84" s="12"/>
+      <c r="M84" s="12"/>
+      <c r="N84" s="12"/>
+      <c r="O84" s="12"/>
+    </row>
+    <row r="85" spans="10:17" x14ac:dyDescent="0.2">
+      <c r="J85" s="12" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="83" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F83" s="12" t="s">
+      <c r="L85" s="12"/>
+      <c r="M85" s="12"/>
+      <c r="N85" s="12"/>
+      <c r="O85" s="12"/>
+    </row>
+    <row r="86" spans="10:17" x14ac:dyDescent="0.2">
+      <c r="J86" s="12" t="s">
         <v>459</v>
       </c>
-    </row>
-    <row r="84" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F84" s="12" t="s">
+      <c r="L86" s="12"/>
+      <c r="M86" s="12"/>
+      <c r="N86" s="12"/>
+      <c r="O86" s="12"/>
+    </row>
+    <row r="87" spans="10:17" x14ac:dyDescent="0.2">
+      <c r="J87" s="12" t="s">
         <v>460</v>
       </c>
-    </row>
-    <row r="85" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F85" s="12" t="s">
+      <c r="L87" s="12"/>
+      <c r="M87" s="12"/>
+      <c r="N87" s="12"/>
+      <c r="O87" s="12"/>
+    </row>
+    <row r="88" spans="10:17" x14ac:dyDescent="0.2">
+      <c r="J88" s="12" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="86" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F86" s="12" t="s">
+      <c r="L88" s="12"/>
+      <c r="M88" s="12"/>
+      <c r="N88" s="12"/>
+      <c r="O88" s="12"/>
+    </row>
+    <row r="89" spans="10:17" x14ac:dyDescent="0.2">
+      <c r="J89" s="12" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="87" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F87" s="12" t="s">
+      <c r="L89" s="12"/>
+      <c r="M89" s="12"/>
+      <c r="N89" s="12"/>
+      <c r="O89" s="12"/>
+    </row>
+    <row r="90" spans="10:17" x14ac:dyDescent="0.2">
+      <c r="J90" s="12" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="88" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F88" s="12" t="s">
+      <c r="L90" s="12"/>
+      <c r="M90" s="12"/>
+      <c r="N90" s="12"/>
+      <c r="O90" s="12"/>
+    </row>
+    <row r="91" spans="10:17" x14ac:dyDescent="0.2">
+      <c r="J91" s="12" t="s">
         <v>464</v>
       </c>
-    </row>
-    <row r="89" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F89" s="12" t="s">
+      <c r="L91" s="12"/>
+      <c r="M91" s="12"/>
+      <c r="N91" s="12"/>
+      <c r="O91" s="12"/>
+    </row>
+    <row r="92" spans="10:17" x14ac:dyDescent="0.2">
+      <c r="J92" s="30" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="90" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F90" s="12" t="s">
+      <c r="L92" s="12"/>
+      <c r="M92" s="12"/>
+      <c r="N92" s="12"/>
+      <c r="O92" s="12"/>
+    </row>
+    <row r="93" spans="10:17" x14ac:dyDescent="0.2">
+      <c r="J93" s="12" t="s">
         <v>466</v>
       </c>
-    </row>
-    <row r="91" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F91" s="12" t="s">
+      <c r="L93" s="12"/>
+      <c r="M93" s="12"/>
+      <c r="N93" s="12"/>
+      <c r="O93" s="12"/>
+    </row>
+    <row r="94" spans="10:17" x14ac:dyDescent="0.2">
+      <c r="J94" s="12" t="s">
         <v>467</v>
       </c>
-    </row>
-    <row r="92" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F92" s="12" t="s">
+      <c r="L94" s="12"/>
+      <c r="M94" s="12"/>
+      <c r="N94" s="12"/>
+      <c r="O94" s="12"/>
+    </row>
+    <row r="95" spans="10:17" x14ac:dyDescent="0.2">
+      <c r="J95" s="30" t="s">
         <v>468</v>
       </c>
-    </row>
-    <row r="93" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F93" s="12" t="s">
+      <c r="L95" s="12"/>
+      <c r="M95" s="12"/>
+      <c r="N95" s="12"/>
+      <c r="O95" s="12"/>
+    </row>
+    <row r="96" spans="10:17" x14ac:dyDescent="0.2">
+      <c r="J96" s="12" t="s">
         <v>469</v>
       </c>
-    </row>
-    <row r="94" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F94" s="12" t="s">
+      <c r="L96" s="12"/>
+      <c r="M96" s="12"/>
+      <c r="N96" s="12"/>
+      <c r="O96" s="12"/>
+    </row>
+    <row r="97" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="J97" s="12" t="s">
         <v>470</v>
       </c>
-    </row>
-    <row r="95" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F95" s="12" t="s">
+      <c r="L97" s="12"/>
+      <c r="M97" s="12"/>
+      <c r="N97" s="12"/>
+      <c r="O97" s="12"/>
+    </row>
+    <row r="98" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="J98" s="30" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="96" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F96" s="12" t="s">
+    <row r="99" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="J99" s="12" t="s">
         <v>472</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F97" s="12" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B104" s="12" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A105" s="15" t="s">
         <v>143</v>
       </c>
@@ -6194,7 +6443,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B106" s="12" t="s">
         <v>41</v>
       </c>
@@ -6202,7 +6451,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B107" s="12" t="s">
         <v>387</v>
       </c>
@@ -6210,7 +6459,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B108" s="12" t="s">
         <v>50</v>
       </c>
@@ -6218,7 +6467,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B109" s="12" t="s">
         <v>83</v>
       </c>
@@ -6226,13 +6475,13 @@
         <v>408</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B110" s="12" t="s">
         <v>388</v>
       </c>
       <c r="C110" s="21"/>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B111" s="12" t="s">
         <v>88</v>
       </c>
@@ -6240,13 +6489,13 @@
         <v>409</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B112" s="12" t="s">
         <v>389</v>
       </c>
       <c r="C112" s="21"/>
     </row>
-    <row r="113" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B113" s="12" t="s">
         <v>105</v>
       </c>
@@ -6254,7 +6503,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="114" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B114" s="12" t="s">
         <v>77</v>
       </c>
@@ -6262,7 +6511,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="115" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B115" s="12" t="s">
         <v>10</v>
       </c>
@@ -6270,13 +6519,13 @@
         <v>411</v>
       </c>
     </row>
-    <row r="116" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B116" s="12" t="s">
         <v>390</v>
       </c>
       <c r="C116" s="21"/>
     </row>
-    <row r="117" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B117" s="12" t="s">
         <v>113</v>
       </c>
@@ -6284,7 +6533,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="118" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B118" s="12" t="s">
         <v>26</v>
       </c>
@@ -6292,7 +6541,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="119" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B119" s="12" t="s">
         <v>47</v>
       </c>
@@ -6300,7 +6549,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="120" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B120" s="12" t="s">
         <v>23</v>
       </c>
@@ -6308,7 +6557,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="121" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B121" s="12" t="s">
         <v>81</v>
       </c>
@@ -6316,7 +6565,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="122" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B122" s="12" t="s">
         <v>69</v>
       </c>
@@ -6324,7 +6573,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="123" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B123" s="12" t="s">
         <v>29</v>
       </c>
@@ -6332,13 +6581,13 @@
         <v>406</v>
       </c>
     </row>
-    <row r="124" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B124" s="12" t="s">
         <v>391</v>
       </c>
       <c r="C124" s="21"/>
     </row>
-    <row r="125" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B125" s="12" t="s">
         <v>44</v>
       </c>
@@ -6346,7 +6595,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="126" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B126" s="12" t="s">
         <v>82</v>
       </c>
@@ -6354,7 +6603,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="127" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B127" s="12" t="s">
         <v>100</v>
       </c>
@@ -6362,7 +6611,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="128" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B128" s="12" t="s">
         <v>53</v>
       </c>
@@ -6370,7 +6619,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="129" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B129" s="14" t="s">
         <v>76</v>
       </c>
@@ -6378,7 +6627,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="130" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B130" s="12" t="s">
         <v>392</v>
       </c>
@@ -6386,25 +6635,25 @@
         <v>405</v>
       </c>
     </row>
-    <row r="131" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B131" s="12" t="s">
         <v>393</v>
       </c>
       <c r="C131" s="21"/>
     </row>
-    <row r="132" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B132" s="12" t="s">
         <v>394</v>
       </c>
       <c r="C132" s="21"/>
     </row>
-    <row r="133" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B133" s="12" t="s">
         <v>395</v>
       </c>
       <c r="C133" s="21"/>
     </row>
-    <row r="134" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B134" s="12" t="s">
         <v>66</v>
       </c>
@@ -6412,7 +6661,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="135" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B135" s="12" t="s">
         <v>27</v>
       </c>
@@ -6420,13 +6669,13 @@
         <v>406</v>
       </c>
     </row>
-    <row r="136" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B136" s="12" t="s">
         <v>396</v>
       </c>
       <c r="C136" s="21"/>
     </row>
-    <row r="137" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B137" s="12" t="s">
         <v>59</v>
       </c>
@@ -6434,7 +6683,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="138" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B138" s="12" t="s">
         <v>79</v>
       </c>
@@ -6442,7 +6691,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="139" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B139" s="12" t="s">
         <v>103</v>
       </c>
@@ -6450,7 +6699,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="140" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B140" s="12" t="s">
         <v>108</v>
       </c>
@@ -6458,19 +6707,19 @@
         <v>416</v>
       </c>
     </row>
-    <row r="141" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B141" s="12" t="s">
         <v>397</v>
       </c>
       <c r="C141" s="21"/>
     </row>
-    <row r="142" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B142" s="12" t="s">
         <v>398</v>
       </c>
       <c r="C142" s="21"/>
     </row>
-    <row r="143" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="143" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B143" s="12" t="s">
         <v>37</v>
       </c>
@@ -6478,13 +6727,13 @@
         <v>405</v>
       </c>
     </row>
-    <row r="144" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B144" s="12" t="s">
         <v>399</v>
       </c>
       <c r="C144" s="21"/>
     </row>
-    <row r="145" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B145" s="14" t="s">
         <v>93</v>
       </c>
@@ -6492,7 +6741,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="146" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B146" s="12" t="s">
         <v>97</v>
       </c>
@@ -6500,7 +6749,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="147" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="147" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B147" s="12" t="s">
         <v>400</v>
       </c>
@@ -6508,7 +6757,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="148" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="148" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B148" s="12" t="s">
         <v>94</v>
       </c>
@@ -6516,7 +6765,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="149" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="149" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B149" s="14" t="s">
         <v>36</v>
       </c>
@@ -6524,7 +6773,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="150" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="150" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B150" s="12" t="s">
         <v>42</v>
       </c>
@@ -6532,13 +6781,13 @@
         <v>405</v>
       </c>
     </row>
-    <row r="151" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="151" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B151" s="12" t="s">
         <v>401</v>
       </c>
       <c r="C151" s="21"/>
     </row>
-    <row r="152" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="152" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B152" s="12" t="s">
         <v>101</v>
       </c>
@@ -6546,7 +6795,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="153" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="153" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B153" s="14" t="s">
         <v>107</v>
       </c>
@@ -6554,7 +6803,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="154" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="154" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B154" s="12" t="s">
         <v>95</v>
       </c>
@@ -6562,13 +6811,13 @@
         <v>410</v>
       </c>
     </row>
-    <row r="155" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="155" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B155" s="12" t="s">
         <v>402</v>
       </c>
       <c r="C155" s="21"/>
     </row>
-    <row r="156" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="156" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B156" s="12" t="s">
         <v>102</v>
       </c>
@@ -6576,7 +6825,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="157" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="157" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B157" s="12" t="s">
         <v>98</v>
       </c>
@@ -6584,7 +6833,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="158" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="158" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B158" s="12" t="s">
         <v>96</v>
       </c>
@@ -6592,7 +6841,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="159" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="159" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B159" s="12" t="s">
         <v>99</v>
       </c>
@@ -6600,7 +6849,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="160" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="160" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B160" s="12" t="s">
         <v>46</v>
       </c>
@@ -6608,7 +6857,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="161" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="161" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B161" s="12" t="s">
         <v>39</v>
       </c>
@@ -6616,13 +6865,16 @@
         <v>405</v>
       </c>
     </row>
-    <row r="162" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="162" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B162" s="12" t="s">
         <v>403</v>
       </c>
       <c r="C162" s="21"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="J57:J99">
+    <sortCondition ref="J99"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
discussed new phygad data
</commit_message>
<xml_diff>
--- a/Townes vs Broad.xlsx
+++ b/Townes vs Broad.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robin\Dropbox\Mein PC (Gemeinsamer-PC)\Documents\GitHub\Ichneumonidae\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF7AA36F-4918-4D6B-BCAE-2FCECE5F7E7B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5046447D-4D81-4284-9DA5-D4C23E4A398A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="2" xr2:uid="{63889695-902D-49DB-8829-7F5E2426025F}"/>
+    <workbookView xWindow="105" yWindow="45" windowWidth="15765" windowHeight="14550" activeTab="2" xr2:uid="{63889695-902D-49DB-8829-7F5E2426025F}"/>
   </bookViews>
   <sheets>
     <sheet name="TOWNES" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="926" uniqueCount="548">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="918" uniqueCount="548">
   <si>
     <t>Epelaspis</t>
   </si>
@@ -1730,7 +1730,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1797,6 +1797,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1810,7 +1816,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1846,6 +1852,7 @@
     <xf numFmtId="49" fontId="4" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -2162,8 +2169,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3325E525-F9CE-447C-9C7C-9E0C969A72AA}">
   <dimension ref="A1:R96"/>
   <sheetViews>
-    <sheetView topLeftCell="J52" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="Q57" sqref="Q57"/>
+    <sheetView topLeftCell="G1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5426,8 +5433,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EED08F7F-A003-4C3B-8646-FC85C271AAFB}">
   <dimension ref="A1:Q163"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="F118" sqref="F118"/>
+    <sheetView tabSelected="1" topLeftCell="A102" workbookViewId="0">
+      <selection activeCell="H112" sqref="H112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6482,9 +6489,7 @@
       <c r="E106" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="F106" s="11" t="s">
-        <v>388</v>
-      </c>
+      <c r="F106" s="10"/>
     </row>
     <row r="107" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B107" s="14" t="s">
@@ -6496,9 +6501,7 @@
       <c r="E107" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="F107" s="11" t="s">
-        <v>389</v>
-      </c>
+      <c r="F107" s="10"/>
     </row>
     <row r="108" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B108" s="14" t="s">
@@ -6510,9 +6513,7 @@
       <c r="E108" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="F108" s="11" t="s">
-        <v>390</v>
-      </c>
+      <c r="F108" s="10"/>
     </row>
     <row r="109" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B109" s="12" t="s">
@@ -6524,9 +6525,7 @@
       <c r="E109" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="F109" s="11" t="s">
-        <v>391</v>
-      </c>
+      <c r="F109" s="10"/>
     </row>
     <row r="110" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B110" s="12" t="s">
@@ -6536,9 +6535,7 @@
       <c r="E110" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="F110" s="11" t="s">
-        <v>393</v>
-      </c>
+      <c r="F110" s="10"/>
     </row>
     <row r="111" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B111" s="14" t="s">
@@ -6562,16 +6559,14 @@
       <c r="E112" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="F112" s="11" t="s">
-        <v>395</v>
-      </c>
+      <c r="F112" s="10"/>
     </row>
     <row r="113" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B113" s="12" t="s">
         <v>389</v>
       </c>
       <c r="C113" s="21"/>
-      <c r="E113" s="13" t="s">
+      <c r="E113" s="35" t="s">
         <v>44</v>
       </c>
       <c r="F113" s="34" t="s">
@@ -6585,7 +6580,7 @@
       <c r="C114" s="21" t="s">
         <v>410</v>
       </c>
-      <c r="E114" s="13" t="s">
+      <c r="E114" s="35" t="s">
         <v>82</v>
       </c>
       <c r="F114" s="34" t="s">
@@ -6616,16 +6611,14 @@
       <c r="E116" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="F116" s="11" t="s">
-        <v>401</v>
-      </c>
+      <c r="F116" s="10"/>
     </row>
     <row r="117" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B117" s="12" t="s">
         <v>390</v>
       </c>
       <c r="C117" s="21"/>
-      <c r="E117" s="13" t="s">
+      <c r="E117" s="35" t="s">
         <v>79</v>
       </c>
       <c r="F117" s="34" t="s">
@@ -6653,9 +6646,7 @@
       <c r="C119" s="21" t="s">
         <v>406</v>
       </c>
-      <c r="E119" s="13" t="s">
-        <v>37</v>
-      </c>
+      <c r="E119" s="10"/>
     </row>
     <row r="120" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B120" s="14" t="s">
@@ -6750,7 +6741,7 @@
       <c r="C128" s="21" t="s">
         <v>410</v>
       </c>
-      <c r="E128" s="13" t="s">
+      <c r="E128" s="35" t="s">
         <v>96</v>
       </c>
     </row>

</xml_diff>

<commit_message>
corrected DataSet of Genus Assertion
</commit_message>
<xml_diff>
--- a/Townes vs Broad.xlsx
+++ b/Townes vs Broad.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robin\Dropbox\Mein PC (Gemeinsamer-PC)\Documents\GitHub\Ichneumonidae\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF0BE90D-7BA6-43FA-A67F-304244E903C7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1538463-3AB9-45EE-937B-8433EA4EB4CF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11790" yWindow="525" windowWidth="15765" windowHeight="14550" activeTab="2" xr2:uid="{63889695-902D-49DB-8829-7F5E2426025F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{63889695-902D-49DB-8829-7F5E2426025F}"/>
   </bookViews>
   <sheets>
     <sheet name="TOWNES" sheetId="1" r:id="rId1"/>
@@ -1730,7 +1730,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1803,6 +1803,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1816,7 +1822,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1853,6 +1859,8 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="4" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -2169,8 +2177,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3325E525-F9CE-447C-9C7C-9E0C969A72AA}">
   <dimension ref="A1:R96"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2414,7 +2422,7 @@
       <c r="D10" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="E10" s="23" t="s">
+      <c r="E10" s="37" t="s">
         <v>40</v>
       </c>
       <c r="F10" s="31" t="s">
@@ -2448,7 +2456,7 @@
       <c r="E11" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="F11" s="36" t="s">
         <v>44</v>
       </c>
       <c r="G11" s="12"/>
@@ -2564,7 +2572,7 @@
       <c r="E15" s="12"/>
       <c r="F15" s="12"/>
       <c r="G15" s="12"/>
-      <c r="H15" s="12" t="s">
+      <c r="H15" s="10" t="s">
         <v>59</v>
       </c>
       <c r="I15" s="12"/>
@@ -5433,8 +5441,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EED08F7F-A003-4C3B-8646-FC85C271AAFB}">
   <dimension ref="A1:Q163"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A104" workbookViewId="0">
-      <selection activeCell="F118" sqref="F111:F118"/>
+    <sheetView topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="B134" sqref="B134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
havent pushed in a while
</commit_message>
<xml_diff>
--- a/Townes vs Broad.xlsx
+++ b/Townes vs Broad.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robin\Dropbox\Mein PC (Gemeinsamer-PC)\Documents\GitHub\Ichneumonidae\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1538463-3AB9-45EE-937B-8433EA4EB4CF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBB118FF-C9C9-4C83-B815-A264BF700741}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{63889695-902D-49DB-8829-7F5E2426025F}"/>
+    <workbookView xWindow="1650" yWindow="510" windowWidth="15765" windowHeight="14550" activeTab="2" xr2:uid="{63889695-902D-49DB-8829-7F5E2426025F}"/>
   </bookViews>
   <sheets>
     <sheet name="TOWNES" sheetId="1" r:id="rId1"/>
@@ -1730,7 +1730,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1787,12 +1787,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF7030A0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1800,12 +1794,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1822,7 +1810,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1855,12 +1843,8 @@
     <xf numFmtId="49" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="4" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="4" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -2177,8 +2161,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3325E525-F9CE-447C-9C7C-9E0C969A72AA}">
   <dimension ref="A1:R96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView topLeftCell="A33" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2339,16 +2323,16 @@
       <c r="C8" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="32" t="s">
+      <c r="D8" s="20" t="s">
         <v>28</v>
       </c>
       <c r="E8" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="F8" s="31" t="s">
+      <c r="F8" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="G8" s="31" t="s">
+      <c r="G8" s="14" t="s">
         <v>53</v>
       </c>
       <c r="H8" s="19" t="s">
@@ -2369,7 +2353,7 @@
       <c r="M8" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="N8" s="32" t="s">
+      <c r="N8" s="20" t="s">
         <v>109</v>
       </c>
       <c r="O8" s="19" t="s">
@@ -2393,7 +2377,7 @@
       <c r="H9" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="I9" s="31" t="s">
+      <c r="I9" s="14" t="s">
         <v>69</v>
       </c>
       <c r="J9" s="19" t="s">
@@ -2408,7 +2392,7 @@
       <c r="M9" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="N9" s="31" t="s">
+      <c r="N9" s="14" t="s">
         <v>108</v>
       </c>
       <c r="O9" s="12" t="s">
@@ -2422,10 +2406,10 @@
       <c r="D10" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="E10" s="37" t="s">
+      <c r="E10" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="F10" s="31" t="s">
+      <c r="F10" s="14" t="s">
         <v>47</v>
       </c>
       <c r="G10" s="12"/>
@@ -2447,7 +2431,7 @@
       <c r="O10" s="12"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C11" s="31" t="s">
+      <c r="C11" s="14" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="19" t="s">
@@ -2456,7 +2440,7 @@
       <c r="E11" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="F11" s="36" t="s">
+      <c r="F11" s="10" t="s">
         <v>44</v>
       </c>
       <c r="G11" s="12"/>
@@ -2512,13 +2496,13 @@
       <c r="C13" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="D13" s="31" t="s">
+      <c r="D13" s="14" t="s">
         <v>26</v>
       </c>
       <c r="E13" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="F13" s="31" t="s">
+      <c r="F13" s="14" t="s">
         <v>46</v>
       </c>
       <c r="G13" s="12"/>
@@ -2637,7 +2621,7 @@
       <c r="C18" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="D18" s="31" t="s">
+      <c r="D18" s="14" t="s">
         <v>27</v>
       </c>
       <c r="E18" s="12"/>
@@ -3244,14 +3228,14 @@
       </c>
     </row>
     <row r="56" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C56" s="33" t="s">
-        <v>153</v>
+      <c r="C56" s="4" t="s">
+        <v>155</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="F56" s="5" t="s">
         <v>231</v>
@@ -3272,7 +3256,7 @@
       <c r="N56" s="26" t="s">
         <v>300</v>
       </c>
-      <c r="O56" s="33" t="s">
+      <c r="O56" s="2" t="s">
         <v>324</v>
       </c>
       <c r="P56" s="5" t="s">
@@ -3287,10 +3271,10 @@
         <v>154</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>166</v>
+        <v>195</v>
       </c>
       <c r="E57" s="5" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="F57" s="9" t="s">
         <v>220</v>
@@ -3313,19 +3297,19 @@
       <c r="P57" s="5" t="s">
         <v>330</v>
       </c>
-      <c r="Q57" s="33" t="s">
+      <c r="Q57" s="2" t="s">
         <v>354</v>
       </c>
     </row>
     <row r="58" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C58" s="4" t="s">
-        <v>155</v>
+      <c r="C58" t="s">
+        <v>158</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>167</v>
+        <v>179</v>
       </c>
       <c r="E58" s="5" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="F58" s="5" t="s">
         <v>225</v>
@@ -3339,7 +3323,7 @@
       <c r="N58" s="5" t="s">
         <v>302</v>
       </c>
-      <c r="O58" s="33" t="s">
+      <c r="O58" s="2" t="s">
         <v>323</v>
       </c>
       <c r="P58" s="5" t="s">
@@ -3347,14 +3331,14 @@
       </c>
     </row>
     <row r="59" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C59" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="D59" s="5" t="s">
-        <v>168</v>
+      <c r="C59" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="D59" t="s">
+        <v>192</v>
       </c>
       <c r="E59" s="5" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="F59" s="5" t="s">
         <v>224</v>
@@ -3376,14 +3360,14 @@
       </c>
     </row>
     <row r="60" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C60" s="33" t="s">
-        <v>157</v>
+      <c r="C60" s="2" t="s">
+        <v>160</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E60" s="5" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="F60" s="5" t="s">
         <v>219</v>
@@ -3405,14 +3389,14 @@
       </c>
     </row>
     <row r="61" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C61" t="s">
-        <v>158</v>
+      <c r="C61" s="2" t="s">
+        <v>161</v>
       </c>
       <c r="D61" s="6" t="s">
-        <v>170</v>
+        <v>189</v>
       </c>
       <c r="E61" s="5" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="F61" s="5" t="s">
         <v>221</v>
@@ -3435,13 +3419,13 @@
     </row>
     <row r="62" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C62" s="5" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="E62" s="5" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="F62" s="5" t="s">
         <v>227</v>
@@ -3463,14 +3447,14 @@
       </c>
     </row>
     <row r="63" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C63" s="33" t="s">
-        <v>160</v>
+      <c r="C63" s="5" t="s">
+        <v>159</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="E63" s="5" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="F63" s="5" t="s">
         <v>230</v>
@@ -3492,14 +3476,14 @@
       </c>
     </row>
     <row r="64" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C64" s="33" t="s">
-        <v>161</v>
+      <c r="C64" s="2" t="s">
+        <v>153</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>173</v>
+        <v>180</v>
       </c>
       <c r="E64" s="5" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="F64" s="5" t="s">
         <v>222</v>
@@ -3521,11 +3505,11 @@
       <c r="C65" t="s">
         <v>162</v>
       </c>
-      <c r="D65" s="6" t="s">
-        <v>174</v>
+      <c r="D65" s="5" t="s">
+        <v>203</v>
       </c>
       <c r="E65" s="5" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="F65" s="5" t="s">
         <v>229</v>
@@ -3545,9 +3529,9 @@
     </row>
     <row r="66" spans="3:16" x14ac:dyDescent="0.25">
       <c r="D66" s="5" t="s">
-        <v>175</v>
-      </c>
-      <c r="F66" s="33" t="s">
+        <v>181</v>
+      </c>
+      <c r="F66" s="2" t="s">
         <v>226</v>
       </c>
       <c r="H66" s="5" t="s">
@@ -3565,7 +3549,7 @@
     </row>
     <row r="67" spans="3:16" x14ac:dyDescent="0.25">
       <c r="D67" s="5" t="s">
-        <v>176</v>
+        <v>184</v>
       </c>
       <c r="F67" s="5" t="s">
         <v>232</v>
@@ -3585,7 +3569,7 @@
     </row>
     <row r="68" spans="3:16" x14ac:dyDescent="0.25">
       <c r="D68" s="5" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="F68" s="5" t="s">
         <v>223</v>
@@ -3605,7 +3589,7 @@
     </row>
     <row r="69" spans="3:16" x14ac:dyDescent="0.25">
       <c r="D69" s="5" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="H69" s="5" t="s">
         <v>252</v>
@@ -3622,7 +3606,7 @@
     </row>
     <row r="70" spans="3:16" x14ac:dyDescent="0.25">
       <c r="D70" s="5" t="s">
-        <v>179</v>
+        <v>188</v>
       </c>
       <c r="H70" s="5" t="s">
         <v>253</v>
@@ -3639,7 +3623,7 @@
     </row>
     <row r="71" spans="3:16" x14ac:dyDescent="0.25">
       <c r="D71" s="5" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="H71" s="5" t="s">
         <v>254</v>
@@ -3656,7 +3640,7 @@
     </row>
     <row r="72" spans="3:16" x14ac:dyDescent="0.25">
       <c r="D72" s="5" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="H72" s="5" t="s">
         <v>255</v>
@@ -3669,8 +3653,8 @@
       </c>
     </row>
     <row r="73" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="D73" s="5" t="s">
-        <v>182</v>
+      <c r="D73" s="6" t="s">
+        <v>170</v>
       </c>
       <c r="H73" s="5" t="s">
         <v>256</v>
@@ -3681,7 +3665,7 @@
     </row>
     <row r="74" spans="3:16" x14ac:dyDescent="0.25">
       <c r="D74" s="5" t="s">
-        <v>183</v>
+        <v>166</v>
       </c>
       <c r="H74" t="s">
         <v>257</v>
@@ -3692,7 +3676,7 @@
     </row>
     <row r="75" spans="3:16" x14ac:dyDescent="0.25">
       <c r="D75" s="5" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="H75" s="5" t="s">
         <v>258</v>
@@ -3703,7 +3687,7 @@
     </row>
     <row r="76" spans="3:16" x14ac:dyDescent="0.25">
       <c r="D76" s="5" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="H76" s="5" t="s">
         <v>259</v>
@@ -3713,8 +3697,8 @@
       </c>
     </row>
     <row r="77" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="D77" s="5" t="s">
-        <v>186</v>
+      <c r="D77" s="6" t="s">
+        <v>174</v>
       </c>
       <c r="H77" s="5" t="s">
         <v>260</v>
@@ -3725,7 +3709,7 @@
     </row>
     <row r="78" spans="3:16" x14ac:dyDescent="0.25">
       <c r="D78" s="5" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="H78" s="5" t="s">
         <v>261</v>
@@ -3733,15 +3717,15 @@
     </row>
     <row r="79" spans="3:16" x14ac:dyDescent="0.25">
       <c r="D79" s="5" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="H79" s="5" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="80" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="D80" s="6" t="s">
-        <v>189</v>
+      <c r="D80" s="5" t="s">
+        <v>191</v>
       </c>
       <c r="H80" s="5" t="s">
         <v>263</v>
@@ -3749,23 +3733,23 @@
     </row>
     <row r="81" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D81" s="5" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="H81" s="5" t="s">
         <v>264</v>
       </c>
     </row>
     <row r="82" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D82" s="5" t="s">
-        <v>191</v>
+      <c r="D82" t="s">
+        <v>201</v>
       </c>
       <c r="H82" s="5" t="s">
         <v>265</v>
       </c>
     </row>
     <row r="83" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D83" t="s">
-        <v>192</v>
+      <c r="D83" s="5" t="s">
+        <v>165</v>
       </c>
       <c r="H83" s="5" t="s">
         <v>266</v>
@@ -3773,15 +3757,15 @@
     </row>
     <row r="84" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D84" s="5" t="s">
-        <v>193</v>
+        <v>200</v>
       </c>
       <c r="H84" s="5" t="s">
         <v>267</v>
       </c>
     </row>
     <row r="85" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D85" t="s">
-        <v>194</v>
+      <c r="D85" s="5" t="s">
+        <v>196</v>
       </c>
       <c r="H85" s="5" t="s">
         <v>268</v>
@@ -3789,7 +3773,7 @@
     </row>
     <row r="86" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D86" s="5" t="s">
-        <v>195</v>
+        <v>204</v>
       </c>
       <c r="H86" s="5" t="s">
         <v>269</v>
@@ -3797,7 +3781,7 @@
     </row>
     <row r="87" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D87" s="5" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="H87" s="5" t="s">
         <v>270</v>
@@ -3805,42 +3789,42 @@
     </row>
     <row r="88" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D88" s="5" t="s">
-        <v>197</v>
+        <v>168</v>
       </c>
     </row>
     <row r="89" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D89" s="5" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
     </row>
     <row r="90" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D90" s="5" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="91" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D91" s="5" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
     </row>
     <row r="92" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D92" t="s">
-        <v>201</v>
+      <c r="D92" s="5" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="93" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D93" s="5" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="94" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D94" s="5" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
     </row>
     <row r="95" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D95" s="5" t="s">
-        <v>204</v>
+      <c r="D95" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="96" spans="4:8" x14ac:dyDescent="0.25">
@@ -3849,8 +3833,8 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="N8:N9">
-    <sortCondition ref="N7:N9"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="E56:E65">
+    <sortCondition ref="E55:E65"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3861,7 +3845,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03C0ADB5-C0E5-4138-BDA1-AB6896EBEF9E}">
   <dimension ref="A1:A377"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
@@ -5441,8 +5425,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EED08F7F-A003-4C3B-8646-FC85C271AAFB}">
   <dimension ref="A1:Q163"/>
   <sheetViews>
-    <sheetView topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="B134" sqref="B134"/>
+    <sheetView tabSelected="1" topLeftCell="A110" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5589,7 +5573,7 @@
       <c r="C27" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="D27" s="31" t="s">
+      <c r="D27" s="14" t="s">
         <v>324</v>
       </c>
       <c r="E27" s="18" t="s">
@@ -5706,7 +5690,7 @@
       <c r="C36" s="14" t="s">
         <v>369</v>
       </c>
-      <c r="D36" s="31" t="s">
+      <c r="D36" s="14" t="s">
         <v>157</v>
       </c>
       <c r="E36" s="18" t="s">
@@ -5730,7 +5714,7 @@
       <c r="C38" s="14" t="s">
         <v>370</v>
       </c>
-      <c r="D38" s="31" t="s">
+      <c r="D38" s="14" t="s">
         <v>160</v>
       </c>
       <c r="E38" s="18" t="s">
@@ -5750,7 +5734,7 @@
       <c r="C40" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="D40" s="31" t="s">
+      <c r="D40" s="14" t="s">
         <v>161</v>
       </c>
       <c r="E40" s="18" t="s">
@@ -5794,7 +5778,7 @@
       <c r="C44" s="20" t="s">
         <v>135</v>
       </c>
-      <c r="D44" s="31" t="s">
+      <c r="D44" s="14" t="s">
         <v>226</v>
       </c>
       <c r="E44" s="18" t="s">
@@ -5802,7 +5786,7 @@
       </c>
     </row>
     <row r="45" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="D45" s="31" t="s">
+      <c r="D45" s="14" t="s">
         <v>323</v>
       </c>
       <c r="E45" s="18" t="s">
@@ -5818,7 +5802,7 @@
       </c>
     </row>
     <row r="47" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="D47" s="31" t="s">
+      <c r="D47" s="14" t="s">
         <v>354</v>
       </c>
       <c r="E47" s="18" t="s">
@@ -5826,7 +5810,7 @@
       </c>
     </row>
     <row r="48" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="D48" s="31" t="s">
+      <c r="D48" s="14" t="s">
         <v>153</v>
       </c>
       <c r="E48" s="18" t="s">
@@ -6483,7 +6467,7 @@
       <c r="E105" s="13" t="s">
         <v>546</v>
       </c>
-      <c r="F105" s="34" t="s">
+      <c r="F105" s="31" t="s">
         <v>547</v>
       </c>
     </row>
@@ -6553,7 +6537,7 @@
       <c r="E111" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="F111" s="34" t="s">
+      <c r="F111" s="31" t="s">
         <v>394</v>
       </c>
     </row>
@@ -6574,10 +6558,10 @@
         <v>389</v>
       </c>
       <c r="C113" s="21"/>
-      <c r="E113" s="35" t="s">
+      <c r="E113" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="F113" s="34" t="s">
+      <c r="F113" s="31" t="s">
         <v>396</v>
       </c>
     </row>
@@ -6588,10 +6572,10 @@
       <c r="C114" s="21" t="s">
         <v>410</v>
       </c>
-      <c r="E114" s="35" t="s">
+      <c r="E114" s="32" t="s">
         <v>82</v>
       </c>
-      <c r="F114" s="34" t="s">
+      <c r="F114" s="31" t="s">
         <v>397</v>
       </c>
     </row>
@@ -6605,7 +6589,7 @@
       <c r="E115" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="F115" s="34" t="s">
+      <c r="F115" s="31" t="s">
         <v>398</v>
       </c>
     </row>
@@ -6626,10 +6610,10 @@
         <v>390</v>
       </c>
       <c r="C117" s="21"/>
-      <c r="E117" s="35" t="s">
+      <c r="E117" s="32" t="s">
         <v>79</v>
       </c>
-      <c r="F117" s="34" t="s">
+      <c r="F117" s="31" t="s">
         <v>402</v>
       </c>
     </row>
@@ -6643,7 +6627,7 @@
       <c r="E118" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="F118" s="34" t="s">
+      <c r="F118" s="31" t="s">
         <v>403</v>
       </c>
     </row>
@@ -6749,7 +6733,7 @@
       <c r="C128" s="21" t="s">
         <v>410</v>
       </c>
-      <c r="E128" s="35" t="s">
+      <c r="E128" s="32" t="s">
         <v>96</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ordered structure in data
</commit_message>
<xml_diff>
--- a/Townes vs Broad.xlsx
+++ b/Townes vs Broad.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robin\Dropbox\Mein PC (Gemeinsamer-PC)\Documents\GitHub\Ichneumonidae\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBB118FF-C9C9-4C83-B815-A264BF700741}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E30BBDE0-F08E-4E65-8B1E-A95E6AC24958}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1650" yWindow="510" windowWidth="15765" windowHeight="14550" activeTab="2" xr2:uid="{63889695-902D-49DB-8829-7F5E2426025F}"/>
+    <workbookView xWindow="10080" yWindow="960" windowWidth="15765" windowHeight="14550" activeTab="2" xr2:uid="{63889695-902D-49DB-8829-7F5E2426025F}"/>
   </bookViews>
   <sheets>
     <sheet name="TOWNES" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="918" uniqueCount="548">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="915" uniqueCount="580">
   <si>
     <t>Epelaspis</t>
   </si>
@@ -1157,9 +1157,6 @@
     <t>Pleolophus</t>
   </si>
   <si>
-    <t>!</t>
-  </si>
-  <si>
     <t>CRYPTINI</t>
   </si>
   <si>
@@ -1676,10 +1673,109 @@
     <t>in Ichneumoninae key als Tribe</t>
   </si>
   <si>
-    <t>24.03.2020 Townes</t>
-  </si>
-  <si>
-    <t>BOLD SYSTEMS</t>
+    <t>ALOMYINI</t>
+  </si>
+  <si>
+    <t>Pseudalomya</t>
+  </si>
+  <si>
+    <t>PROTICHNEUMONINI</t>
+  </si>
+  <si>
+    <t>PROTICHNEUMONINA</t>
+  </si>
+  <si>
+    <t>APATETORINA</t>
+  </si>
+  <si>
+    <t>Apatetor</t>
+  </si>
+  <si>
+    <t>TROGINI</t>
+  </si>
+  <si>
+    <t>CALLAJOPPINA</t>
+  </si>
+  <si>
+    <t>TROGINA</t>
+  </si>
+  <si>
+    <t>Ectopoides</t>
+  </si>
+  <si>
+    <t>Afrectopius</t>
+  </si>
+  <si>
+    <t>Cyclolabellus</t>
+  </si>
+  <si>
+    <t>Neolinycus</t>
+  </si>
+  <si>
+    <t>Carlsonia</t>
+  </si>
+  <si>
+    <t>Notoplatylabus</t>
+  </si>
+  <si>
+    <t>Levansa</t>
+  </si>
+  <si>
+    <t>Cratolaboides</t>
+  </si>
+  <si>
+    <t>Pagarenes</t>
+  </si>
+  <si>
+    <t>Clypeolabus</t>
+  </si>
+  <si>
+    <t>Hirtolabus</t>
+  </si>
+  <si>
+    <t>Rhyssolabus</t>
+  </si>
+  <si>
+    <t>Ambloplisus</t>
+  </si>
+  <si>
+    <t>Acantholabus</t>
+  </si>
+  <si>
+    <t>Platybirmania</t>
+  </si>
+  <si>
+    <t>Neolevansa</t>
+  </si>
+  <si>
+    <t>Lamprojoppa</t>
+  </si>
+  <si>
+    <t>Pachyjoppa</t>
+  </si>
+  <si>
+    <t>Lissolaboides</t>
+  </si>
+  <si>
+    <t>Cratolabus</t>
+  </si>
+  <si>
+    <t>Tropicolabus</t>
+  </si>
+  <si>
+    <t>Spanophatnus</t>
+  </si>
+  <si>
+    <t>Neeurylabia</t>
+  </si>
+  <si>
+    <t>Heinrichiellus</t>
+  </si>
+  <si>
+    <t>Abzaria</t>
+  </si>
+  <si>
+    <t>Pyramidophorus</t>
   </si>
 </sst>
 </file>
@@ -1730,7 +1826,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1787,13 +1883,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1833,18 +1923,18 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -2161,8 +2251,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3325E525-F9CE-447C-9C7C-9E0C969A72AA}">
   <dimension ref="A1:R96"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2223,7 +2313,7 @@
         <v>115</v>
       </c>
       <c r="Q5" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
@@ -2274,481 +2364,481 @@
         <v>0</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C7" s="22" t="s">
+      <c r="C7" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="E7" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="F7" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="G7" s="22" t="s">
+      <c r="E7" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="F7" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="G7" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="H7" s="22" t="s">
+      <c r="H7" s="20" t="s">
         <v>55</v>
       </c>
       <c r="I7" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="J7" s="22" t="s">
+      <c r="J7" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="K7" s="14" t="s">
+      <c r="K7" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="L7" s="22" t="s">
+      <c r="L7" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="M7" s="14" t="s">
+      <c r="M7" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="N7" s="14" t="s">
+      <c r="N7" s="20" t="s">
         <v>107</v>
       </c>
-      <c r="O7" s="22" t="s">
+      <c r="O7" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="R7" s="24"/>
+      <c r="R7" s="23"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C8" s="19" t="s">
+      <c r="C8" s="22" t="s">
         <v>14</v>
       </c>
       <c r="D8" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="F8" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="G8" s="14" t="s">
+      <c r="E8" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="G8" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="H8" s="19" t="s">
+      <c r="H8" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="I8" s="19" t="s">
+      <c r="I8" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="J8" s="19" t="s">
+      <c r="J8" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="K8" s="12" t="s">
+      <c r="K8" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="L8" s="19" t="s">
+      <c r="L8" s="22" t="s">
         <v>91</v>
       </c>
-      <c r="M8" s="12" t="s">
+      <c r="M8" s="20" t="s">
         <v>105</v>
       </c>
       <c r="N8" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="O8" s="19" t="s">
+      <c r="O8" s="22" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C9" s="19" t="s">
+      <c r="C9" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="22" t="s">
+      <c r="D9" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="F9" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="G9" s="12"/>
-      <c r="H9" s="19" t="s">
+      <c r="E9" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="I9" s="14" t="s">
+      <c r="I9" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="J9" s="19" t="s">
+      <c r="J9" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="K9" s="12" t="s">
+      <c r="K9" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="L9" s="12" t="s">
+      <c r="L9" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="M9" s="12" t="s">
+      <c r="M9" s="20" t="s">
         <v>100</v>
       </c>
-      <c r="N9" s="14" t="s">
+      <c r="N9" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="O9" s="12" t="s">
+      <c r="O9" s="20" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C10" s="19" t="s">
+      <c r="C10" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="19" t="s">
+      <c r="D10" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="E10" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="F10" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="G10" s="12"/>
-      <c r="H10" s="19" t="s">
+      <c r="E10" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="19" t="s">
+      <c r="I10" s="22"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="L10" s="19" t="s">
+      <c r="L10" s="22" t="s">
         <v>89</v>
       </c>
-      <c r="M10" s="12" t="s">
+      <c r="M10" s="20" t="s">
         <v>103</v>
       </c>
-      <c r="N10" s="12"/>
-      <c r="O10" s="12"/>
+      <c r="N10" s="22"/>
+      <c r="O10" s="22"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="19" t="s">
+      <c r="D11" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="E11" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="F11" s="10" t="s">
+      <c r="E11" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="F11" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="G11" s="12"/>
-      <c r="H11" s="19" t="s">
+      <c r="G11" s="22"/>
+      <c r="H11" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12"/>
-      <c r="K11" s="19" t="s">
+      <c r="I11" s="22"/>
+      <c r="J11" s="22"/>
+      <c r="K11" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="L11" s="19" t="s">
+      <c r="L11" s="22" t="s">
         <v>90</v>
       </c>
-      <c r="M11" s="12" t="s">
+      <c r="M11" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="N11" s="12"/>
-      <c r="O11" s="12"/>
+      <c r="N11" s="22"/>
+      <c r="O11" s="22"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C12" s="19" t="s">
+      <c r="C12" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="19" t="s">
+      <c r="D12" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="E12" s="12" t="s">
+      <c r="E12" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="F12" s="19" t="s">
+      <c r="F12" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="G12" s="12"/>
-      <c r="H12" s="23" t="s">
+      <c r="G12" s="22"/>
+      <c r="H12" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="I12" s="12"/>
-      <c r="J12" s="12"/>
-      <c r="K12" s="12" t="s">
+      <c r="I12" s="22"/>
+      <c r="J12" s="22"/>
+      <c r="K12" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="L12" s="19" t="s">
+      <c r="L12" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="M12" s="12" t="s">
+      <c r="M12" s="20" t="s">
         <v>104</v>
       </c>
-      <c r="N12" s="12"/>
-      <c r="O12" s="12"/>
+      <c r="N12" s="22"/>
+      <c r="O12" s="22"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C13" s="22" t="s">
+      <c r="C13" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="D13" s="14" t="s">
+      <c r="D13" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="E13" s="12" t="s">
+      <c r="E13" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="F13" s="14" t="s">
+      <c r="F13" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="G13" s="12"/>
-      <c r="H13" s="19" t="s">
+      <c r="G13" s="22"/>
+      <c r="H13" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="I13" s="12"/>
-      <c r="J13" s="12"/>
-      <c r="K13" s="12" t="s">
+      <c r="I13" s="22"/>
+      <c r="J13" s="22"/>
+      <c r="K13" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="L13" s="12"/>
-      <c r="M13" s="12" t="s">
+      <c r="L13" s="22"/>
+      <c r="M13" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="N13" s="12"/>
-      <c r="O13" s="12"/>
+      <c r="N13" s="22"/>
+      <c r="O13" s="22"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C14" s="19" t="s">
+      <c r="C14" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="D14" s="19" t="s">
+      <c r="D14" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12" t="s">
+      <c r="E14" s="22"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12"/>
-      <c r="K14" s="12" t="s">
+      <c r="I14" s="22"/>
+      <c r="J14" s="22"/>
+      <c r="K14" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="L14" s="12"/>
-      <c r="M14" s="12" t="s">
+      <c r="L14" s="22"/>
+      <c r="M14" s="20" t="s">
         <v>101</v>
       </c>
-      <c r="N14" s="12"/>
-      <c r="O14" s="12"/>
+      <c r="N14" s="22"/>
+      <c r="O14" s="22"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C15" s="19" t="s">
+      <c r="C15" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="12" t="s">
+      <c r="D15" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="10" t="s">
+      <c r="E15" s="22"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="I15" s="12"/>
-      <c r="J15" s="12"/>
-      <c r="K15" s="19" t="s">
+      <c r="I15" s="22"/>
+      <c r="J15" s="22"/>
+      <c r="K15" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="L15" s="12"/>
-      <c r="M15" s="12" t="s">
+      <c r="L15" s="22"/>
+      <c r="M15" s="20" t="s">
         <v>95</v>
       </c>
-      <c r="N15" s="12"/>
-      <c r="O15" s="12"/>
+      <c r="N15" s="22"/>
+      <c r="O15" s="22"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C16" s="19" t="s">
+      <c r="C16" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="D16" s="12" t="s">
+      <c r="D16" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="19" t="s">
+      <c r="E16" s="22"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="I16" s="12"/>
-      <c r="J16" s="12"/>
-      <c r="K16" s="12"/>
-      <c r="L16" s="12"/>
-      <c r="M16" s="12" t="s">
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
+      <c r="K16" s="22"/>
+      <c r="L16" s="22"/>
+      <c r="M16" s="20" t="s">
         <v>102</v>
       </c>
-      <c r="N16" s="12"/>
-      <c r="O16" s="12"/>
+      <c r="N16" s="22"/>
+      <c r="O16" s="22"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C17" s="19" t="s">
+      <c r="C17" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="D17" s="19" t="s">
+      <c r="D17" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="19" t="s">
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="I17" s="12"/>
-      <c r="J17" s="12"/>
-      <c r="K17" s="12"/>
-      <c r="L17" s="12"/>
-      <c r="M17" s="12" t="s">
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
+      <c r="K17" s="22"/>
+      <c r="L17" s="22"/>
+      <c r="M17" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="N17" s="12"/>
-      <c r="O17" s="12"/>
+      <c r="N17" s="22"/>
+      <c r="O17" s="22"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C18" s="22" t="s">
+      <c r="C18" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D18" s="14" t="s">
+      <c r="D18" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="19" t="s">
+      <c r="E18" s="22"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="I18" s="12"/>
-      <c r="J18" s="12"/>
-      <c r="K18" s="12"/>
-      <c r="L18" s="12"/>
-      <c r="M18" s="12" t="s">
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
+      <c r="K18" s="22"/>
+      <c r="L18" s="22"/>
+      <c r="M18" s="22" t="s">
         <v>96</v>
       </c>
-      <c r="N18" s="12"/>
-      <c r="O18" s="12"/>
+      <c r="N18" s="22"/>
+      <c r="O18" s="22"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C19" s="19" t="s">
+      <c r="C19" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="D19" s="19" t="s">
+      <c r="D19" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="12"/>
-      <c r="J19" s="12"/>
-      <c r="K19" s="12"/>
-      <c r="L19" s="12"/>
-      <c r="M19" s="12" t="s">
+      <c r="E19" s="22"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="22"/>
+      <c r="H19" s="22"/>
+      <c r="I19" s="22"/>
+      <c r="J19" s="22"/>
+      <c r="K19" s="22"/>
+      <c r="L19" s="22"/>
+      <c r="M19" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="N19" s="12"/>
-      <c r="O19" s="12"/>
+      <c r="N19" s="22"/>
+      <c r="O19" s="22"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C20" s="19" t="s">
+      <c r="C20" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="D20" s="19" t="s">
+      <c r="D20" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="12"/>
-      <c r="H20" s="12"/>
-      <c r="I20" s="12"/>
-      <c r="J20" s="12"/>
-      <c r="K20" s="12"/>
-      <c r="L20" s="12"/>
-      <c r="M20" s="12"/>
-      <c r="N20" s="12"/>
-      <c r="O20" s="12"/>
+      <c r="E20" s="22"/>
+      <c r="F20" s="22"/>
+      <c r="G20" s="22"/>
+      <c r="H20" s="22"/>
+      <c r="I20" s="22"/>
+      <c r="J20" s="22"/>
+      <c r="K20" s="22"/>
+      <c r="L20" s="22"/>
+      <c r="M20" s="22"/>
+      <c r="N20" s="22"/>
+      <c r="O20" s="22"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C21" s="19" t="s">
+      <c r="C21" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="D21" s="22" t="s">
+      <c r="D21" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="12"/>
-      <c r="J21" s="12"/>
-      <c r="K21" s="12"/>
-      <c r="L21" s="12"/>
-      <c r="M21" s="12"/>
-      <c r="N21" s="12"/>
-      <c r="O21" s="12"/>
+      <c r="E21" s="22"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="22"/>
+      <c r="H21" s="22"/>
+      <c r="I21" s="22"/>
+      <c r="J21" s="22"/>
+      <c r="K21" s="22"/>
+      <c r="L21" s="22"/>
+      <c r="M21" s="22"/>
+      <c r="N21" s="22"/>
+      <c r="O21" s="22"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C22" s="19" t="s">
+      <c r="C22" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="12"/>
-      <c r="H22" s="12"/>
-      <c r="I22" s="12"/>
-      <c r="J22" s="12"/>
-      <c r="K22" s="12"/>
-      <c r="L22" s="12"/>
-      <c r="M22" s="12"/>
-      <c r="N22" s="12"/>
-      <c r="O22" s="12"/>
+      <c r="D22" s="22"/>
+      <c r="E22" s="22"/>
+      <c r="F22" s="22"/>
+      <c r="G22" s="22"/>
+      <c r="H22" s="22"/>
+      <c r="I22" s="22"/>
+      <c r="J22" s="22"/>
+      <c r="K22" s="22"/>
+      <c r="L22" s="22"/>
+      <c r="M22" s="22"/>
+      <c r="N22" s="22"/>
+      <c r="O22" s="22"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C23" s="19" t="s">
+      <c r="C23" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="25"/>
-      <c r="H23" s="25"/>
-      <c r="I23" s="25"/>
-      <c r="J23" s="25"/>
-      <c r="K23" s="12"/>
-      <c r="L23" s="12"/>
-      <c r="M23" s="12"/>
-      <c r="N23" s="12"/>
-      <c r="O23" s="12"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="22"/>
+      <c r="F23" s="22"/>
+      <c r="G23" s="30"/>
+      <c r="H23" s="30"/>
+      <c r="I23" s="30"/>
+      <c r="J23" s="30"/>
+      <c r="K23" s="22"/>
+      <c r="L23" s="22"/>
+      <c r="M23" s="22"/>
+      <c r="N23" s="22"/>
+      <c r="O23" s="22"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C24" s="19" t="s">
+      <c r="C24" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="D24" s="12"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="12"/>
-      <c r="I24" s="12"/>
-      <c r="J24" s="12"/>
-      <c r="K24" s="12"/>
-      <c r="L24" s="12"/>
-      <c r="M24" s="12"/>
-      <c r="N24" s="12"/>
-      <c r="O24" s="12"/>
+      <c r="D24" s="22"/>
+      <c r="E24" s="22"/>
+      <c r="F24" s="25"/>
+      <c r="G24" s="25"/>
+      <c r="H24" s="22"/>
+      <c r="I24" s="22"/>
+      <c r="J24" s="22"/>
+      <c r="K24" s="22"/>
+      <c r="L24" s="22"/>
+      <c r="M24" s="22"/>
+      <c r="N24" s="22"/>
+      <c r="O24" s="22"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="F25" s="4"/>
@@ -2765,7 +2855,7 @@
       <c r="G26" s="4"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="7" t="s">
         <v>131</v>
       </c>
       <c r="E27" s="4"/>
@@ -2781,7 +2871,7 @@
       <c r="O27" s="4"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="7" t="s">
         <v>139</v>
       </c>
       <c r="E28" s="4"/>
@@ -2845,7 +2935,7 @@
       <c r="O31" s="4"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B32" s="2" t="s">
+      <c r="B32" s="7" t="s">
         <v>123</v>
       </c>
       <c r="E32" s="4"/>
@@ -2861,11 +2951,8 @@
       <c r="O32" s="4"/>
     </row>
     <row r="33" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B33" s="7" t="s">
+      <c r="B33" s="32" t="s">
         <v>128</v>
-      </c>
-      <c r="C33" t="s">
-        <v>373</v>
       </c>
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
@@ -2896,11 +2983,8 @@
       <c r="O34" s="4"/>
     </row>
     <row r="35" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B35" s="9" t="s">
+      <c r="B35" s="7" t="s">
         <v>119</v>
-      </c>
-      <c r="C35" t="s">
-        <v>373</v>
       </c>
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
@@ -2947,15 +3031,12 @@
       <c r="O37" s="4"/>
     </row>
     <row r="38" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B38" s="9" t="s">
+      <c r="B38" s="7" t="s">
         <v>117</v>
-      </c>
-      <c r="C38" t="s">
-        <v>373</v>
       </c>
       <c r="E38" s="4"/>
       <c r="F38" s="4"/>
-      <c r="G38" s="26"/>
+      <c r="G38" s="24"/>
       <c r="H38" s="4"/>
       <c r="I38" s="4"/>
       <c r="J38" s="4"/>
@@ -2966,15 +3047,12 @@
       <c r="O38" s="4"/>
     </row>
     <row r="39" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B39" s="9" t="s">
+      <c r="B39" s="7" t="s">
         <v>118</v>
-      </c>
-      <c r="C39" t="s">
-        <v>373</v>
       </c>
       <c r="E39" s="4"/>
       <c r="F39" s="4"/>
-      <c r="G39" s="26"/>
+      <c r="G39" s="24"/>
       <c r="H39" s="4"/>
       <c r="I39" s="4"/>
       <c r="J39" s="4"/>
@@ -2985,12 +3063,12 @@
       <c r="O39" s="4"/>
     </row>
     <row r="40" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B40" s="2" t="s">
+      <c r="B40" s="7" t="s">
         <v>136</v>
       </c>
       <c r="E40" s="4"/>
       <c r="F40" s="4"/>
-      <c r="G40" s="26"/>
+      <c r="G40" s="24"/>
       <c r="H40" s="4"/>
       <c r="I40" s="4"/>
       <c r="J40" s="4"/>
@@ -3001,15 +3079,12 @@
       <c r="O40" s="4"/>
     </row>
     <row r="41" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B41" s="9" t="s">
+      <c r="B41" s="7" t="s">
         <v>122</v>
-      </c>
-      <c r="C41" t="s">
-        <v>373</v>
       </c>
       <c r="E41" s="4"/>
       <c r="F41" s="4"/>
-      <c r="G41" s="26"/>
+      <c r="G41" s="24"/>
       <c r="H41" s="4"/>
       <c r="I41" s="4"/>
       <c r="J41" s="4"/>
@@ -3025,7 +3100,7 @@
       </c>
       <c r="E42" s="4"/>
       <c r="F42" s="4"/>
-      <c r="G42" s="26"/>
+      <c r="G42" s="24"/>
       <c r="H42" s="4"/>
       <c r="I42" s="4"/>
       <c r="J42" s="4"/>
@@ -3036,11 +3111,8 @@
       <c r="O42" s="4"/>
     </row>
     <row r="43" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B43" s="9" t="s">
+      <c r="B43" s="7" t="s">
         <v>140</v>
-      </c>
-      <c r="C43" t="s">
-        <v>373</v>
       </c>
       <c r="E43" s="4"/>
       <c r="F43" s="4"/>
@@ -3060,7 +3132,7 @@
       </c>
       <c r="E44" s="4"/>
       <c r="F44" s="4"/>
-      <c r="G44" s="27"/>
+      <c r="G44" s="25"/>
       <c r="H44" s="4"/>
       <c r="I44" s="4"/>
       <c r="J44" s="4"/>
@@ -3071,21 +3143,18 @@
       <c r="O44" s="4"/>
     </row>
     <row r="45" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B45" s="9" t="s">
+      <c r="B45" s="7" t="s">
         <v>120</v>
-      </c>
-      <c r="C45" t="s">
-        <v>373</v>
       </c>
       <c r="F45" s="4"/>
       <c r="G45" s="4"/>
     </row>
     <row r="46" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B46" s="2" t="s">
+      <c r="B46" s="7" t="s">
         <v>132</v>
       </c>
       <c r="F46" s="4"/>
-      <c r="G46" s="26"/>
+      <c r="G46" s="24"/>
     </row>
     <row r="47" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B47" s="7" t="s">
@@ -3095,31 +3164,25 @@
       <c r="G47" s="4"/>
     </row>
     <row r="48" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B48" s="2" t="s">
+      <c r="B48" s="7" t="s">
         <v>130</v>
       </c>
       <c r="F48" s="4"/>
-      <c r="G48" s="26"/>
+      <c r="G48" s="24"/>
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B49" s="9" t="s">
+      <c r="B49" s="32" t="s">
         <v>138</v>
       </c>
-      <c r="C49" t="s">
-        <v>373</v>
-      </c>
     </row>
     <row r="50" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B50" s="2" t="s">
+      <c r="B50" s="7" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="51" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B51" s="9" t="s">
+      <c r="B51" s="7" t="s">
         <v>121</v>
-      </c>
-      <c r="C51" t="s">
-        <v>373</v>
       </c>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.25">
@@ -3217,7 +3280,7 @@
       <c r="N55" s="9" t="s">
         <v>299</v>
       </c>
-      <c r="O55" s="28" t="s">
+      <c r="O55" s="26" t="s">
         <v>318</v>
       </c>
       <c r="P55" s="2" t="s">
@@ -3234,7 +3297,7 @@
       <c r="D56" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="E56" s="5" t="s">
+      <c r="E56" s="31" t="s">
         <v>212</v>
       </c>
       <c r="F56" s="5" t="s">
@@ -3253,7 +3316,7 @@
       <c r="K56" s="5" t="s">
         <v>293</v>
       </c>
-      <c r="N56" s="26" t="s">
+      <c r="N56" s="24" t="s">
         <v>300</v>
       </c>
       <c r="O56" s="2" t="s">
@@ -3288,7 +3351,7 @@
       <c r="I57" s="5" t="s">
         <v>274</v>
       </c>
-      <c r="N57" s="26" t="s">
+      <c r="N57" s="24" t="s">
         <v>301</v>
       </c>
       <c r="O57" s="5" t="s">
@@ -3349,7 +3412,7 @@
       <c r="I59" s="5" t="s">
         <v>276</v>
       </c>
-      <c r="N59" s="26" t="s">
+      <c r="N59" s="24" t="s">
         <v>303</v>
       </c>
       <c r="O59" s="5" t="s">
@@ -3378,7 +3441,7 @@
       <c r="I60" s="5" t="s">
         <v>277</v>
       </c>
-      <c r="N60" s="26" t="s">
+      <c r="N60" s="24" t="s">
         <v>304</v>
       </c>
       <c r="O60" s="5" t="s">
@@ -3404,10 +3467,10 @@
       <c r="H61" s="5" t="s">
         <v>244</v>
       </c>
-      <c r="I61" s="5" t="s">
+      <c r="I61" s="31" t="s">
         <v>278</v>
       </c>
-      <c r="N61" s="26" t="s">
+      <c r="N61" s="24" t="s">
         <v>305</v>
       </c>
       <c r="O61" s="2" t="s">
@@ -3436,7 +3499,7 @@
       <c r="I62" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="N62" s="26" t="s">
+      <c r="N62" s="24" t="s">
         <v>306</v>
       </c>
       <c r="O62" s="5" t="s">
@@ -3465,7 +3528,7 @@
       <c r="I63" s="5" t="s">
         <v>280</v>
       </c>
-      <c r="N63" s="26" t="s">
+      <c r="N63" s="24" t="s">
         <v>307</v>
       </c>
       <c r="O63" s="9" t="s">
@@ -3494,7 +3557,7 @@
       <c r="I64" s="5" t="s">
         <v>281</v>
       </c>
-      <c r="N64" s="26" t="s">
+      <c r="N64" s="24" t="s">
         <v>308</v>
       </c>
       <c r="P64" s="5" t="s">
@@ -3520,7 +3583,7 @@
       <c r="I65" s="5" t="s">
         <v>282</v>
       </c>
-      <c r="N65" s="26" t="s">
+      <c r="N65" s="24" t="s">
         <v>309</v>
       </c>
       <c r="P65" s="5" t="s">
@@ -3540,7 +3603,7 @@
       <c r="I66" s="5" t="s">
         <v>283</v>
       </c>
-      <c r="N66" s="26" t="s">
+      <c r="N66" s="24" t="s">
         <v>310</v>
       </c>
       <c r="P66" s="5" t="s">
@@ -3560,7 +3623,7 @@
       <c r="I67" s="5" t="s">
         <v>284</v>
       </c>
-      <c r="N67" s="26" t="s">
+      <c r="N67" s="24" t="s">
         <v>311</v>
       </c>
       <c r="P67" s="5" t="s">
@@ -3580,7 +3643,7 @@
       <c r="I68" s="5" t="s">
         <v>285</v>
       </c>
-      <c r="N68" s="26" t="s">
+      <c r="N68" s="24" t="s">
         <v>312</v>
       </c>
       <c r="P68" s="5" t="s">
@@ -3597,7 +3660,7 @@
       <c r="I69" s="5" t="s">
         <v>286</v>
       </c>
-      <c r="N69" s="26" t="s">
+      <c r="N69" s="24" t="s">
         <v>313</v>
       </c>
       <c r="P69" s="5" t="s">
@@ -3614,7 +3677,7 @@
       <c r="I70" s="5" t="s">
         <v>287</v>
       </c>
-      <c r="N70" s="26" t="s">
+      <c r="N70" s="24" t="s">
         <v>314</v>
       </c>
       <c r="P70" s="5" t="s">
@@ -3833,8 +3896,8 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="E56:E65">
-    <sortCondition ref="E55:E65"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="M8:M19">
+    <sortCondition ref="M7:M19"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3858,62 +3921,62 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
@@ -3923,62 +3986,62 @@
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
@@ -3988,7 +4051,7 @@
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
@@ -4003,7 +4066,7 @@
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
@@ -4018,7 +4081,7 @@
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
@@ -4033,7 +4096,7 @@
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
@@ -4053,7 +4116,7 @@
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="8" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
@@ -4093,7 +4156,7 @@
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="8" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
@@ -4123,22 +4186,22 @@
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="8" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="8" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="8" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="8" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
@@ -4153,7 +4216,7 @@
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
@@ -4178,12 +4241,12 @@
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" s="8" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" s="8" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
@@ -4193,7 +4256,7 @@
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" s="8" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
@@ -4228,7 +4291,7 @@
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" s="8" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
@@ -4248,7 +4311,7 @@
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" s="8" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
@@ -4283,192 +4346,192 @@
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" s="8" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" s="8" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" s="8" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" s="8" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" s="8" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" s="8" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" s="8" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" s="8" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" s="8" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" s="8" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" s="8" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" s="8" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" s="8" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" s="8" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" s="8" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" s="8" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103" s="8" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" s="8" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105" s="8" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" s="8" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" s="8" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108" s="8" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109" s="8" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110" s="8" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111" s="8" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112" s="8" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113" s="8" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114" s="8" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115" s="8" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116" s="8" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117" s="8" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118" s="8" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A119" s="8" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A120" s="8" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A121" s="8" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A122" s="8" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A123" s="8" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A124" s="8" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.25">
@@ -4478,17 +4541,17 @@
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A126" s="8" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A127" s="8" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A128" s="8" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.25">
@@ -4498,7 +4561,7 @@
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A130" s="8" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.25">
@@ -4508,62 +4571,62 @@
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A132" s="8" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A133" s="8" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A134" s="8" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A135" s="8" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A136" s="8" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A137" s="8" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A138" s="8" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A139" s="8" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A140" s="8" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A141" s="8" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A142" s="8" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A143" s="8" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.25">
@@ -4578,7 +4641,7 @@
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A146" s="8" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.25">
@@ -4588,7 +4651,7 @@
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A148" s="8" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.25">
@@ -4598,52 +4661,52 @@
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A150" s="8" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A151" s="8" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A152" s="8" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A153" s="8" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A154" s="8" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A155" s="8" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A156" s="8" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A157" s="8" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A158" s="8" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A159" s="8" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.25">
@@ -4653,22 +4716,22 @@
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A161" s="8" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A162" s="8" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A163" s="8" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A164" s="8" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.25">
@@ -4808,7 +4871,7 @@
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A192" s="8" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.25">
@@ -4838,7 +4901,7 @@
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A198" s="8" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.25">
@@ -4913,7 +4976,7 @@
     </row>
     <row r="213" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A213" s="8" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="214" spans="1:1" x14ac:dyDescent="0.25">
@@ -5423,25 +5486,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EED08F7F-A003-4C3B-8646-FC85C271AAFB}">
-  <dimension ref="A1:Q163"/>
+  <dimension ref="A1:T163"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A110" workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="S72" sqref="S72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="15"/>
-    <col min="2" max="2" width="18.42578125" style="12" customWidth="1"/>
-    <col min="3" max="3" width="19.140625" style="12" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" style="12" customWidth="1"/>
-    <col min="5" max="5" width="20.28515625" style="12" customWidth="1"/>
-    <col min="6" max="6" width="21" style="12" customWidth="1"/>
-    <col min="7" max="7" width="17.140625" style="12" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" style="12"/>
-    <col min="9" max="9" width="15.42578125" style="12" customWidth="1"/>
-    <col min="10" max="10" width="16.140625" style="12" customWidth="1"/>
-    <col min="11" max="11" width="17.140625" style="12" customWidth="1"/>
+    <col min="1" max="1" width="20.5703125" style="15" customWidth="1"/>
+    <col min="2" max="11" width="20.5703125" style="12" customWidth="1"/>
+    <col min="12" max="20" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -5498,21 +5553,21 @@
       <c r="A15" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="B15" s="29" t="s">
+      <c r="B15" s="27" t="s">
         <v>357</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B16" s="11" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B18" s="12" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
@@ -5544,10 +5599,10 @@
         <v>359</v>
       </c>
       <c r="C25" s="12" t="s">
+        <v>521</v>
+      </c>
+      <c r="D25" s="12" t="s">
         <v>522</v>
-      </c>
-      <c r="D25" s="12" t="s">
-        <v>523</v>
       </c>
       <c r="M25" s="4"/>
       <c r="N25" s="4"/>
@@ -5560,11 +5615,11 @@
         <v>364</v>
       </c>
       <c r="D26" s="17" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="E26" s="18"/>
       <c r="G26" s="8" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="M26" s="4"/>
       <c r="N26" s="10"/>
@@ -5577,7 +5632,7 @@
         <v>324</v>
       </c>
       <c r="E27" s="18" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="G27" s="8"/>
       <c r="M27" s="4"/>
@@ -5591,7 +5646,7 @@
         <v>155</v>
       </c>
       <c r="E28" s="18" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="G28"/>
       <c r="M28" s="4"/>
@@ -5605,7 +5660,7 @@
         <v>152</v>
       </c>
       <c r="E29" s="18" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="M29" s="4"/>
       <c r="N29" s="10"/>
@@ -5618,7 +5673,7 @@
         <v>158</v>
       </c>
       <c r="E30" s="18" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="M30" s="4"/>
       <c r="N30" s="10"/>
@@ -5631,7 +5686,7 @@
         <v>192</v>
       </c>
       <c r="E31" s="18" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="M31" s="4"/>
       <c r="N31" s="10"/>
@@ -5644,7 +5699,7 @@
         <v>189</v>
       </c>
       <c r="E32" s="18" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="M32" s="4"/>
       <c r="N32" s="10"/>
@@ -5654,7 +5709,7 @@
         <v>367</v>
       </c>
       <c r="D33" s="10" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="E33" s="18"/>
       <c r="M33" s="4"/>
@@ -5681,7 +5736,7 @@
         <v>170</v>
       </c>
       <c r="E35" s="18" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="M35" s="4"/>
       <c r="N35" s="10"/>
@@ -5694,7 +5749,7 @@
         <v>157</v>
       </c>
       <c r="E36" s="18" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="M36" s="4"/>
       <c r="N36" s="10"/>
@@ -5707,7 +5762,7 @@
         <v>65</v>
       </c>
       <c r="E37" s="19" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="38" spans="3:14" x14ac:dyDescent="0.25">
@@ -5718,7 +5773,7 @@
         <v>160</v>
       </c>
       <c r="E38" s="18" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="39" spans="3:14" x14ac:dyDescent="0.25">
@@ -5726,7 +5781,7 @@
         <v>371</v>
       </c>
       <c r="D39" s="10" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E39" s="18"/>
     </row>
@@ -5738,7 +5793,7 @@
         <v>161</v>
       </c>
       <c r="E40" s="18" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="41" spans="3:14" x14ac:dyDescent="0.25">
@@ -5749,7 +5804,7 @@
         <v>174</v>
       </c>
       <c r="E41" s="18" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="42" spans="3:14" x14ac:dyDescent="0.25">
@@ -5760,7 +5815,7 @@
         <v>257</v>
       </c>
       <c r="E42" s="18" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="43" spans="3:14" x14ac:dyDescent="0.25">
@@ -5771,7 +5826,7 @@
         <v>201</v>
       </c>
       <c r="E43" s="18" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="44" spans="3:14" x14ac:dyDescent="0.25">
@@ -5782,7 +5837,7 @@
         <v>226</v>
       </c>
       <c r="E44" s="18" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="45" spans="3:14" x14ac:dyDescent="0.25">
@@ -5790,15 +5845,15 @@
         <v>323</v>
       </c>
       <c r="E45" s="18" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="46" spans="3:14" x14ac:dyDescent="0.25">
       <c r="D46" s="11" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="E46" s="18" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="47" spans="3:14" x14ac:dyDescent="0.25">
@@ -5806,7 +5861,7 @@
         <v>354</v>
       </c>
       <c r="E47" s="18" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="48" spans="3:14" x14ac:dyDescent="0.25">
@@ -5814,26 +5869,26 @@
         <v>153</v>
       </c>
       <c r="E48" s="18" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
       <c r="D49" s="12" t="s">
         <v>162</v>
       </c>
       <c r="E49" s="18" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
       <c r="D50" s="12" t="s">
         <v>194</v>
       </c>
       <c r="E50" s="18" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A55" s="15" t="s">
         <v>143</v>
       </c>
@@ -5841,620 +5896,757 @@
         <v>360</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B56" s="15" t="s">
         <v>114</v>
       </c>
       <c r="C56" s="12" t="s">
-        <v>534</v>
+        <v>545</v>
       </c>
       <c r="D56" s="12" t="s">
         <v>533</v>
       </c>
       <c r="E56" s="12" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
       <c r="F56" s="12" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="G56" s="12" t="s">
-        <v>418</v>
+        <v>537</v>
       </c>
       <c r="H56" s="12" t="s">
+        <v>417</v>
+      </c>
+      <c r="I56" s="12" t="s">
+        <v>419</v>
+      </c>
+      <c r="J56" s="12" t="s">
         <v>420</v>
       </c>
-      <c r="I56" s="12" t="s">
+      <c r="K56" s="12" t="s">
         <v>421</v>
       </c>
-      <c r="J56" s="12" t="s">
+      <c r="L56" s="12" t="s">
+        <v>529</v>
+      </c>
+      <c r="M56" s="12" t="s">
+        <v>539</v>
+      </c>
+      <c r="N56" s="12" t="s">
         <v>422</v>
       </c>
-      <c r="K56" s="12" t="s">
-        <v>530</v>
-      </c>
-      <c r="L56" s="12" t="s">
-        <v>540</v>
-      </c>
-      <c r="M56" s="12" t="s">
+      <c r="O56" s="12" t="s">
         <v>423</v>
       </c>
-      <c r="N56" s="12" t="s">
-        <v>424</v>
-      </c>
-      <c r="O56" s="12" t="s">
-        <v>480</v>
-      </c>
       <c r="P56" s="12" t="s">
-        <v>506</v>
+        <v>479</v>
       </c>
       <c r="Q56" s="12" t="s">
-        <v>519</v>
-      </c>
-    </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+        <v>505</v>
+      </c>
+      <c r="R56" s="12" t="s">
+        <v>547</v>
+      </c>
+      <c r="S56" s="12" t="s">
+        <v>551</v>
+      </c>
+      <c r="T56" s="12" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B57" s="15"/>
       <c r="C57" s="14" t="s">
-        <v>535</v>
+        <v>546</v>
       </c>
       <c r="D57" s="14" t="s">
-        <v>532</v>
+        <v>534</v>
       </c>
       <c r="E57" s="14" t="s">
-        <v>537</v>
+        <v>531</v>
       </c>
       <c r="F57" s="14" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="G57" s="14" t="s">
-        <v>419</v>
+        <v>538</v>
       </c>
       <c r="H57" s="14" t="s">
+        <v>418</v>
+      </c>
+      <c r="I57" s="14" t="s">
+        <v>424</v>
+      </c>
+      <c r="J57" s="12" t="s">
+        <v>525</v>
+      </c>
+      <c r="K57" s="28" t="s">
+        <v>472</v>
+      </c>
+      <c r="L57" s="14" t="s">
+        <v>530</v>
+      </c>
+      <c r="M57" s="14" t="s">
+        <v>540</v>
+      </c>
+      <c r="N57" s="12" t="s">
+        <v>475</v>
+      </c>
+      <c r="O57" s="12" t="s">
+        <v>478</v>
+      </c>
+      <c r="P57" s="28" t="s">
+        <v>480</v>
+      </c>
+      <c r="Q57" s="2" t="s">
+        <v>578</v>
+      </c>
+      <c r="R57" s="12" t="s">
+        <v>548</v>
+      </c>
+      <c r="S57" s="12" t="s">
+        <v>552</v>
+      </c>
+      <c r="T57" s="14" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B58" s="15"/>
+      <c r="J58" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="K58" s="12" t="s">
+        <v>473</v>
+      </c>
+      <c r="L58" s="12"/>
+      <c r="N58" s="14" t="s">
+        <v>476</v>
+      </c>
+      <c r="O58" s="14" t="s">
+        <v>542</v>
+      </c>
+      <c r="P58" s="12" t="s">
+        <v>481</v>
+      </c>
+      <c r="Q58" s="2" t="s">
+        <v>567</v>
+      </c>
+      <c r="R58" s="14" t="s">
+        <v>430</v>
+      </c>
+      <c r="S58" s="14" t="s">
         <v>425</v>
       </c>
-      <c r="I57" s="12" t="s">
-        <v>526</v>
-      </c>
-      <c r="J57" s="30" t="s">
-        <v>473</v>
-      </c>
-      <c r="K57" s="14" t="s">
-        <v>531</v>
-      </c>
-      <c r="L57" s="14" t="s">
+    </row>
+    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B59" s="15"/>
+      <c r="J59" s="12" t="s">
+        <v>427</v>
+      </c>
+      <c r="K59" s="14" t="s">
+        <v>543</v>
+      </c>
+      <c r="L59" s="12"/>
+      <c r="N59" s="12" t="s">
+        <v>477</v>
+      </c>
+      <c r="O59" s="12"/>
+      <c r="P59" s="28" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q59" s="2" t="s">
+        <v>555</v>
+      </c>
+      <c r="R59" s="12" t="s">
+        <v>549</v>
+      </c>
+      <c r="S59" s="12" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B60" s="15"/>
+      <c r="J60" s="14" t="s">
+        <v>428</v>
+      </c>
+      <c r="K60" s="14" t="s">
+        <v>474</v>
+      </c>
+      <c r="L60" s="12"/>
+      <c r="N60" s="12"/>
+      <c r="O60" s="12"/>
+      <c r="P60" s="12" t="s">
+        <v>483</v>
+      </c>
+      <c r="Q60" s="2" t="s">
+        <v>566</v>
+      </c>
+      <c r="R60" s="14" t="s">
+        <v>550</v>
+      </c>
+      <c r="S60" s="14" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B61" s="15"/>
+      <c r="J61" s="12" t="s">
+        <v>429</v>
+      </c>
+      <c r="K61" s="12" t="s">
+        <v>434</v>
+      </c>
+      <c r="L61" s="12"/>
+      <c r="N61" s="12"/>
+      <c r="O61" s="12"/>
+      <c r="P61" s="12" t="s">
+        <v>484</v>
+      </c>
+      <c r="Q61" s="14" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B62" s="15"/>
+      <c r="J62" s="14" t="s">
+        <v>430</v>
+      </c>
+      <c r="K62" s="28" t="s">
+        <v>435</v>
+      </c>
+      <c r="L62" s="12"/>
+      <c r="N62" s="12"/>
+      <c r="O62" s="12"/>
+      <c r="P62" s="28" t="s">
+        <v>485</v>
+      </c>
+      <c r="Q62" s="14" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B63" s="15"/>
+      <c r="J63" s="12" t="s">
+        <v>431</v>
+      </c>
+      <c r="K63" s="12" t="s">
+        <v>436</v>
+      </c>
+      <c r="L63" s="12"/>
+      <c r="N63" s="12"/>
+      <c r="O63" s="12"/>
+      <c r="P63" s="12" t="s">
+        <v>486</v>
+      </c>
+      <c r="Q63" s="14" t="s">
+        <v>558</v>
+      </c>
+      <c r="R63" s="12"/>
+    </row>
+    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B64" s="15"/>
+      <c r="J64" s="12" t="s">
+        <v>432</v>
+      </c>
+      <c r="K64" s="12" t="s">
+        <v>437</v>
+      </c>
+      <c r="L64" s="12"/>
+      <c r="N64" s="12"/>
+      <c r="O64" s="12"/>
+      <c r="P64" s="12" t="s">
+        <v>487</v>
+      </c>
+      <c r="Q64" s="14" t="s">
+        <v>563</v>
+      </c>
+      <c r="R64" s="12"/>
+    </row>
+    <row r="65" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B65" s="15"/>
+      <c r="K65" s="14" t="s">
+        <v>438</v>
+      </c>
+      <c r="L65" s="12"/>
+      <c r="N65" s="12"/>
+      <c r="O65" s="12"/>
+      <c r="P65" s="12" t="s">
+        <v>488</v>
+      </c>
+      <c r="Q65" s="14" t="s">
+        <v>561</v>
+      </c>
+      <c r="R65" s="12"/>
+    </row>
+    <row r="66" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B66" s="15"/>
+      <c r="K66" s="12" t="s">
+        <v>439</v>
+      </c>
+      <c r="L66" s="12"/>
+      <c r="N66" s="12"/>
+      <c r="O66" s="12"/>
+      <c r="P66" s="12" t="s">
+        <v>489</v>
+      </c>
+      <c r="Q66" s="14" t="s">
+        <v>573</v>
+      </c>
+      <c r="R66" s="12"/>
+    </row>
+    <row r="67" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B67" s="15"/>
+      <c r="K67" s="12" t="s">
+        <v>440</v>
+      </c>
+      <c r="L67" s="12"/>
+      <c r="N67" s="12"/>
+      <c r="O67" s="12"/>
+      <c r="P67" s="12" t="s">
+        <v>490</v>
+      </c>
+      <c r="Q67" s="14" t="s">
+        <v>508</v>
+      </c>
+      <c r="R67" s="12"/>
+    </row>
+    <row r="68" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B68" s="15"/>
+      <c r="K68" s="12" t="s">
+        <v>441</v>
+      </c>
+      <c r="L68" s="12"/>
+      <c r="N68" s="12"/>
+      <c r="O68" s="12"/>
+      <c r="P68" s="12" t="s">
+        <v>491</v>
+      </c>
+      <c r="Q68" s="14" t="s">
+        <v>556</v>
+      </c>
+      <c r="R68" s="12"/>
+    </row>
+    <row r="69" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B69" s="15"/>
+      <c r="K69" s="12" t="s">
+        <v>442</v>
+      </c>
+      <c r="L69" s="12"/>
+      <c r="N69" s="12"/>
+      <c r="O69" s="12"/>
+      <c r="P69" s="12" t="s">
+        <v>492</v>
+      </c>
+      <c r="Q69" s="14" t="s">
+        <v>509</v>
+      </c>
+      <c r="R69" s="12"/>
+    </row>
+    <row r="70" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B70" s="15"/>
+      <c r="K70" s="12" t="s">
+        <v>443</v>
+      </c>
+      <c r="L70" s="12"/>
+      <c r="N70" s="12"/>
+      <c r="O70" s="12"/>
+      <c r="P70" s="12" t="s">
+        <v>493</v>
+      </c>
+      <c r="Q70" s="14" t="s">
+        <v>554</v>
+      </c>
+      <c r="R70" s="12"/>
+    </row>
+    <row r="71" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="K71" s="12" t="s">
+        <v>444</v>
+      </c>
+      <c r="L71" s="12"/>
+      <c r="N71" s="12"/>
+      <c r="O71" s="12"/>
+      <c r="P71" s="12" t="s">
+        <v>494</v>
+      </c>
+      <c r="Q71" s="14" t="s">
+        <v>510</v>
+      </c>
+      <c r="R71" s="12"/>
+    </row>
+    <row r="72" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="K72" s="12" t="s">
+        <v>445</v>
+      </c>
+      <c r="L72" s="12"/>
+      <c r="N72" s="12"/>
+      <c r="O72" s="12"/>
+      <c r="P72" s="12" t="s">
+        <v>495</v>
+      </c>
+      <c r="Q72" s="14" t="s">
+        <v>577</v>
+      </c>
+      <c r="R72" s="12"/>
+    </row>
+    <row r="73" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="K73" s="28" t="s">
+        <v>446</v>
+      </c>
+      <c r="L73" s="12"/>
+      <c r="N73" s="12"/>
+      <c r="O73" s="12"/>
+      <c r="P73" s="12" t="s">
+        <v>496</v>
+      </c>
+      <c r="Q73" s="14" t="s">
+        <v>564</v>
+      </c>
+      <c r="R73" s="12"/>
+    </row>
+    <row r="74" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="K74" s="12" t="s">
+        <v>447</v>
+      </c>
+      <c r="L74" s="12"/>
+      <c r="N74" s="12"/>
+      <c r="O74" s="12"/>
+      <c r="P74" s="12" t="s">
+        <v>497</v>
+      </c>
+      <c r="Q74" s="14" t="s">
+        <v>511</v>
+      </c>
+      <c r="R74" s="12"/>
+    </row>
+    <row r="75" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="K75" s="28" t="s">
+        <v>448</v>
+      </c>
+      <c r="L75" s="12"/>
+      <c r="N75" s="12"/>
+      <c r="O75" s="12"/>
+      <c r="P75" s="12" t="s">
+        <v>498</v>
+      </c>
+      <c r="Q75" s="14" t="s">
+        <v>570</v>
+      </c>
+      <c r="R75" s="12"/>
+    </row>
+    <row r="76" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="K76" s="12" t="s">
+        <v>449</v>
+      </c>
+      <c r="L76" s="12"/>
+      <c r="N76" s="12"/>
+      <c r="O76" s="12"/>
+      <c r="P76" s="12" t="s">
+        <v>499</v>
+      </c>
+      <c r="Q76" s="14" t="s">
+        <v>560</v>
+      </c>
+      <c r="R76" s="12"/>
+    </row>
+    <row r="77" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="K77" s="12" t="s">
+        <v>450</v>
+      </c>
+      <c r="L77" s="12"/>
+      <c r="N77" s="12"/>
+      <c r="O77" s="12"/>
+      <c r="P77" s="12" t="s">
+        <v>500</v>
+      </c>
+      <c r="Q77" s="33" t="s">
+        <v>512</v>
+      </c>
+      <c r="R77" s="12"/>
+    </row>
+    <row r="78" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="K78" s="14" t="s">
+        <v>428</v>
+      </c>
+      <c r="L78" s="12"/>
+      <c r="N78" s="12"/>
+      <c r="O78" s="12"/>
+      <c r="P78" s="28" t="s">
+        <v>501</v>
+      </c>
+      <c r="Q78" s="14" t="s">
+        <v>572</v>
+      </c>
+      <c r="R78" s="12"/>
+    </row>
+    <row r="79" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="K79" s="28" t="s">
+        <v>451</v>
+      </c>
+      <c r="L79" s="12"/>
+      <c r="N79" s="12"/>
+      <c r="O79" s="12"/>
+      <c r="P79" s="12" t="s">
+        <v>502</v>
+      </c>
+      <c r="Q79" s="14" t="s">
+        <v>576</v>
+      </c>
+      <c r="R79" s="12"/>
+    </row>
+    <row r="80" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="K80" s="14" t="s">
+        <v>452</v>
+      </c>
+      <c r="L80" s="12"/>
+      <c r="N80" s="12"/>
+      <c r="O80" s="12"/>
+      <c r="P80" s="12" t="s">
+        <v>503</v>
+      </c>
+      <c r="Q80" s="14" t="s">
+        <v>569</v>
+      </c>
+      <c r="R80" s="12"/>
+    </row>
+    <row r="81" spans="11:18" x14ac:dyDescent="0.25">
+      <c r="K81" s="14" t="s">
         <v>541</v>
       </c>
-      <c r="M57" s="12" t="s">
-        <v>476</v>
-      </c>
-      <c r="N57" s="12" t="s">
-        <v>479</v>
-      </c>
-      <c r="O57" s="30" t="s">
-        <v>481</v>
-      </c>
-      <c r="P57" s="12" t="s">
-        <v>507</v>
-      </c>
-      <c r="Q57" s="14" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B58" s="15"/>
-      <c r="I58" s="12" t="s">
-        <v>426</v>
-      </c>
-      <c r="J58" s="12" t="s">
-        <v>474</v>
-      </c>
-      <c r="M58" s="14" t="s">
-        <v>477</v>
-      </c>
-      <c r="N58" s="14" t="s">
-        <v>543</v>
-      </c>
-      <c r="O58" s="12" t="s">
-        <v>482</v>
-      </c>
-      <c r="P58" s="12" t="s">
-        <v>508</v>
-      </c>
-      <c r="Q58" s="12"/>
-    </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B59" s="15"/>
-      <c r="I59" s="12" t="s">
-        <v>427</v>
-      </c>
-      <c r="J59" s="14" t="s">
-        <v>544</v>
-      </c>
-      <c r="M59" s="12" t="s">
-        <v>478</v>
-      </c>
-      <c r="N59" s="12"/>
-      <c r="O59" s="30" t="s">
-        <v>483</v>
-      </c>
-      <c r="P59" s="12" t="s">
-        <v>509</v>
-      </c>
-      <c r="Q59" s="12"/>
-    </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B60" s="15"/>
-      <c r="I60" s="12" t="s">
-        <v>428</v>
-      </c>
-      <c r="J60" s="14" t="s">
-        <v>475</v>
-      </c>
-      <c r="M60" s="12"/>
-      <c r="N60" s="12"/>
-      <c r="O60" s="12" t="s">
-        <v>484</v>
-      </c>
-      <c r="P60" s="12" t="s">
-        <v>510</v>
-      </c>
-      <c r="Q60" s="12"/>
-    </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B61" s="15"/>
-      <c r="I61" s="30" t="s">
-        <v>429</v>
-      </c>
-      <c r="J61" s="12" t="s">
-        <v>435</v>
-      </c>
-      <c r="M61" s="12"/>
-      <c r="N61" s="12"/>
-      <c r="O61" s="12" t="s">
-        <v>485</v>
-      </c>
-      <c r="P61" s="12" t="s">
-        <v>511</v>
-      </c>
-      <c r="Q61" s="12"/>
-    </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B62" s="15"/>
-      <c r="I62" s="12" t="s">
-        <v>430</v>
-      </c>
-      <c r="J62" s="30" t="s">
-        <v>436</v>
-      </c>
-      <c r="M62" s="12"/>
-      <c r="N62" s="12"/>
-      <c r="O62" s="30" t="s">
-        <v>486</v>
-      </c>
-      <c r="P62" s="12" t="s">
-        <v>512</v>
-      </c>
-      <c r="Q62" s="12"/>
-    </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B63" s="15"/>
-      <c r="I63" s="12" t="s">
-        <v>431</v>
-      </c>
-      <c r="J63" s="12" t="s">
-        <v>437</v>
-      </c>
-      <c r="M63" s="12"/>
-      <c r="N63" s="12"/>
-      <c r="O63" s="12" t="s">
-        <v>487</v>
-      </c>
-      <c r="P63" s="12" t="s">
-        <v>513</v>
-      </c>
-      <c r="Q63" s="12"/>
-    </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B64" s="15"/>
-      <c r="I64" s="12" t="s">
-        <v>432</v>
-      </c>
-      <c r="J64" s="12" t="s">
-        <v>438</v>
-      </c>
-      <c r="M64" s="12"/>
-      <c r="N64" s="12"/>
-      <c r="O64" s="12" t="s">
-        <v>488</v>
-      </c>
-      <c r="P64" s="14" t="s">
-        <v>514</v>
-      </c>
-      <c r="Q64" s="12"/>
-    </row>
-    <row r="65" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B65" s="15"/>
-      <c r="I65" s="12" t="s">
-        <v>433</v>
-      </c>
-      <c r="J65" s="14" t="s">
-        <v>439</v>
-      </c>
-      <c r="M65" s="12"/>
-      <c r="N65" s="12"/>
-      <c r="O65" s="12" t="s">
-        <v>489</v>
-      </c>
-      <c r="P65" s="12" t="s">
-        <v>515</v>
-      </c>
-      <c r="Q65" s="12"/>
-    </row>
-    <row r="66" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B66" s="15"/>
-      <c r="I66" s="12" t="s">
-        <v>434</v>
-      </c>
-      <c r="J66" s="12" t="s">
-        <v>440</v>
-      </c>
-      <c r="M66" s="12"/>
-      <c r="N66" s="12"/>
-      <c r="O66" s="12" t="s">
-        <v>490</v>
-      </c>
-      <c r="P66" s="12" t="s">
-        <v>516</v>
-      </c>
-      <c r="Q66" s="12"/>
-    </row>
-    <row r="67" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B67" s="15"/>
-      <c r="J67" s="12" t="s">
-        <v>441</v>
-      </c>
-      <c r="M67" s="12"/>
-      <c r="N67" s="12"/>
-      <c r="O67" s="12" t="s">
-        <v>491</v>
-      </c>
-      <c r="P67" s="12" t="s">
-        <v>517</v>
-      </c>
-      <c r="Q67" s="12"/>
-    </row>
-    <row r="68" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B68" s="15"/>
-      <c r="J68" s="12" t="s">
-        <v>442</v>
-      </c>
-      <c r="M68" s="12"/>
-      <c r="N68" s="12"/>
-      <c r="O68" s="12" t="s">
-        <v>492</v>
-      </c>
-      <c r="P68" s="12" t="s">
-        <v>518</v>
-      </c>
-      <c r="Q68" s="12"/>
-    </row>
-    <row r="69" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B69" s="15"/>
-      <c r="J69" s="12" t="s">
-        <v>443</v>
-      </c>
-      <c r="M69" s="12"/>
-      <c r="N69" s="12"/>
-      <c r="O69" s="12" t="s">
-        <v>493</v>
-      </c>
-      <c r="P69" s="12"/>
-      <c r="Q69" s="12"/>
-    </row>
-    <row r="70" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B70" s="15"/>
-      <c r="J70" s="12" t="s">
-        <v>444</v>
-      </c>
-      <c r="M70" s="12"/>
-      <c r="N70" s="12"/>
-      <c r="O70" s="12" t="s">
-        <v>494</v>
-      </c>
-      <c r="P70" s="12"/>
-      <c r="Q70" s="12"/>
-    </row>
-    <row r="71" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="J71" s="12" t="s">
-        <v>445</v>
-      </c>
-      <c r="M71" s="12"/>
-      <c r="N71" s="12"/>
-      <c r="O71" s="12" t="s">
-        <v>495</v>
-      </c>
-      <c r="P71" s="12"/>
-      <c r="Q71" s="12"/>
-    </row>
-    <row r="72" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="J72" s="12" t="s">
-        <v>446</v>
-      </c>
-      <c r="M72" s="12"/>
-      <c r="N72" s="12"/>
-      <c r="O72" s="12" t="s">
-        <v>496</v>
-      </c>
-      <c r="P72" s="12"/>
-      <c r="Q72" s="12"/>
-    </row>
-    <row r="73" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="J73" s="30" t="s">
-        <v>447</v>
-      </c>
-      <c r="M73" s="12"/>
-      <c r="N73" s="12"/>
-      <c r="O73" s="12" t="s">
-        <v>497</v>
-      </c>
-      <c r="P73" s="12"/>
-      <c r="Q73" s="12"/>
-    </row>
-    <row r="74" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="J74" s="12" t="s">
-        <v>448</v>
-      </c>
-      <c r="M74" s="12"/>
-      <c r="N74" s="12"/>
-      <c r="O74" s="12" t="s">
-        <v>498</v>
-      </c>
-      <c r="P74" s="12"/>
-      <c r="Q74" s="12"/>
-    </row>
-    <row r="75" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="J75" s="30" t="s">
-        <v>449</v>
-      </c>
-      <c r="M75" s="12"/>
-      <c r="N75" s="12"/>
-      <c r="O75" s="12" t="s">
-        <v>499</v>
-      </c>
-      <c r="P75" s="12"/>
-      <c r="Q75" s="12"/>
-    </row>
-    <row r="76" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="J76" s="12" t="s">
-        <v>450</v>
-      </c>
-      <c r="M76" s="12"/>
-      <c r="N76" s="12"/>
-      <c r="O76" s="12" t="s">
-        <v>500</v>
-      </c>
-      <c r="P76" s="12"/>
-      <c r="Q76" s="12"/>
-    </row>
-    <row r="77" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="J77" s="12" t="s">
-        <v>451</v>
-      </c>
-      <c r="M77" s="12"/>
-      <c r="N77" s="12"/>
-      <c r="O77" s="12" t="s">
-        <v>501</v>
-      </c>
-      <c r="P77" s="12"/>
-      <c r="Q77" s="12"/>
-    </row>
-    <row r="78" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="J78" s="30" t="s">
-        <v>452</v>
-      </c>
-      <c r="M78" s="12"/>
-      <c r="N78" s="12"/>
-      <c r="O78" s="30" t="s">
-        <v>502</v>
-      </c>
-      <c r="P78" s="12"/>
-      <c r="Q78" s="12"/>
-    </row>
-    <row r="79" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="J79" s="14" t="s">
+      <c r="L81" s="12"/>
+      <c r="N81" s="12"/>
+      <c r="O81" s="12"/>
+      <c r="P81" s="12" t="s">
+        <v>504</v>
+      </c>
+      <c r="Q81" s="14" t="s">
+        <v>557</v>
+      </c>
+      <c r="R81" s="12"/>
+    </row>
+    <row r="82" spans="11:18" x14ac:dyDescent="0.25">
+      <c r="K82" s="14" t="s">
         <v>453</v>
-      </c>
-      <c r="M79" s="12"/>
-      <c r="N79" s="12"/>
-      <c r="O79" s="12" t="s">
-        <v>503</v>
-      </c>
-      <c r="P79" s="12"/>
-      <c r="Q79" s="12"/>
-    </row>
-    <row r="80" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="J80" s="14" t="s">
-        <v>542</v>
-      </c>
-      <c r="M80" s="12"/>
-      <c r="N80" s="12"/>
-      <c r="O80" s="12" t="s">
-        <v>504</v>
-      </c>
-      <c r="P80" s="12"/>
-      <c r="Q80" s="12"/>
-    </row>
-    <row r="81" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="J81" s="14" t="s">
-        <v>454</v>
-      </c>
-      <c r="M81" s="12"/>
-      <c r="N81" s="12"/>
-      <c r="O81" s="12" t="s">
-        <v>505</v>
-      </c>
-      <c r="P81" s="12"/>
-      <c r="Q81" s="12"/>
-    </row>
-    <row r="82" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="J82" s="12" t="s">
-        <v>455</v>
       </c>
       <c r="L82" s="12"/>
       <c r="M82" s="12"/>
       <c r="N82" s="12"/>
       <c r="O82" s="12"/>
-    </row>
-    <row r="83" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="J83" s="12" t="s">
-        <v>456</v>
+      <c r="P82" s="12"/>
+      <c r="Q82" s="14" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="83" spans="11:18" x14ac:dyDescent="0.25">
+      <c r="K83" s="12" t="s">
+        <v>454</v>
       </c>
       <c r="L83" s="12"/>
       <c r="M83" s="12"/>
       <c r="N83" s="12"/>
       <c r="O83" s="12"/>
-    </row>
-    <row r="84" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="J84" s="12" t="s">
-        <v>457</v>
+      <c r="P83" s="12"/>
+      <c r="Q83" s="14" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="84" spans="11:18" x14ac:dyDescent="0.25">
+      <c r="K84" s="12" t="s">
+        <v>455</v>
       </c>
       <c r="L84" s="12"/>
       <c r="M84" s="12"/>
       <c r="N84" s="12"/>
       <c r="O84" s="12"/>
-    </row>
-    <row r="85" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="J85" s="12" t="s">
-        <v>458</v>
+      <c r="P84" s="12"/>
+      <c r="Q84" s="12" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="85" spans="11:18" x14ac:dyDescent="0.25">
+      <c r="K85" s="12" t="s">
+        <v>456</v>
       </c>
       <c r="L85" s="12"/>
       <c r="M85" s="12"/>
       <c r="N85" s="12"/>
       <c r="O85" s="12"/>
-    </row>
-    <row r="86" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="J86" s="12" t="s">
-        <v>459</v>
+      <c r="P85" s="12"/>
+      <c r="Q85" s="14" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="86" spans="11:18" x14ac:dyDescent="0.25">
+      <c r="K86" s="12" t="s">
+        <v>457</v>
       </c>
       <c r="L86" s="12"/>
       <c r="M86" s="12"/>
       <c r="N86" s="12"/>
       <c r="O86" s="12"/>
-    </row>
-    <row r="87" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="J87" s="12" t="s">
-        <v>460</v>
+      <c r="P86" s="12"/>
+      <c r="Q86" s="14" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="87" spans="11:18" x14ac:dyDescent="0.25">
+      <c r="K87" s="12" t="s">
+        <v>458</v>
       </c>
       <c r="L87" s="12"/>
       <c r="M87" s="12"/>
       <c r="N87" s="12"/>
       <c r="O87" s="12"/>
-    </row>
-    <row r="88" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="J88" s="12" t="s">
-        <v>461</v>
+      <c r="P87" s="12"/>
+      <c r="Q87" s="12" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="88" spans="11:18" x14ac:dyDescent="0.25">
+      <c r="K88" s="12" t="s">
+        <v>459</v>
       </c>
       <c r="L88" s="12"/>
       <c r="M88" s="12"/>
       <c r="N88" s="12"/>
       <c r="O88" s="12"/>
-    </row>
-    <row r="89" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="J89" s="12" t="s">
-        <v>462</v>
+      <c r="P88" s="12"/>
+      <c r="Q88" s="12" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="89" spans="11:18" x14ac:dyDescent="0.25">
+      <c r="K89" s="12" t="s">
+        <v>460</v>
       </c>
       <c r="L89" s="12"/>
       <c r="M89" s="12"/>
       <c r="N89" s="12"/>
       <c r="O89" s="12"/>
-    </row>
-    <row r="90" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="J90" s="12" t="s">
-        <v>463</v>
+      <c r="P89" s="12"/>
+      <c r="Q89" s="14" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="90" spans="11:18" x14ac:dyDescent="0.25">
+      <c r="K90" s="12" t="s">
+        <v>461</v>
       </c>
       <c r="L90" s="12"/>
       <c r="M90" s="12"/>
       <c r="N90" s="12"/>
       <c r="O90" s="12"/>
-    </row>
-    <row r="91" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="J91" s="12" t="s">
-        <v>464</v>
+      <c r="P90" s="12"/>
+      <c r="Q90" s="14" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="91" spans="11:18" x14ac:dyDescent="0.25">
+      <c r="K91" s="12" t="s">
+        <v>462</v>
       </c>
       <c r="L91" s="12"/>
       <c r="M91" s="12"/>
       <c r="N91" s="12"/>
       <c r="O91" s="12"/>
-    </row>
-    <row r="92" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="J92" s="30" t="s">
-        <v>465</v>
+      <c r="P91" s="12"/>
+      <c r="Q91" s="14" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="92" spans="11:18" x14ac:dyDescent="0.25">
+      <c r="K92" s="12" t="s">
+        <v>463</v>
       </c>
       <c r="L92" s="12"/>
       <c r="M92" s="12"/>
       <c r="N92" s="12"/>
       <c r="O92" s="12"/>
-    </row>
-    <row r="93" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="J93" s="12" t="s">
-        <v>466</v>
+      <c r="P92" s="12"/>
+      <c r="Q92" s="14" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="93" spans="11:18" x14ac:dyDescent="0.25">
+      <c r="K93" s="28" t="s">
+        <v>464</v>
       </c>
       <c r="L93" s="12"/>
       <c r="M93" s="12"/>
       <c r="N93" s="12"/>
       <c r="O93" s="12"/>
-    </row>
-    <row r="94" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="J94" s="12" t="s">
-        <v>467</v>
+      <c r="P93" s="12"/>
+      <c r="Q93" s="14" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="94" spans="11:18" x14ac:dyDescent="0.25">
+      <c r="K94" s="12" t="s">
+        <v>465</v>
       </c>
       <c r="L94" s="12"/>
       <c r="M94" s="12"/>
       <c r="N94" s="12"/>
       <c r="O94" s="12"/>
-    </row>
-    <row r="95" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="J95" s="30" t="s">
-        <v>468</v>
+      <c r="P94" s="12"/>
+      <c r="Q94" s="12" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="95" spans="11:18" x14ac:dyDescent="0.25">
+      <c r="K95" s="12" t="s">
+        <v>466</v>
       </c>
       <c r="L95" s="12"/>
       <c r="M95" s="12"/>
       <c r="N95" s="12"/>
       <c r="O95" s="12"/>
-    </row>
-    <row r="96" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="J96" s="12" t="s">
-        <v>469</v>
+      <c r="P95" s="12"/>
+    </row>
+    <row r="96" spans="11:18" x14ac:dyDescent="0.25">
+      <c r="K96" s="28" t="s">
+        <v>467</v>
       </c>
       <c r="L96" s="12"/>
       <c r="M96" s="12"/>
       <c r="N96" s="12"/>
       <c r="O96" s="12"/>
-    </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="J97" s="12" t="s">
-        <v>470</v>
+      <c r="P96" s="12"/>
+    </row>
+    <row r="97" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K97" s="12" t="s">
+        <v>468</v>
       </c>
       <c r="L97" s="12"/>
       <c r="M97" s="12"/>
       <c r="N97" s="12"/>
       <c r="O97" s="12"/>
-    </row>
-    <row r="98" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="J98" s="30" t="s">
+      <c r="P97" s="12"/>
+    </row>
+    <row r="98" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K98" s="12" t="s">
+        <v>469</v>
+      </c>
+      <c r="L98" s="12"/>
+    </row>
+    <row r="99" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K99" s="28" t="s">
+        <v>470</v>
+      </c>
+      <c r="L99" s="12"/>
+    </row>
+    <row r="100" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K100" s="12" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="J99" s="12" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="104" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B104" s="12" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="105" spans="1:15" x14ac:dyDescent="0.25">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="105" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A105" s="15" t="s">
         <v>143</v>
       </c>
@@ -6462,403 +6654,352 @@
         <v>361</v>
       </c>
       <c r="C105" s="21" t="s">
-        <v>417</v>
-      </c>
-      <c r="E105" s="13" t="s">
-        <v>546</v>
-      </c>
-      <c r="F105" s="31" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="106" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B106" s="12" t="s">
+        <v>416</v>
+      </c>
+      <c r="E105" s="29"/>
+      <c r="F105" s="29"/>
+    </row>
+    <row r="106" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B106" s="14" t="s">
         <v>41</v>
       </c>
       <c r="C106" s="21" t="s">
+        <v>404</v>
+      </c>
+      <c r="E106" s="29"/>
+      <c r="F106" s="29"/>
+    </row>
+    <row r="107" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B107" s="14" t="s">
+        <v>386</v>
+      </c>
+      <c r="C107" s="21" t="s">
         <v>405</v>
       </c>
-      <c r="E106" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="F106" s="10"/>
-    </row>
-    <row r="107" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B107" s="14" t="s">
-        <v>387</v>
-      </c>
-      <c r="C107" s="21" t="s">
-        <v>406</v>
-      </c>
-      <c r="E107" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="F107" s="10"/>
-    </row>
-    <row r="108" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E107" s="29"/>
+      <c r="F107" s="29"/>
+    </row>
+    <row r="108" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B108" s="14" t="s">
         <v>50</v>
       </c>
       <c r="C108" s="21" t="s">
+        <v>406</v>
+      </c>
+      <c r="E108" s="29"/>
+      <c r="F108" s="29"/>
+    </row>
+    <row r="109" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B109" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="C109" s="21" t="s">
         <v>407</v>
       </c>
-      <c r="E108" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="F108" s="10"/>
-    </row>
-    <row r="109" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B109" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="C109" s="21" t="s">
-        <v>408</v>
-      </c>
-      <c r="E109" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="F109" s="10"/>
-    </row>
-    <row r="110" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E109" s="29"/>
+      <c r="F109" s="29"/>
+    </row>
+    <row r="110" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B110" s="12" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C110" s="21"/>
-      <c r="E110" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="F110" s="10"/>
-    </row>
-    <row r="111" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E110" s="29"/>
+      <c r="F110" s="29"/>
+    </row>
+    <row r="111" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B111" s="14" t="s">
         <v>109</v>
       </c>
       <c r="C111" s="21"/>
-      <c r="E111" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="F111" s="31" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="112" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B112" s="12" t="s">
+      <c r="E111" s="29"/>
+      <c r="F111" s="29"/>
+    </row>
+    <row r="112" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B112" s="14" t="s">
         <v>88</v>
       </c>
       <c r="C112" s="21" t="s">
-        <v>409</v>
-      </c>
-      <c r="E112" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="F112" s="10"/>
+        <v>408</v>
+      </c>
+      <c r="E112" s="29"/>
+      <c r="F112" s="29"/>
     </row>
     <row r="113" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B113" s="12" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C113" s="21"/>
-      <c r="E113" s="32" t="s">
-        <v>44</v>
-      </c>
-      <c r="F113" s="31" t="s">
-        <v>396</v>
-      </c>
+      <c r="E113" s="29"/>
+      <c r="F113" s="29"/>
     </row>
     <row r="114" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B114" s="12" t="s">
+      <c r="B114" s="14" t="s">
         <v>105</v>
       </c>
       <c r="C114" s="21" t="s">
-        <v>410</v>
-      </c>
-      <c r="E114" s="32" t="s">
-        <v>82</v>
-      </c>
-      <c r="F114" s="31" t="s">
-        <v>397</v>
-      </c>
+        <v>409</v>
+      </c>
+      <c r="E114" s="29"/>
+      <c r="F114" s="29"/>
     </row>
     <row r="115" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B115" s="12" t="s">
+      <c r="B115" s="14" t="s">
         <v>77</v>
       </c>
       <c r="C115" s="21" t="s">
-        <v>408</v>
-      </c>
-      <c r="E115" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="F115" s="31" t="s">
-        <v>398</v>
-      </c>
+        <v>407</v>
+      </c>
+      <c r="E115" s="29"/>
+      <c r="F115" s="29"/>
     </row>
     <row r="116" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B116" s="14" t="s">
         <v>10</v>
       </c>
       <c r="C116" s="21" t="s">
-        <v>411</v>
-      </c>
-      <c r="E116" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="F116" s="10"/>
+        <v>410</v>
+      </c>
+      <c r="E116" s="29"/>
+      <c r="F116" s="29"/>
     </row>
     <row r="117" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B117" s="12" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C117" s="21"/>
-      <c r="E117" s="32" t="s">
-        <v>79</v>
-      </c>
-      <c r="F117" s="31" t="s">
-        <v>402</v>
-      </c>
+      <c r="E117" s="29"/>
+      <c r="F117" s="29"/>
     </row>
     <row r="118" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B118" s="12" t="s">
+      <c r="B118" s="14" t="s">
         <v>113</v>
       </c>
       <c r="C118" s="21" t="s">
-        <v>412</v>
-      </c>
-      <c r="E118" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="F118" s="31" t="s">
-        <v>403</v>
-      </c>
+        <v>411</v>
+      </c>
+      <c r="E118" s="29"/>
+      <c r="F118" s="29"/>
     </row>
     <row r="119" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B119" s="14" t="s">
         <v>26</v>
       </c>
       <c r="C119" s="21" t="s">
-        <v>406</v>
-      </c>
-      <c r="E119" s="10"/>
+        <v>405</v>
+      </c>
+      <c r="E119" s="29"/>
+      <c r="F119" s="29"/>
     </row>
     <row r="120" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B120" s="14" t="s">
         <v>47</v>
       </c>
       <c r="C120" s="21" t="s">
-        <v>407</v>
-      </c>
-      <c r="E120" s="13" t="s">
-        <v>97</v>
-      </c>
+        <v>406</v>
+      </c>
+      <c r="E120" s="29"/>
+      <c r="F120" s="29"/>
     </row>
     <row r="121" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B121" s="12" t="s">
+      <c r="B121" s="14" t="s">
         <v>23</v>
       </c>
       <c r="C121" s="21" t="s">
-        <v>406</v>
-      </c>
-      <c r="E121" s="13" t="s">
-        <v>400</v>
-      </c>
+        <v>405</v>
+      </c>
+      <c r="E121" s="29"/>
+      <c r="F121" s="29"/>
     </row>
     <row r="122" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B122" s="14" t="s">
         <v>81</v>
       </c>
       <c r="C122" s="21" t="s">
-        <v>408</v>
-      </c>
-      <c r="E122" s="13" t="s">
-        <v>94</v>
-      </c>
+        <v>407</v>
+      </c>
+      <c r="E122" s="29"/>
+      <c r="F122" s="29"/>
     </row>
     <row r="123" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B123" s="14" t="s">
         <v>69</v>
       </c>
       <c r="C123" s="21" t="s">
-        <v>413</v>
-      </c>
-      <c r="E123" s="13" t="s">
-        <v>42</v>
-      </c>
+        <v>412</v>
+      </c>
+      <c r="E123" s="29"/>
+      <c r="F123" s="29"/>
     </row>
     <row r="124" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B124" s="14" t="s">
         <v>29</v>
       </c>
       <c r="C124" s="21" t="s">
-        <v>406</v>
-      </c>
-      <c r="E124" s="13" t="s">
-        <v>101</v>
-      </c>
+        <v>405</v>
+      </c>
+      <c r="E124" s="29"/>
+      <c r="F124" s="29"/>
     </row>
     <row r="125" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B125" s="12" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C125" s="21"/>
-      <c r="E125" s="13" t="s">
-        <v>95</v>
-      </c>
+      <c r="E125" s="29"/>
+      <c r="F125" s="29"/>
     </row>
     <row r="126" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B126" s="12" t="s">
+      <c r="B126" s="14" t="s">
         <v>44</v>
       </c>
       <c r="C126" s="21" t="s">
+        <v>406</v>
+      </c>
+      <c r="E126" s="29"/>
+      <c r="F126" s="29"/>
+    </row>
+    <row r="127" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B127" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="C127" s="21" t="s">
         <v>407</v>
       </c>
-      <c r="E126" s="13" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="127" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B127" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="C127" s="21" t="s">
-        <v>408</v>
-      </c>
-      <c r="E127" s="13" t="s">
-        <v>98</v>
-      </c>
+      <c r="E127" s="29"/>
+      <c r="F127" s="29"/>
     </row>
     <row r="128" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B128" s="14" t="s">
         <v>100</v>
       </c>
       <c r="C128" s="21" t="s">
-        <v>410</v>
-      </c>
-      <c r="E128" s="32" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="129" spans="2:5" x14ac:dyDescent="0.25">
+        <v>409</v>
+      </c>
+      <c r="E128" s="29"/>
+      <c r="F128" s="29"/>
+    </row>
+    <row r="129" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B129" s="14" t="s">
         <v>53</v>
       </c>
       <c r="C129" s="21" t="s">
-        <v>414</v>
-      </c>
-      <c r="E129" s="13" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="130" spans="2:5" x14ac:dyDescent="0.25">
+        <v>413</v>
+      </c>
+      <c r="E129" s="29"/>
+      <c r="F129" s="29"/>
+    </row>
+    <row r="130" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B130" s="14" t="s">
         <v>76</v>
       </c>
       <c r="C130" s="21" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="131" spans="2:5" x14ac:dyDescent="0.25">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="131" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B131" s="14" t="s">
+        <v>391</v>
+      </c>
+      <c r="C131" s="21" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="132" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B132" s="12" t="s">
         <v>392</v>
       </c>
-      <c r="C131" s="21" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="132" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B132" s="12" t="s">
+      <c r="C132" s="21"/>
+    </row>
+    <row r="133" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B133" s="12" t="s">
         <v>393</v>
       </c>
-      <c r="C132" s="21"/>
-    </row>
-    <row r="133" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B133" s="12" t="s">
+      <c r="C133" s="21"/>
+    </row>
+    <row r="134" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B134" s="12" t="s">
         <v>394</v>
       </c>
-      <c r="C133" s="21"/>
-    </row>
-    <row r="134" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B134" s="12" t="s">
-        <v>395</v>
-      </c>
       <c r="C134" s="21"/>
     </row>
-    <row r="135" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B135" s="12" t="s">
+    <row r="135" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B135" s="14" t="s">
         <v>66</v>
       </c>
       <c r="C135" s="21" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="136" spans="2:5" x14ac:dyDescent="0.25">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="136" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B136" s="14" t="s">
         <v>27</v>
       </c>
       <c r="C136" s="21" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="137" spans="2:5" x14ac:dyDescent="0.25">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="137" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B137" s="12" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C137" s="21"/>
     </row>
-    <row r="138" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B138" s="12" t="s">
+    <row r="138" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B138" s="14" t="s">
         <v>59</v>
       </c>
       <c r="C138" s="21" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="139" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B139" s="12" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="139" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B139" s="14" t="s">
         <v>79</v>
       </c>
       <c r="C139" s="21" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="140" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B140" s="12" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="140" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B140" s="14" t="s">
         <v>103</v>
       </c>
       <c r="C140" s="21" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="141" spans="2:5" x14ac:dyDescent="0.25">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="141" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B141" s="14" t="s">
         <v>108</v>
       </c>
       <c r="C141" s="21" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="142" spans="2:5" x14ac:dyDescent="0.25">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="142" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B142" s="12" t="s">
+        <v>396</v>
+      </c>
+      <c r="C142" s="21"/>
+    </row>
+    <row r="143" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B143" s="12" t="s">
         <v>397</v>
       </c>
-      <c r="C142" s="21"/>
-    </row>
-    <row r="143" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B143" s="12" t="s">
-        <v>398</v>
-      </c>
       <c r="C143" s="21"/>
     </row>
-    <row r="144" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B144" s="12" t="s">
         <v>37</v>
       </c>
       <c r="C144" s="21" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="145" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B145" s="14" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C145" s="21"/>
     </row>
@@ -6867,31 +7008,31 @@
         <v>93</v>
       </c>
       <c r="C146" s="21" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="147" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B147" s="12" t="s">
+      <c r="B147" s="14" t="s">
         <v>97</v>
       </c>
       <c r="C147" s="21" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="148" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B148" s="12" t="s">
-        <v>400</v>
+      <c r="B148" s="14" t="s">
+        <v>399</v>
       </c>
       <c r="C148" s="21" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="149" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B149" s="12" t="s">
+      <c r="B149" s="14" t="s">
         <v>94</v>
       </c>
       <c r="C149" s="21" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="150" spans="2:3" x14ac:dyDescent="0.25">
@@ -6899,29 +7040,29 @@
         <v>36</v>
       </c>
       <c r="C150" s="21" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="151" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B151" s="12" t="s">
+      <c r="B151" s="14" t="s">
         <v>42</v>
       </c>
       <c r="C151" s="21" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="152" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B152" s="12" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C152" s="21"/>
     </row>
     <row r="153" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B153" s="12" t="s">
+      <c r="B153" s="14" t="s">
         <v>101</v>
       </c>
       <c r="C153" s="21" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="154" spans="2:3" x14ac:dyDescent="0.25">
@@ -6929,37 +7070,37 @@
         <v>107</v>
       </c>
       <c r="C154" s="21" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="155" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B155" s="12" t="s">
+      <c r="B155" s="14" t="s">
         <v>95</v>
       </c>
       <c r="C155" s="21" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="156" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B156" s="12" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C156" s="21"/>
     </row>
     <row r="157" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B157" s="12" t="s">
+      <c r="B157" s="14" t="s">
         <v>102</v>
       </c>
       <c r="C157" s="21" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="158" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B158" s="12" t="s">
+      <c r="B158" s="14" t="s">
         <v>98</v>
       </c>
       <c r="C158" s="21" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="159" spans="2:3" x14ac:dyDescent="0.25">
@@ -6967,7 +7108,7 @@
         <v>96</v>
       </c>
       <c r="C159" s="21" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="160" spans="2:3" x14ac:dyDescent="0.25">
@@ -6975,7 +7116,7 @@
         <v>99</v>
       </c>
       <c r="C160" s="21" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="161" spans="2:3" x14ac:dyDescent="0.25">
@@ -6983,26 +7124,26 @@
         <v>46</v>
       </c>
       <c r="C161" s="21" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="162" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B162" s="12" t="s">
+      <c r="B162" s="14" t="s">
         <v>39</v>
       </c>
       <c r="C162" s="21" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="163" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B163" s="12" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C163" s="21"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="J57:J99">
-    <sortCondition ref="J99"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="K57:K99">
+    <sortCondition ref="K99"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
changed to status before 1
</commit_message>
<xml_diff>
--- a/Townes vs Broad.xlsx
+++ b/Townes vs Broad.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robin\Dropbox\Mein PC (Gemeinsamer-PC)\Documents\GitHub\Ichneumonidae\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E30BBDE0-F08E-4E65-8B1E-A95E6AC24958}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBB118FF-C9C9-4C83-B815-A264BF700741}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10080" yWindow="960" windowWidth="15765" windowHeight="14550" activeTab="2" xr2:uid="{63889695-902D-49DB-8829-7F5E2426025F}"/>
+    <workbookView xWindow="1650" yWindow="510" windowWidth="15765" windowHeight="14550" activeTab="2" xr2:uid="{63889695-902D-49DB-8829-7F5E2426025F}"/>
   </bookViews>
   <sheets>
     <sheet name="TOWNES" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="915" uniqueCount="580">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="918" uniqueCount="548">
   <si>
     <t>Epelaspis</t>
   </si>
@@ -1157,6 +1157,9 @@
     <t>Pleolophus</t>
   </si>
   <si>
+    <t>!</t>
+  </si>
+  <si>
     <t>CRYPTINI</t>
   </si>
   <si>
@@ -1673,109 +1676,10 @@
     <t>in Ichneumoninae key als Tribe</t>
   </si>
   <si>
-    <t>ALOMYINI</t>
-  </si>
-  <si>
-    <t>Pseudalomya</t>
-  </si>
-  <si>
-    <t>PROTICHNEUMONINI</t>
-  </si>
-  <si>
-    <t>PROTICHNEUMONINA</t>
-  </si>
-  <si>
-    <t>APATETORINA</t>
-  </si>
-  <si>
-    <t>Apatetor</t>
-  </si>
-  <si>
-    <t>TROGINI</t>
-  </si>
-  <si>
-    <t>CALLAJOPPINA</t>
-  </si>
-  <si>
-    <t>TROGINA</t>
-  </si>
-  <si>
-    <t>Ectopoides</t>
-  </si>
-  <si>
-    <t>Afrectopius</t>
-  </si>
-  <si>
-    <t>Cyclolabellus</t>
-  </si>
-  <si>
-    <t>Neolinycus</t>
-  </si>
-  <si>
-    <t>Carlsonia</t>
-  </si>
-  <si>
-    <t>Notoplatylabus</t>
-  </si>
-  <si>
-    <t>Levansa</t>
-  </si>
-  <si>
-    <t>Cratolaboides</t>
-  </si>
-  <si>
-    <t>Pagarenes</t>
-  </si>
-  <si>
-    <t>Clypeolabus</t>
-  </si>
-  <si>
-    <t>Hirtolabus</t>
-  </si>
-  <si>
-    <t>Rhyssolabus</t>
-  </si>
-  <si>
-    <t>Ambloplisus</t>
-  </si>
-  <si>
-    <t>Acantholabus</t>
-  </si>
-  <si>
-    <t>Platybirmania</t>
-  </si>
-  <si>
-    <t>Neolevansa</t>
-  </si>
-  <si>
-    <t>Lamprojoppa</t>
-  </si>
-  <si>
-    <t>Pachyjoppa</t>
-  </si>
-  <si>
-    <t>Lissolaboides</t>
-  </si>
-  <si>
-    <t>Cratolabus</t>
-  </si>
-  <si>
-    <t>Tropicolabus</t>
-  </si>
-  <si>
-    <t>Spanophatnus</t>
-  </si>
-  <si>
-    <t>Neeurylabia</t>
-  </si>
-  <si>
-    <t>Heinrichiellus</t>
-  </si>
-  <si>
-    <t>Abzaria</t>
-  </si>
-  <si>
-    <t>Pyramidophorus</t>
+    <t>24.03.2020 Townes</t>
+  </si>
+  <si>
+    <t>BOLD SYSTEMS</t>
   </si>
 </sst>
 </file>
@@ -1826,7 +1730,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1883,7 +1787,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1923,18 +1833,18 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -2251,8 +2161,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3325E525-F9CE-447C-9C7C-9E0C969A72AA}">
   <dimension ref="A1:R96"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView topLeftCell="A33" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2313,7 +2223,7 @@
         <v>115</v>
       </c>
       <c r="Q5" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
@@ -2364,481 +2274,481 @@
         <v>0</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="22" t="s">
+      <c r="D7" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="E7" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="F7" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="G7" s="20" t="s">
+      <c r="E7" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="G7" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="H7" s="20" t="s">
+      <c r="H7" s="22" t="s">
         <v>55</v>
       </c>
       <c r="I7" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="J7" s="20" t="s">
+      <c r="J7" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="K7" s="20" t="s">
+      <c r="K7" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="L7" s="20" t="s">
+      <c r="L7" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="M7" s="20" t="s">
+      <c r="M7" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="N7" s="20" t="s">
+      <c r="N7" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="O7" s="20" t="s">
+      <c r="O7" s="22" t="s">
         <v>111</v>
       </c>
-      <c r="R7" s="23"/>
+      <c r="R7" s="24"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C8" s="22" t="s">
+      <c r="C8" s="19" t="s">
         <v>14</v>
       </c>
       <c r="D8" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="F8" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="G8" s="20" t="s">
+      <c r="E8" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="G8" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="H8" s="22" t="s">
+      <c r="H8" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="I8" s="22" t="s">
+      <c r="I8" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="J8" s="22" t="s">
+      <c r="J8" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="K8" s="20" t="s">
+      <c r="K8" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="L8" s="22" t="s">
+      <c r="L8" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="M8" s="20" t="s">
+      <c r="M8" s="12" t="s">
         <v>105</v>
       </c>
       <c r="N8" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="O8" s="22" t="s">
+      <c r="O8" s="19" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C9" s="22" t="s">
+      <c r="C9" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="20" t="s">
+      <c r="D9" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="20" t="s">
+      <c r="E9" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="G9" s="12"/>
+      <c r="H9" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="I9" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="J9" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="K9" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="L9" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="M9" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="N9" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="O9" s="12" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C10" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="F9" s="20" t="s">
+      <c r="F10" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="G9" s="22"/>
-      <c r="H9" s="22" t="s">
-        <v>62</v>
-      </c>
-      <c r="I9" s="20" t="s">
-        <v>69</v>
-      </c>
-      <c r="J9" s="22" t="s">
-        <v>73</v>
-      </c>
-      <c r="K9" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="L9" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="M9" s="20" t="s">
-        <v>100</v>
-      </c>
-      <c r="N9" s="20" t="s">
-        <v>108</v>
-      </c>
-      <c r="O9" s="20" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C10" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="E10" s="22" t="s">
+      <c r="G10" s="12"/>
+      <c r="H10" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="L10" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="M10" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="N10" s="12"/>
+      <c r="O10" s="12"/>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C11" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="F10" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="G10" s="22"/>
-      <c r="H10" s="22" t="s">
-        <v>64</v>
-      </c>
-      <c r="I10" s="22"/>
-      <c r="J10" s="22"/>
-      <c r="K10" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="L10" s="22" t="s">
-        <v>89</v>
-      </c>
-      <c r="M10" s="20" t="s">
-        <v>103</v>
-      </c>
-      <c r="N10" s="22"/>
-      <c r="O10" s="22"/>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C11" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="E11" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="F11" s="20" t="s">
+      <c r="F11" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="G11" s="22"/>
-      <c r="H11" s="22" t="s">
+      <c r="G11" s="12"/>
+      <c r="H11" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="I11" s="22"/>
-      <c r="J11" s="22"/>
-      <c r="K11" s="22" t="s">
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="L11" s="22" t="s">
+      <c r="L11" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="M11" s="20" t="s">
+      <c r="M11" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="N11" s="22"/>
-      <c r="O11" s="22"/>
+      <c r="N11" s="12"/>
+      <c r="O11" s="12"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C12" s="22" t="s">
+      <c r="C12" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="22" t="s">
+      <c r="D12" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="E12" s="20" t="s">
+      <c r="E12" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="F12" s="22" t="s">
+      <c r="F12" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="G12" s="22"/>
-      <c r="H12" s="22" t="s">
+      <c r="G12" s="12"/>
+      <c r="H12" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="I12" s="22"/>
-      <c r="J12" s="22"/>
-      <c r="K12" s="20" t="s">
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="L12" s="22" t="s">
+      <c r="L12" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="M12" s="20" t="s">
+      <c r="M12" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="N12" s="22"/>
-      <c r="O12" s="22"/>
+      <c r="N12" s="12"/>
+      <c r="O12" s="12"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C13" s="20" t="s">
+      <c r="C13" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="D13" s="20" t="s">
+      <c r="D13" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="E13" s="20" t="s">
+      <c r="E13" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="F13" s="20" t="s">
+      <c r="F13" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="G13" s="22"/>
-      <c r="H13" s="22" t="s">
+      <c r="G13" s="12"/>
+      <c r="H13" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="I13" s="22"/>
-      <c r="J13" s="22"/>
-      <c r="K13" s="20" t="s">
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="L13" s="22"/>
-      <c r="M13" s="20" t="s">
+      <c r="L13" s="12"/>
+      <c r="M13" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="N13" s="22"/>
-      <c r="O13" s="22"/>
+      <c r="N13" s="12"/>
+      <c r="O13" s="12"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C14" s="22" t="s">
+      <c r="C14" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="D14" s="22" t="s">
+      <c r="D14" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="E14" s="22"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="20" t="s">
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="I14" s="22"/>
-      <c r="J14" s="22"/>
-      <c r="K14" s="20" t="s">
+      <c r="I14" s="12"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="L14" s="22"/>
-      <c r="M14" s="20" t="s">
+      <c r="L14" s="12"/>
+      <c r="M14" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="N14" s="22"/>
-      <c r="O14" s="22"/>
+      <c r="N14" s="12"/>
+      <c r="O14" s="12"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C15" s="22" t="s">
+      <c r="C15" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="20" t="s">
+      <c r="D15" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="E15" s="22"/>
-      <c r="F15" s="22"/>
-      <c r="G15" s="22"/>
-      <c r="H15" s="20" t="s">
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="I15" s="22"/>
-      <c r="J15" s="22"/>
-      <c r="K15" s="22" t="s">
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="L15" s="22"/>
-      <c r="M15" s="20" t="s">
+      <c r="L15" s="12"/>
+      <c r="M15" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="N15" s="22"/>
-      <c r="O15" s="22"/>
+      <c r="N15" s="12"/>
+      <c r="O15" s="12"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C16" s="22" t="s">
+      <c r="C16" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="D16" s="20" t="s">
+      <c r="D16" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="E16" s="22"/>
-      <c r="F16" s="22"/>
-      <c r="G16" s="22"/>
-      <c r="H16" s="22" t="s">
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="I16" s="22"/>
-      <c r="J16" s="22"/>
-      <c r="K16" s="22"/>
-      <c r="L16" s="22"/>
-      <c r="M16" s="20" t="s">
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="12"/>
+      <c r="M16" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="N16" s="22"/>
-      <c r="O16" s="22"/>
+      <c r="N16" s="12"/>
+      <c r="O16" s="12"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C17" s="22" t="s">
+      <c r="C17" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="D17" s="22" t="s">
+      <c r="D17" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="E17" s="22"/>
-      <c r="F17" s="22"/>
-      <c r="G17" s="22"/>
-      <c r="H17" s="22" t="s">
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
-      <c r="K17" s="22"/>
-      <c r="L17" s="22"/>
-      <c r="M17" s="20" t="s">
+      <c r="I17" s="12"/>
+      <c r="J17" s="12"/>
+      <c r="K17" s="12"/>
+      <c r="L17" s="12"/>
+      <c r="M17" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="N17" s="22"/>
-      <c r="O17" s="22"/>
+      <c r="N17" s="12"/>
+      <c r="O17" s="12"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C18" s="20" t="s">
+      <c r="C18" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="D18" s="20" t="s">
+      <c r="D18" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="E18" s="22"/>
-      <c r="F18" s="22"/>
-      <c r="G18" s="22"/>
-      <c r="H18" s="22" t="s">
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="I18" s="22"/>
-      <c r="J18" s="22"/>
-      <c r="K18" s="22"/>
-      <c r="L18" s="22"/>
-      <c r="M18" s="22" t="s">
+      <c r="I18" s="12"/>
+      <c r="J18" s="12"/>
+      <c r="K18" s="12"/>
+      <c r="L18" s="12"/>
+      <c r="M18" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="N18" s="22"/>
-      <c r="O18" s="22"/>
+      <c r="N18" s="12"/>
+      <c r="O18" s="12"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C19" s="22" t="s">
+      <c r="C19" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="D19" s="22" t="s">
+      <c r="D19" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="E19" s="22"/>
-      <c r="F19" s="22"/>
-      <c r="G19" s="22"/>
-      <c r="H19" s="22"/>
-      <c r="I19" s="22"/>
-      <c r="J19" s="22"/>
-      <c r="K19" s="22"/>
-      <c r="L19" s="22"/>
-      <c r="M19" s="20" t="s">
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="12"/>
+      <c r="K19" s="12"/>
+      <c r="L19" s="12"/>
+      <c r="M19" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="N19" s="22"/>
-      <c r="O19" s="22"/>
+      <c r="N19" s="12"/>
+      <c r="O19" s="12"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C20" s="22" t="s">
+      <c r="C20" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="D20" s="22" t="s">
+      <c r="D20" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="E20" s="22"/>
-      <c r="F20" s="22"/>
-      <c r="G20" s="22"/>
-      <c r="H20" s="22"/>
-      <c r="I20" s="22"/>
-      <c r="J20" s="22"/>
-      <c r="K20" s="22"/>
-      <c r="L20" s="22"/>
-      <c r="M20" s="22"/>
-      <c r="N20" s="22"/>
-      <c r="O20" s="22"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="12"/>
+      <c r="K20" s="12"/>
+      <c r="L20" s="12"/>
+      <c r="M20" s="12"/>
+      <c r="N20" s="12"/>
+      <c r="O20" s="12"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C21" s="22" t="s">
+      <c r="C21" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="D21" s="20" t="s">
+      <c r="D21" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="E21" s="22"/>
-      <c r="F21" s="22"/>
-      <c r="G21" s="22"/>
-      <c r="H21" s="22"/>
-      <c r="I21" s="22"/>
-      <c r="J21" s="22"/>
-      <c r="K21" s="22"/>
-      <c r="L21" s="22"/>
-      <c r="M21" s="22"/>
-      <c r="N21" s="22"/>
-      <c r="O21" s="22"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="12"/>
+      <c r="K21" s="12"/>
+      <c r="L21" s="12"/>
+      <c r="M21" s="12"/>
+      <c r="N21" s="12"/>
+      <c r="O21" s="12"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C22" s="22" t="s">
+      <c r="C22" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="D22" s="22"/>
-      <c r="E22" s="22"/>
-      <c r="F22" s="22"/>
-      <c r="G22" s="22"/>
-      <c r="H22" s="22"/>
-      <c r="I22" s="22"/>
-      <c r="J22" s="22"/>
-      <c r="K22" s="22"/>
-      <c r="L22" s="22"/>
-      <c r="M22" s="22"/>
-      <c r="N22" s="22"/>
-      <c r="O22" s="22"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="12"/>
+      <c r="K22" s="12"/>
+      <c r="L22" s="12"/>
+      <c r="M22" s="12"/>
+      <c r="N22" s="12"/>
+      <c r="O22" s="12"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C23" s="22" t="s">
+      <c r="C23" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="D23" s="22"/>
-      <c r="E23" s="22"/>
-      <c r="F23" s="22"/>
-      <c r="G23" s="30"/>
-      <c r="H23" s="30"/>
-      <c r="I23" s="30"/>
-      <c r="J23" s="30"/>
-      <c r="K23" s="22"/>
-      <c r="L23" s="22"/>
-      <c r="M23" s="22"/>
-      <c r="N23" s="22"/>
-      <c r="O23" s="22"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="25"/>
+      <c r="H23" s="25"/>
+      <c r="I23" s="25"/>
+      <c r="J23" s="25"/>
+      <c r="K23" s="12"/>
+      <c r="L23" s="12"/>
+      <c r="M23" s="12"/>
+      <c r="N23" s="12"/>
+      <c r="O23" s="12"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C24" s="22" t="s">
+      <c r="C24" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="D24" s="22"/>
-      <c r="E24" s="22"/>
-      <c r="F24" s="25"/>
-      <c r="G24" s="25"/>
-      <c r="H24" s="22"/>
-      <c r="I24" s="22"/>
-      <c r="J24" s="22"/>
-      <c r="K24" s="22"/>
-      <c r="L24" s="22"/>
-      <c r="M24" s="22"/>
-      <c r="N24" s="22"/>
-      <c r="O24" s="22"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="12"/>
+      <c r="J24" s="12"/>
+      <c r="K24" s="12"/>
+      <c r="L24" s="12"/>
+      <c r="M24" s="12"/>
+      <c r="N24" s="12"/>
+      <c r="O24" s="12"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="F25" s="4"/>
@@ -2855,7 +2765,7 @@
       <c r="G26" s="4"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B27" s="7" t="s">
+      <c r="B27" s="2" t="s">
         <v>131</v>
       </c>
       <c r="E27" s="4"/>
@@ -2871,7 +2781,7 @@
       <c r="O27" s="4"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B28" s="7" t="s">
+      <c r="B28" s="2" t="s">
         <v>139</v>
       </c>
       <c r="E28" s="4"/>
@@ -2935,7 +2845,7 @@
       <c r="O31" s="4"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B32" s="7" t="s">
+      <c r="B32" s="2" t="s">
         <v>123</v>
       </c>
       <c r="E32" s="4"/>
@@ -2951,8 +2861,11 @@
       <c r="O32" s="4"/>
     </row>
     <row r="33" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B33" s="32" t="s">
+      <c r="B33" s="7" t="s">
         <v>128</v>
+      </c>
+      <c r="C33" t="s">
+        <v>373</v>
       </c>
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
@@ -2983,8 +2896,11 @@
       <c r="O34" s="4"/>
     </row>
     <row r="35" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B35" s="7" t="s">
+      <c r="B35" s="9" t="s">
         <v>119</v>
+      </c>
+      <c r="C35" t="s">
+        <v>373</v>
       </c>
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
@@ -3031,12 +2947,15 @@
       <c r="O37" s="4"/>
     </row>
     <row r="38" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B38" s="7" t="s">
+      <c r="B38" s="9" t="s">
         <v>117</v>
+      </c>
+      <c r="C38" t="s">
+        <v>373</v>
       </c>
       <c r="E38" s="4"/>
       <c r="F38" s="4"/>
-      <c r="G38" s="24"/>
+      <c r="G38" s="26"/>
       <c r="H38" s="4"/>
       <c r="I38" s="4"/>
       <c r="J38" s="4"/>
@@ -3047,12 +2966,15 @@
       <c r="O38" s="4"/>
     </row>
     <row r="39" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B39" s="7" t="s">
+      <c r="B39" s="9" t="s">
         <v>118</v>
+      </c>
+      <c r="C39" t="s">
+        <v>373</v>
       </c>
       <c r="E39" s="4"/>
       <c r="F39" s="4"/>
-      <c r="G39" s="24"/>
+      <c r="G39" s="26"/>
       <c r="H39" s="4"/>
       <c r="I39" s="4"/>
       <c r="J39" s="4"/>
@@ -3063,12 +2985,12 @@
       <c r="O39" s="4"/>
     </row>
     <row r="40" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B40" s="7" t="s">
+      <c r="B40" s="2" t="s">
         <v>136</v>
       </c>
       <c r="E40" s="4"/>
       <c r="F40" s="4"/>
-      <c r="G40" s="24"/>
+      <c r="G40" s="26"/>
       <c r="H40" s="4"/>
       <c r="I40" s="4"/>
       <c r="J40" s="4"/>
@@ -3079,12 +3001,15 @@
       <c r="O40" s="4"/>
     </row>
     <row r="41" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B41" s="7" t="s">
+      <c r="B41" s="9" t="s">
         <v>122</v>
+      </c>
+      <c r="C41" t="s">
+        <v>373</v>
       </c>
       <c r="E41" s="4"/>
       <c r="F41" s="4"/>
-      <c r="G41" s="24"/>
+      <c r="G41" s="26"/>
       <c r="H41" s="4"/>
       <c r="I41" s="4"/>
       <c r="J41" s="4"/>
@@ -3100,7 +3025,7 @@
       </c>
       <c r="E42" s="4"/>
       <c r="F42" s="4"/>
-      <c r="G42" s="24"/>
+      <c r="G42" s="26"/>
       <c r="H42" s="4"/>
       <c r="I42" s="4"/>
       <c r="J42" s="4"/>
@@ -3111,8 +3036,11 @@
       <c r="O42" s="4"/>
     </row>
     <row r="43" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B43" s="7" t="s">
+      <c r="B43" s="9" t="s">
         <v>140</v>
+      </c>
+      <c r="C43" t="s">
+        <v>373</v>
       </c>
       <c r="E43" s="4"/>
       <c r="F43" s="4"/>
@@ -3132,7 +3060,7 @@
       </c>
       <c r="E44" s="4"/>
       <c r="F44" s="4"/>
-      <c r="G44" s="25"/>
+      <c r="G44" s="27"/>
       <c r="H44" s="4"/>
       <c r="I44" s="4"/>
       <c r="J44" s="4"/>
@@ -3143,18 +3071,21 @@
       <c r="O44" s="4"/>
     </row>
     <row r="45" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B45" s="7" t="s">
+      <c r="B45" s="9" t="s">
         <v>120</v>
+      </c>
+      <c r="C45" t="s">
+        <v>373</v>
       </c>
       <c r="F45" s="4"/>
       <c r="G45" s="4"/>
     </row>
     <row r="46" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B46" s="7" t="s">
+      <c r="B46" s="2" t="s">
         <v>132</v>
       </c>
       <c r="F46" s="4"/>
-      <c r="G46" s="24"/>
+      <c r="G46" s="26"/>
     </row>
     <row r="47" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B47" s="7" t="s">
@@ -3164,25 +3095,31 @@
       <c r="G47" s="4"/>
     </row>
     <row r="48" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B48" s="7" t="s">
+      <c r="B48" s="2" t="s">
         <v>130</v>
       </c>
       <c r="F48" s="4"/>
-      <c r="G48" s="24"/>
+      <c r="G48" s="26"/>
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B49" s="32" t="s">
+      <c r="B49" s="9" t="s">
         <v>138</v>
       </c>
+      <c r="C49" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="50" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B50" s="7" t="s">
+      <c r="B50" s="2" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="51" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B51" s="7" t="s">
+      <c r="B51" s="9" t="s">
         <v>121</v>
+      </c>
+      <c r="C51" t="s">
+        <v>373</v>
       </c>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.25">
@@ -3280,7 +3217,7 @@
       <c r="N55" s="9" t="s">
         <v>299</v>
       </c>
-      <c r="O55" s="26" t="s">
+      <c r="O55" s="28" t="s">
         <v>318</v>
       </c>
       <c r="P55" s="2" t="s">
@@ -3297,7 +3234,7 @@
       <c r="D56" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="E56" s="31" t="s">
+      <c r="E56" s="5" t="s">
         <v>212</v>
       </c>
       <c r="F56" s="5" t="s">
@@ -3316,7 +3253,7 @@
       <c r="K56" s="5" t="s">
         <v>293</v>
       </c>
-      <c r="N56" s="24" t="s">
+      <c r="N56" s="26" t="s">
         <v>300</v>
       </c>
       <c r="O56" s="2" t="s">
@@ -3351,7 +3288,7 @@
       <c r="I57" s="5" t="s">
         <v>274</v>
       </c>
-      <c r="N57" s="24" t="s">
+      <c r="N57" s="26" t="s">
         <v>301</v>
       </c>
       <c r="O57" s="5" t="s">
@@ -3412,7 +3349,7 @@
       <c r="I59" s="5" t="s">
         <v>276</v>
       </c>
-      <c r="N59" s="24" t="s">
+      <c r="N59" s="26" t="s">
         <v>303</v>
       </c>
       <c r="O59" s="5" t="s">
@@ -3441,7 +3378,7 @@
       <c r="I60" s="5" t="s">
         <v>277</v>
       </c>
-      <c r="N60" s="24" t="s">
+      <c r="N60" s="26" t="s">
         <v>304</v>
       </c>
       <c r="O60" s="5" t="s">
@@ -3467,10 +3404,10 @@
       <c r="H61" s="5" t="s">
         <v>244</v>
       </c>
-      <c r="I61" s="31" t="s">
+      <c r="I61" s="5" t="s">
         <v>278</v>
       </c>
-      <c r="N61" s="24" t="s">
+      <c r="N61" s="26" t="s">
         <v>305</v>
       </c>
       <c r="O61" s="2" t="s">
@@ -3499,7 +3436,7 @@
       <c r="I62" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="N62" s="24" t="s">
+      <c r="N62" s="26" t="s">
         <v>306</v>
       </c>
       <c r="O62" s="5" t="s">
@@ -3528,7 +3465,7 @@
       <c r="I63" s="5" t="s">
         <v>280</v>
       </c>
-      <c r="N63" s="24" t="s">
+      <c r="N63" s="26" t="s">
         <v>307</v>
       </c>
       <c r="O63" s="9" t="s">
@@ -3557,7 +3494,7 @@
       <c r="I64" s="5" t="s">
         <v>281</v>
       </c>
-      <c r="N64" s="24" t="s">
+      <c r="N64" s="26" t="s">
         <v>308</v>
       </c>
       <c r="P64" s="5" t="s">
@@ -3583,7 +3520,7 @@
       <c r="I65" s="5" t="s">
         <v>282</v>
       </c>
-      <c r="N65" s="24" t="s">
+      <c r="N65" s="26" t="s">
         <v>309</v>
       </c>
       <c r="P65" s="5" t="s">
@@ -3603,7 +3540,7 @@
       <c r="I66" s="5" t="s">
         <v>283</v>
       </c>
-      <c r="N66" s="24" t="s">
+      <c r="N66" s="26" t="s">
         <v>310</v>
       </c>
       <c r="P66" s="5" t="s">
@@ -3623,7 +3560,7 @@
       <c r="I67" s="5" t="s">
         <v>284</v>
       </c>
-      <c r="N67" s="24" t="s">
+      <c r="N67" s="26" t="s">
         <v>311</v>
       </c>
       <c r="P67" s="5" t="s">
@@ -3643,7 +3580,7 @@
       <c r="I68" s="5" t="s">
         <v>285</v>
       </c>
-      <c r="N68" s="24" t="s">
+      <c r="N68" s="26" t="s">
         <v>312</v>
       </c>
       <c r="P68" s="5" t="s">
@@ -3660,7 +3597,7 @@
       <c r="I69" s="5" t="s">
         <v>286</v>
       </c>
-      <c r="N69" s="24" t="s">
+      <c r="N69" s="26" t="s">
         <v>313</v>
       </c>
       <c r="P69" s="5" t="s">
@@ -3677,7 +3614,7 @@
       <c r="I70" s="5" t="s">
         <v>287</v>
       </c>
-      <c r="N70" s="24" t="s">
+      <c r="N70" s="26" t="s">
         <v>314</v>
       </c>
       <c r="P70" s="5" t="s">
@@ -3896,8 +3833,8 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="M8:M19">
-    <sortCondition ref="M7:M19"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="E56:E65">
+    <sortCondition ref="E55:E65"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3921,62 +3858,62 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
@@ -3986,62 +3923,62 @@
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
@@ -4051,7 +3988,7 @@
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
@@ -4066,7 +4003,7 @@
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
@@ -4081,7 +4018,7 @@
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
@@ -4096,7 +4033,7 @@
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
@@ -4116,7 +4053,7 @@
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="8" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
@@ -4156,7 +4093,7 @@
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="8" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
@@ -4186,22 +4123,22 @@
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="8" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="8" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="8" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="8" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
@@ -4216,7 +4153,7 @@
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="8" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
@@ -4241,12 +4178,12 @@
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" s="8" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" s="8" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
@@ -4256,7 +4193,7 @@
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" s="8" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
@@ -4291,7 +4228,7 @@
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" s="8" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
@@ -4311,7 +4248,7 @@
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" s="8" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
@@ -4346,192 +4283,192 @@
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" s="8" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" s="8" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" s="8" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" s="8" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" s="8" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" s="8" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" s="8" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" s="8" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" s="8" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" s="8" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" s="8" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" s="8" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" s="8" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" s="8" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" s="8" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" s="8" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103" s="8" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" s="8" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105" s="8" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" s="8" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" s="8" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108" s="8" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109" s="8" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110" s="8" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111" s="8" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112" s="8" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113" s="8" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114" s="8" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115" s="8" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116" s="8" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117" s="8" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118" s="8" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A119" s="8" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A120" s="8" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A121" s="8" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A122" s="8" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A123" s="8" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A124" s="8" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.25">
@@ -4541,17 +4478,17 @@
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A126" s="8" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A127" s="8" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A128" s="8" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.25">
@@ -4561,7 +4498,7 @@
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A130" s="8" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.25">
@@ -4571,62 +4508,62 @@
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A132" s="8" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A133" s="8" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A134" s="8" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A135" s="8" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A136" s="8" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A137" s="8" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A138" s="8" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A139" s="8" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A140" s="8" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A141" s="8" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A142" s="8" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A143" s="8" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.25">
@@ -4641,7 +4578,7 @@
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A146" s="8" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.25">
@@ -4651,7 +4588,7 @@
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A148" s="8" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.25">
@@ -4661,52 +4598,52 @@
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A150" s="8" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A151" s="8" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A152" s="8" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A153" s="8" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A154" s="8" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A155" s="8" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A156" s="8" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A157" s="8" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A158" s="8" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A159" s="8" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.25">
@@ -4716,22 +4653,22 @@
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A161" s="8" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A162" s="8" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A163" s="8" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A164" s="8" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.25">
@@ -4871,7 +4808,7 @@
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A192" s="8" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.25">
@@ -4901,7 +4838,7 @@
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A198" s="8" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.25">
@@ -4976,7 +4913,7 @@
     </row>
     <row r="213" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A213" s="8" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
     </row>
     <row r="214" spans="1:1" x14ac:dyDescent="0.25">
@@ -5486,17 +5423,25 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EED08F7F-A003-4C3B-8646-FC85C271AAFB}">
-  <dimension ref="A1:T163"/>
+  <dimension ref="A1:Q163"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="S72" sqref="S72"/>
+    <sheetView tabSelected="1" topLeftCell="A110" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" style="15" customWidth="1"/>
-    <col min="2" max="11" width="20.5703125" style="12" customWidth="1"/>
-    <col min="12" max="20" width="20.5703125" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" style="15"/>
+    <col min="2" max="2" width="18.42578125" style="12" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" style="12" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" style="12" customWidth="1"/>
+    <col min="5" max="5" width="20.28515625" style="12" customWidth="1"/>
+    <col min="6" max="6" width="21" style="12" customWidth="1"/>
+    <col min="7" max="7" width="17.140625" style="12" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" style="12"/>
+    <col min="9" max="9" width="15.42578125" style="12" customWidth="1"/>
+    <col min="10" max="10" width="16.140625" style="12" customWidth="1"/>
+    <col min="11" max="11" width="17.140625" style="12" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -5553,21 +5498,21 @@
       <c r="A15" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="B15" s="27" t="s">
+      <c r="B15" s="29" t="s">
         <v>357</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B16" s="11" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B18" s="12" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
@@ -5599,10 +5544,10 @@
         <v>359</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="M25" s="4"/>
       <c r="N25" s="4"/>
@@ -5615,11 +5560,11 @@
         <v>364</v>
       </c>
       <c r="D26" s="17" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="E26" s="18"/>
       <c r="G26" s="8" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="M26" s="4"/>
       <c r="N26" s="10"/>
@@ -5632,7 +5577,7 @@
         <v>324</v>
       </c>
       <c r="E27" s="18" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="G27" s="8"/>
       <c r="M27" s="4"/>
@@ -5646,7 +5591,7 @@
         <v>155</v>
       </c>
       <c r="E28" s="18" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="G28"/>
       <c r="M28" s="4"/>
@@ -5660,7 +5605,7 @@
         <v>152</v>
       </c>
       <c r="E29" s="18" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="M29" s="4"/>
       <c r="N29" s="10"/>
@@ -5673,7 +5618,7 @@
         <v>158</v>
       </c>
       <c r="E30" s="18" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="M30" s="4"/>
       <c r="N30" s="10"/>
@@ -5686,7 +5631,7 @@
         <v>192</v>
       </c>
       <c r="E31" s="18" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="M31" s="4"/>
       <c r="N31" s="10"/>
@@ -5699,7 +5644,7 @@
         <v>189</v>
       </c>
       <c r="E32" s="18" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="M32" s="4"/>
       <c r="N32" s="10"/>
@@ -5709,7 +5654,7 @@
         <v>367</v>
       </c>
       <c r="D33" s="10" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="E33" s="18"/>
       <c r="M33" s="4"/>
@@ -5736,7 +5681,7 @@
         <v>170</v>
       </c>
       <c r="E35" s="18" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="M35" s="4"/>
       <c r="N35" s="10"/>
@@ -5749,7 +5694,7 @@
         <v>157</v>
       </c>
       <c r="E36" s="18" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="M36" s="4"/>
       <c r="N36" s="10"/>
@@ -5762,7 +5707,7 @@
         <v>65</v>
       </c>
       <c r="E37" s="19" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="38" spans="3:14" x14ac:dyDescent="0.25">
@@ -5773,7 +5718,7 @@
         <v>160</v>
       </c>
       <c r="E38" s="18" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
     </row>
     <row r="39" spans="3:14" x14ac:dyDescent="0.25">
@@ -5781,7 +5726,7 @@
         <v>371</v>
       </c>
       <c r="D39" s="10" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="E39" s="18"/>
     </row>
@@ -5793,7 +5738,7 @@
         <v>161</v>
       </c>
       <c r="E40" s="18" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
     </row>
     <row r="41" spans="3:14" x14ac:dyDescent="0.25">
@@ -5804,7 +5749,7 @@
         <v>174</v>
       </c>
       <c r="E41" s="18" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
     </row>
     <row r="42" spans="3:14" x14ac:dyDescent="0.25">
@@ -5815,7 +5760,7 @@
         <v>257</v>
       </c>
       <c r="E42" s="18" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
     </row>
     <row r="43" spans="3:14" x14ac:dyDescent="0.25">
@@ -5826,7 +5771,7 @@
         <v>201</v>
       </c>
       <c r="E43" s="18" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
     </row>
     <row r="44" spans="3:14" x14ac:dyDescent="0.25">
@@ -5837,7 +5782,7 @@
         <v>226</v>
       </c>
       <c r="E44" s="18" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
     </row>
     <row r="45" spans="3:14" x14ac:dyDescent="0.25">
@@ -5845,15 +5790,15 @@
         <v>323</v>
       </c>
       <c r="E45" s="18" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
     </row>
     <row r="46" spans="3:14" x14ac:dyDescent="0.25">
       <c r="D46" s="11" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="E46" s="18" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
     </row>
     <row r="47" spans="3:14" x14ac:dyDescent="0.25">
@@ -5861,7 +5806,7 @@
         <v>354</v>
       </c>
       <c r="E47" s="18" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
     </row>
     <row r="48" spans="3:14" x14ac:dyDescent="0.25">
@@ -5869,26 +5814,26 @@
         <v>153</v>
       </c>
       <c r="E48" s="18" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D49" s="12" t="s">
         <v>162</v>
       </c>
       <c r="E49" s="18" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D50" s="12" t="s">
         <v>194</v>
       </c>
       <c r="E50" s="18" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A55" s="15" t="s">
         <v>143</v>
       </c>
@@ -5896,757 +5841,620 @@
         <v>360</v>
       </c>
     </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B56" s="15" t="s">
         <v>114</v>
       </c>
       <c r="C56" s="12" t="s">
-        <v>545</v>
+        <v>534</v>
       </c>
       <c r="D56" s="12" t="s">
         <v>533</v>
       </c>
       <c r="E56" s="12" t="s">
-        <v>532</v>
+        <v>536</v>
       </c>
       <c r="F56" s="12" t="s">
-        <v>535</v>
+        <v>538</v>
       </c>
       <c r="G56" s="12" t="s">
-        <v>537</v>
+        <v>418</v>
       </c>
       <c r="H56" s="12" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
       <c r="I56" s="12" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="J56" s="12" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="K56" s="12" t="s">
-        <v>421</v>
+        <v>530</v>
       </c>
       <c r="L56" s="12" t="s">
-        <v>529</v>
+        <v>540</v>
       </c>
       <c r="M56" s="12" t="s">
-        <v>539</v>
+        <v>423</v>
       </c>
       <c r="N56" s="12" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
       <c r="O56" s="12" t="s">
-        <v>423</v>
+        <v>480</v>
       </c>
       <c r="P56" s="12" t="s">
-        <v>479</v>
+        <v>506</v>
       </c>
       <c r="Q56" s="12" t="s">
-        <v>505</v>
-      </c>
-      <c r="R56" s="12" t="s">
-        <v>547</v>
-      </c>
-      <c r="S56" s="12" t="s">
-        <v>551</v>
-      </c>
-      <c r="T56" s="12" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B57" s="15"/>
       <c r="C57" s="14" t="s">
-        <v>546</v>
+        <v>535</v>
       </c>
       <c r="D57" s="14" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="E57" s="14" t="s">
+        <v>537</v>
+      </c>
+      <c r="F57" s="14" t="s">
+        <v>539</v>
+      </c>
+      <c r="G57" s="14" t="s">
+        <v>419</v>
+      </c>
+      <c r="H57" s="14" t="s">
+        <v>425</v>
+      </c>
+      <c r="I57" s="12" t="s">
+        <v>526</v>
+      </c>
+      <c r="J57" s="30" t="s">
+        <v>473</v>
+      </c>
+      <c r="K57" s="14" t="s">
         <v>531</v>
       </c>
-      <c r="F57" s="14" t="s">
-        <v>536</v>
-      </c>
-      <c r="G57" s="14" t="s">
-        <v>538</v>
-      </c>
-      <c r="H57" s="14" t="s">
-        <v>418</v>
-      </c>
-      <c r="I57" s="14" t="s">
-        <v>424</v>
-      </c>
-      <c r="J57" s="12" t="s">
-        <v>525</v>
-      </c>
-      <c r="K57" s="28" t="s">
-        <v>472</v>
-      </c>
       <c r="L57" s="14" t="s">
-        <v>530</v>
-      </c>
-      <c r="M57" s="14" t="s">
-        <v>540</v>
+        <v>541</v>
+      </c>
+      <c r="M57" s="12" t="s">
+        <v>476</v>
       </c>
       <c r="N57" s="12" t="s">
+        <v>479</v>
+      </c>
+      <c r="O57" s="30" t="s">
+        <v>481</v>
+      </c>
+      <c r="P57" s="12" t="s">
+        <v>507</v>
+      </c>
+      <c r="Q57" s="14" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B58" s="15"/>
+      <c r="I58" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="J58" s="12" t="s">
+        <v>474</v>
+      </c>
+      <c r="M58" s="14" t="s">
+        <v>477</v>
+      </c>
+      <c r="N58" s="14" t="s">
+        <v>543</v>
+      </c>
+      <c r="O58" s="12" t="s">
+        <v>482</v>
+      </c>
+      <c r="P58" s="12" t="s">
+        <v>508</v>
+      </c>
+      <c r="Q58" s="12"/>
+    </row>
+    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B59" s="15"/>
+      <c r="I59" s="12" t="s">
+        <v>427</v>
+      </c>
+      <c r="J59" s="14" t="s">
+        <v>544</v>
+      </c>
+      <c r="M59" s="12" t="s">
+        <v>478</v>
+      </c>
+      <c r="N59" s="12"/>
+      <c r="O59" s="30" t="s">
+        <v>483</v>
+      </c>
+      <c r="P59" s="12" t="s">
+        <v>509</v>
+      </c>
+      <c r="Q59" s="12"/>
+    </row>
+    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B60" s="15"/>
+      <c r="I60" s="12" t="s">
+        <v>428</v>
+      </c>
+      <c r="J60" s="14" t="s">
         <v>475</v>
       </c>
-      <c r="O57" s="12" t="s">
-        <v>478</v>
-      </c>
-      <c r="P57" s="28" t="s">
-        <v>480</v>
-      </c>
-      <c r="Q57" s="2" t="s">
-        <v>578</v>
-      </c>
-      <c r="R57" s="12" t="s">
-        <v>548</v>
-      </c>
-      <c r="S57" s="12" t="s">
-        <v>552</v>
-      </c>
-      <c r="T57" s="14" t="s">
-        <v>519</v>
-      </c>
-    </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B58" s="15"/>
-      <c r="J58" s="12" t="s">
-        <v>426</v>
-      </c>
-      <c r="K58" s="12" t="s">
-        <v>473</v>
-      </c>
-      <c r="L58" s="12"/>
-      <c r="N58" s="14" t="s">
-        <v>476</v>
-      </c>
-      <c r="O58" s="14" t="s">
+      <c r="M60" s="12"/>
+      <c r="N60" s="12"/>
+      <c r="O60" s="12" t="s">
+        <v>484</v>
+      </c>
+      <c r="P60" s="12" t="s">
+        <v>510</v>
+      </c>
+      <c r="Q60" s="12"/>
+    </row>
+    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B61" s="15"/>
+      <c r="I61" s="30" t="s">
+        <v>429</v>
+      </c>
+      <c r="J61" s="12" t="s">
+        <v>435</v>
+      </c>
+      <c r="M61" s="12"/>
+      <c r="N61" s="12"/>
+      <c r="O61" s="12" t="s">
+        <v>485</v>
+      </c>
+      <c r="P61" s="12" t="s">
+        <v>511</v>
+      </c>
+      <c r="Q61" s="12"/>
+    </row>
+    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B62" s="15"/>
+      <c r="I62" s="12" t="s">
+        <v>430</v>
+      </c>
+      <c r="J62" s="30" t="s">
+        <v>436</v>
+      </c>
+      <c r="M62" s="12"/>
+      <c r="N62" s="12"/>
+      <c r="O62" s="30" t="s">
+        <v>486</v>
+      </c>
+      <c r="P62" s="12" t="s">
+        <v>512</v>
+      </c>
+      <c r="Q62" s="12"/>
+    </row>
+    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B63" s="15"/>
+      <c r="I63" s="12" t="s">
+        <v>431</v>
+      </c>
+      <c r="J63" s="12" t="s">
+        <v>437</v>
+      </c>
+      <c r="M63" s="12"/>
+      <c r="N63" s="12"/>
+      <c r="O63" s="12" t="s">
+        <v>487</v>
+      </c>
+      <c r="P63" s="12" t="s">
+        <v>513</v>
+      </c>
+      <c r="Q63" s="12"/>
+    </row>
+    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B64" s="15"/>
+      <c r="I64" s="12" t="s">
+        <v>432</v>
+      </c>
+      <c r="J64" s="12" t="s">
+        <v>438</v>
+      </c>
+      <c r="M64" s="12"/>
+      <c r="N64" s="12"/>
+      <c r="O64" s="12" t="s">
+        <v>488</v>
+      </c>
+      <c r="P64" s="14" t="s">
+        <v>514</v>
+      </c>
+      <c r="Q64" s="12"/>
+    </row>
+    <row r="65" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B65" s="15"/>
+      <c r="I65" s="12" t="s">
+        <v>433</v>
+      </c>
+      <c r="J65" s="14" t="s">
+        <v>439</v>
+      </c>
+      <c r="M65" s="12"/>
+      <c r="N65" s="12"/>
+      <c r="O65" s="12" t="s">
+        <v>489</v>
+      </c>
+      <c r="P65" s="12" t="s">
+        <v>515</v>
+      </c>
+      <c r="Q65" s="12"/>
+    </row>
+    <row r="66" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B66" s="15"/>
+      <c r="I66" s="12" t="s">
+        <v>434</v>
+      </c>
+      <c r="J66" s="12" t="s">
+        <v>440</v>
+      </c>
+      <c r="M66" s="12"/>
+      <c r="N66" s="12"/>
+      <c r="O66" s="12" t="s">
+        <v>490</v>
+      </c>
+      <c r="P66" s="12" t="s">
+        <v>516</v>
+      </c>
+      <c r="Q66" s="12"/>
+    </row>
+    <row r="67" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B67" s="15"/>
+      <c r="J67" s="12" t="s">
+        <v>441</v>
+      </c>
+      <c r="M67" s="12"/>
+      <c r="N67" s="12"/>
+      <c r="O67" s="12" t="s">
+        <v>491</v>
+      </c>
+      <c r="P67" s="12" t="s">
+        <v>517</v>
+      </c>
+      <c r="Q67" s="12"/>
+    </row>
+    <row r="68" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B68" s="15"/>
+      <c r="J68" s="12" t="s">
+        <v>442</v>
+      </c>
+      <c r="M68" s="12"/>
+      <c r="N68" s="12"/>
+      <c r="O68" s="12" t="s">
+        <v>492</v>
+      </c>
+      <c r="P68" s="12" t="s">
+        <v>518</v>
+      </c>
+      <c r="Q68" s="12"/>
+    </row>
+    <row r="69" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B69" s="15"/>
+      <c r="J69" s="12" t="s">
+        <v>443</v>
+      </c>
+      <c r="M69" s="12"/>
+      <c r="N69" s="12"/>
+      <c r="O69" s="12" t="s">
+        <v>493</v>
+      </c>
+      <c r="P69" s="12"/>
+      <c r="Q69" s="12"/>
+    </row>
+    <row r="70" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B70" s="15"/>
+      <c r="J70" s="12" t="s">
+        <v>444</v>
+      </c>
+      <c r="M70" s="12"/>
+      <c r="N70" s="12"/>
+      <c r="O70" s="12" t="s">
+        <v>494</v>
+      </c>
+      <c r="P70" s="12"/>
+      <c r="Q70" s="12"/>
+    </row>
+    <row r="71" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="J71" s="12" t="s">
+        <v>445</v>
+      </c>
+      <c r="M71" s="12"/>
+      <c r="N71" s="12"/>
+      <c r="O71" s="12" t="s">
+        <v>495</v>
+      </c>
+      <c r="P71" s="12"/>
+      <c r="Q71" s="12"/>
+    </row>
+    <row r="72" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="J72" s="12" t="s">
+        <v>446</v>
+      </c>
+      <c r="M72" s="12"/>
+      <c r="N72" s="12"/>
+      <c r="O72" s="12" t="s">
+        <v>496</v>
+      </c>
+      <c r="P72" s="12"/>
+      <c r="Q72" s="12"/>
+    </row>
+    <row r="73" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="J73" s="30" t="s">
+        <v>447</v>
+      </c>
+      <c r="M73" s="12"/>
+      <c r="N73" s="12"/>
+      <c r="O73" s="12" t="s">
+        <v>497</v>
+      </c>
+      <c r="P73" s="12"/>
+      <c r="Q73" s="12"/>
+    </row>
+    <row r="74" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="J74" s="12" t="s">
+        <v>448</v>
+      </c>
+      <c r="M74" s="12"/>
+      <c r="N74" s="12"/>
+      <c r="O74" s="12" t="s">
+        <v>498</v>
+      </c>
+      <c r="P74" s="12"/>
+      <c r="Q74" s="12"/>
+    </row>
+    <row r="75" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="J75" s="30" t="s">
+        <v>449</v>
+      </c>
+      <c r="M75" s="12"/>
+      <c r="N75" s="12"/>
+      <c r="O75" s="12" t="s">
+        <v>499</v>
+      </c>
+      <c r="P75" s="12"/>
+      <c r="Q75" s="12"/>
+    </row>
+    <row r="76" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="J76" s="12" t="s">
+        <v>450</v>
+      </c>
+      <c r="M76" s="12"/>
+      <c r="N76" s="12"/>
+      <c r="O76" s="12" t="s">
+        <v>500</v>
+      </c>
+      <c r="P76" s="12"/>
+      <c r="Q76" s="12"/>
+    </row>
+    <row r="77" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="J77" s="12" t="s">
+        <v>451</v>
+      </c>
+      <c r="M77" s="12"/>
+      <c r="N77" s="12"/>
+      <c r="O77" s="12" t="s">
+        <v>501</v>
+      </c>
+      <c r="P77" s="12"/>
+      <c r="Q77" s="12"/>
+    </row>
+    <row r="78" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="J78" s="30" t="s">
+        <v>452</v>
+      </c>
+      <c r="M78" s="12"/>
+      <c r="N78" s="12"/>
+      <c r="O78" s="30" t="s">
+        <v>502</v>
+      </c>
+      <c r="P78" s="12"/>
+      <c r="Q78" s="12"/>
+    </row>
+    <row r="79" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="J79" s="14" t="s">
+        <v>453</v>
+      </c>
+      <c r="M79" s="12"/>
+      <c r="N79" s="12"/>
+      <c r="O79" s="12" t="s">
+        <v>503</v>
+      </c>
+      <c r="P79" s="12"/>
+      <c r="Q79" s="12"/>
+    </row>
+    <row r="80" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="J80" s="14" t="s">
         <v>542</v>
       </c>
-      <c r="P58" s="12" t="s">
-        <v>481</v>
-      </c>
-      <c r="Q58" s="2" t="s">
-        <v>567</v>
-      </c>
-      <c r="R58" s="14" t="s">
-        <v>430</v>
-      </c>
-      <c r="S58" s="14" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B59" s="15"/>
-      <c r="J59" s="12" t="s">
-        <v>427</v>
-      </c>
-      <c r="K59" s="14" t="s">
-        <v>543</v>
-      </c>
-      <c r="L59" s="12"/>
-      <c r="N59" s="12" t="s">
-        <v>477</v>
-      </c>
-      <c r="O59" s="12"/>
-      <c r="P59" s="28" t="s">
-        <v>482</v>
-      </c>
-      <c r="Q59" s="2" t="s">
-        <v>555</v>
-      </c>
-      <c r="R59" s="12" t="s">
-        <v>549</v>
-      </c>
-      <c r="S59" s="12" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B60" s="15"/>
-      <c r="J60" s="14" t="s">
-        <v>428</v>
-      </c>
-      <c r="K60" s="14" t="s">
-        <v>474</v>
-      </c>
-      <c r="L60" s="12"/>
-      <c r="N60" s="12"/>
-      <c r="O60" s="12"/>
-      <c r="P60" s="12" t="s">
-        <v>483</v>
-      </c>
-      <c r="Q60" s="2" t="s">
-        <v>566</v>
-      </c>
-      <c r="R60" s="14" t="s">
-        <v>550</v>
-      </c>
-      <c r="S60" s="14" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B61" s="15"/>
-      <c r="J61" s="12" t="s">
-        <v>429</v>
-      </c>
-      <c r="K61" s="12" t="s">
-        <v>434</v>
-      </c>
-      <c r="L61" s="12"/>
-      <c r="N61" s="12"/>
-      <c r="O61" s="12"/>
-      <c r="P61" s="12" t="s">
-        <v>484</v>
-      </c>
-      <c r="Q61" s="14" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B62" s="15"/>
-      <c r="J62" s="14" t="s">
-        <v>430</v>
-      </c>
-      <c r="K62" s="28" t="s">
-        <v>435</v>
-      </c>
-      <c r="L62" s="12"/>
-      <c r="N62" s="12"/>
-      <c r="O62" s="12"/>
-      <c r="P62" s="28" t="s">
-        <v>485</v>
-      </c>
-      <c r="Q62" s="14" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B63" s="15"/>
-      <c r="J63" s="12" t="s">
-        <v>431</v>
-      </c>
-      <c r="K63" s="12" t="s">
-        <v>436</v>
-      </c>
-      <c r="L63" s="12"/>
-      <c r="N63" s="12"/>
-      <c r="O63" s="12"/>
-      <c r="P63" s="12" t="s">
-        <v>486</v>
-      </c>
-      <c r="Q63" s="14" t="s">
-        <v>558</v>
-      </c>
-      <c r="R63" s="12"/>
-    </row>
-    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B64" s="15"/>
-      <c r="J64" s="12" t="s">
-        <v>432</v>
-      </c>
-      <c r="K64" s="12" t="s">
-        <v>437</v>
-      </c>
-      <c r="L64" s="12"/>
-      <c r="N64" s="12"/>
-      <c r="O64" s="12"/>
-      <c r="P64" s="12" t="s">
-        <v>487</v>
-      </c>
-      <c r="Q64" s="14" t="s">
-        <v>563</v>
-      </c>
-      <c r="R64" s="12"/>
-    </row>
-    <row r="65" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B65" s="15"/>
-      <c r="K65" s="14" t="s">
-        <v>438</v>
-      </c>
-      <c r="L65" s="12"/>
-      <c r="N65" s="12"/>
-      <c r="O65" s="12"/>
-      <c r="P65" s="12" t="s">
-        <v>488</v>
-      </c>
-      <c r="Q65" s="14" t="s">
-        <v>561</v>
-      </c>
-      <c r="R65" s="12"/>
-    </row>
-    <row r="66" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B66" s="15"/>
-      <c r="K66" s="12" t="s">
-        <v>439</v>
-      </c>
-      <c r="L66" s="12"/>
-      <c r="N66" s="12"/>
-      <c r="O66" s="12"/>
-      <c r="P66" s="12" t="s">
-        <v>489</v>
-      </c>
-      <c r="Q66" s="14" t="s">
-        <v>573</v>
-      </c>
-      <c r="R66" s="12"/>
-    </row>
-    <row r="67" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B67" s="15"/>
-      <c r="K67" s="12" t="s">
-        <v>440</v>
-      </c>
-      <c r="L67" s="12"/>
-      <c r="N67" s="12"/>
-      <c r="O67" s="12"/>
-      <c r="P67" s="12" t="s">
-        <v>490</v>
-      </c>
-      <c r="Q67" s="14" t="s">
-        <v>508</v>
-      </c>
-      <c r="R67" s="12"/>
-    </row>
-    <row r="68" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B68" s="15"/>
-      <c r="K68" s="12" t="s">
-        <v>441</v>
-      </c>
-      <c r="L68" s="12"/>
-      <c r="N68" s="12"/>
-      <c r="O68" s="12"/>
-      <c r="P68" s="12" t="s">
-        <v>491</v>
-      </c>
-      <c r="Q68" s="14" t="s">
-        <v>556</v>
-      </c>
-      <c r="R68" s="12"/>
-    </row>
-    <row r="69" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B69" s="15"/>
-      <c r="K69" s="12" t="s">
-        <v>442</v>
-      </c>
-      <c r="L69" s="12"/>
-      <c r="N69" s="12"/>
-      <c r="O69" s="12"/>
-      <c r="P69" s="12" t="s">
-        <v>492</v>
-      </c>
-      <c r="Q69" s="14" t="s">
-        <v>509</v>
-      </c>
-      <c r="R69" s="12"/>
-    </row>
-    <row r="70" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B70" s="15"/>
-      <c r="K70" s="12" t="s">
-        <v>443</v>
-      </c>
-      <c r="L70" s="12"/>
-      <c r="N70" s="12"/>
-      <c r="O70" s="12"/>
-      <c r="P70" s="12" t="s">
-        <v>493</v>
-      </c>
-      <c r="Q70" s="14" t="s">
-        <v>554</v>
-      </c>
-      <c r="R70" s="12"/>
-    </row>
-    <row r="71" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="K71" s="12" t="s">
-        <v>444</v>
-      </c>
-      <c r="L71" s="12"/>
-      <c r="N71" s="12"/>
-      <c r="O71" s="12"/>
-      <c r="P71" s="12" t="s">
-        <v>494</v>
-      </c>
-      <c r="Q71" s="14" t="s">
-        <v>510</v>
-      </c>
-      <c r="R71" s="12"/>
-    </row>
-    <row r="72" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="K72" s="12" t="s">
-        <v>445</v>
-      </c>
-      <c r="L72" s="12"/>
-      <c r="N72" s="12"/>
-      <c r="O72" s="12"/>
-      <c r="P72" s="12" t="s">
-        <v>495</v>
-      </c>
-      <c r="Q72" s="14" t="s">
-        <v>577</v>
-      </c>
-      <c r="R72" s="12"/>
-    </row>
-    <row r="73" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="K73" s="28" t="s">
-        <v>446</v>
-      </c>
-      <c r="L73" s="12"/>
-      <c r="N73" s="12"/>
-      <c r="O73" s="12"/>
-      <c r="P73" s="12" t="s">
-        <v>496</v>
-      </c>
-      <c r="Q73" s="14" t="s">
-        <v>564</v>
-      </c>
-      <c r="R73" s="12"/>
-    </row>
-    <row r="74" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="K74" s="12" t="s">
-        <v>447</v>
-      </c>
-      <c r="L74" s="12"/>
-      <c r="N74" s="12"/>
-      <c r="O74" s="12"/>
-      <c r="P74" s="12" t="s">
-        <v>497</v>
-      </c>
-      <c r="Q74" s="14" t="s">
-        <v>511</v>
-      </c>
-      <c r="R74" s="12"/>
-    </row>
-    <row r="75" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="K75" s="28" t="s">
-        <v>448</v>
-      </c>
-      <c r="L75" s="12"/>
-      <c r="N75" s="12"/>
-      <c r="O75" s="12"/>
-      <c r="P75" s="12" t="s">
-        <v>498</v>
-      </c>
-      <c r="Q75" s="14" t="s">
-        <v>570</v>
-      </c>
-      <c r="R75" s="12"/>
-    </row>
-    <row r="76" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="K76" s="12" t="s">
-        <v>449</v>
-      </c>
-      <c r="L76" s="12"/>
-      <c r="N76" s="12"/>
-      <c r="O76" s="12"/>
-      <c r="P76" s="12" t="s">
-        <v>499</v>
-      </c>
-      <c r="Q76" s="14" t="s">
-        <v>560</v>
-      </c>
-      <c r="R76" s="12"/>
-    </row>
-    <row r="77" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="K77" s="12" t="s">
-        <v>450</v>
-      </c>
-      <c r="L77" s="12"/>
-      <c r="N77" s="12"/>
-      <c r="O77" s="12"/>
-      <c r="P77" s="12" t="s">
-        <v>500</v>
-      </c>
-      <c r="Q77" s="33" t="s">
-        <v>512</v>
-      </c>
-      <c r="R77" s="12"/>
-    </row>
-    <row r="78" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="K78" s="14" t="s">
-        <v>428</v>
-      </c>
-      <c r="L78" s="12"/>
-      <c r="N78" s="12"/>
-      <c r="O78" s="12"/>
-      <c r="P78" s="28" t="s">
-        <v>501</v>
-      </c>
-      <c r="Q78" s="14" t="s">
-        <v>572</v>
-      </c>
-      <c r="R78" s="12"/>
-    </row>
-    <row r="79" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="K79" s="28" t="s">
-        <v>451</v>
-      </c>
-      <c r="L79" s="12"/>
-      <c r="N79" s="12"/>
-      <c r="O79" s="12"/>
-      <c r="P79" s="12" t="s">
-        <v>502</v>
-      </c>
-      <c r="Q79" s="14" t="s">
-        <v>576</v>
-      </c>
-      <c r="R79" s="12"/>
-    </row>
-    <row r="80" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="K80" s="14" t="s">
-        <v>452</v>
-      </c>
-      <c r="L80" s="12"/>
+      <c r="M80" s="12"/>
       <c r="N80" s="12"/>
-      <c r="O80" s="12"/>
-      <c r="P80" s="12" t="s">
-        <v>503</v>
-      </c>
-      <c r="Q80" s="14" t="s">
-        <v>569</v>
-      </c>
-      <c r="R80" s="12"/>
-    </row>
-    <row r="81" spans="11:18" x14ac:dyDescent="0.25">
-      <c r="K81" s="14" t="s">
-        <v>541</v>
-      </c>
-      <c r="L81" s="12"/>
+      <c r="O80" s="12" t="s">
+        <v>504</v>
+      </c>
+      <c r="P80" s="12"/>
+      <c r="Q80" s="12"/>
+    </row>
+    <row r="81" spans="10:17" x14ac:dyDescent="0.25">
+      <c r="J81" s="14" t="s">
+        <v>454</v>
+      </c>
+      <c r="M81" s="12"/>
       <c r="N81" s="12"/>
-      <c r="O81" s="12"/>
-      <c r="P81" s="12" t="s">
-        <v>504</v>
-      </c>
-      <c r="Q81" s="14" t="s">
-        <v>557</v>
-      </c>
-      <c r="R81" s="12"/>
-    </row>
-    <row r="82" spans="11:18" x14ac:dyDescent="0.25">
-      <c r="K82" s="14" t="s">
-        <v>453</v>
+      <c r="O81" s="12" t="s">
+        <v>505</v>
+      </c>
+      <c r="P81" s="12"/>
+      <c r="Q81" s="12"/>
+    </row>
+    <row r="82" spans="10:17" x14ac:dyDescent="0.25">
+      <c r="J82" s="12" t="s">
+        <v>455</v>
       </c>
       <c r="L82" s="12"/>
       <c r="M82" s="12"/>
       <c r="N82" s="12"/>
       <c r="O82" s="12"/>
-      <c r="P82" s="12"/>
-      <c r="Q82" s="14" t="s">
-        <v>559</v>
-      </c>
-    </row>
-    <row r="83" spans="11:18" x14ac:dyDescent="0.25">
-      <c r="K83" s="12" t="s">
-        <v>454</v>
+    </row>
+    <row r="83" spans="10:17" x14ac:dyDescent="0.25">
+      <c r="J83" s="12" t="s">
+        <v>456</v>
       </c>
       <c r="L83" s="12"/>
       <c r="M83" s="12"/>
       <c r="N83" s="12"/>
       <c r="O83" s="12"/>
-      <c r="P83" s="12"/>
-      <c r="Q83" s="14" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="84" spans="11:18" x14ac:dyDescent="0.25">
-      <c r="K84" s="12" t="s">
-        <v>455</v>
+    </row>
+    <row r="84" spans="10:17" x14ac:dyDescent="0.25">
+      <c r="J84" s="12" t="s">
+        <v>457</v>
       </c>
       <c r="L84" s="12"/>
       <c r="M84" s="12"/>
       <c r="N84" s="12"/>
       <c r="O84" s="12"/>
-      <c r="P84" s="12"/>
-      <c r="Q84" s="12" t="s">
-        <v>562</v>
-      </c>
-    </row>
-    <row r="85" spans="11:18" x14ac:dyDescent="0.25">
-      <c r="K85" s="12" t="s">
-        <v>456</v>
+    </row>
+    <row r="85" spans="10:17" x14ac:dyDescent="0.25">
+      <c r="J85" s="12" t="s">
+        <v>458</v>
       </c>
       <c r="L85" s="12"/>
       <c r="M85" s="12"/>
       <c r="N85" s="12"/>
       <c r="O85" s="12"/>
-      <c r="P85" s="12"/>
-      <c r="Q85" s="14" t="s">
-        <v>568</v>
-      </c>
-    </row>
-    <row r="86" spans="11:18" x14ac:dyDescent="0.25">
-      <c r="K86" s="12" t="s">
-        <v>457</v>
+    </row>
+    <row r="86" spans="10:17" x14ac:dyDescent="0.25">
+      <c r="J86" s="12" t="s">
+        <v>459</v>
       </c>
       <c r="L86" s="12"/>
       <c r="M86" s="12"/>
       <c r="N86" s="12"/>
       <c r="O86" s="12"/>
-      <c r="P86" s="12"/>
-      <c r="Q86" s="14" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="87" spans="11:18" x14ac:dyDescent="0.25">
-      <c r="K87" s="12" t="s">
-        <v>458</v>
+    </row>
+    <row r="87" spans="10:17" x14ac:dyDescent="0.25">
+      <c r="J87" s="12" t="s">
+        <v>460</v>
       </c>
       <c r="L87" s="12"/>
       <c r="M87" s="12"/>
       <c r="N87" s="12"/>
       <c r="O87" s="12"/>
-      <c r="P87" s="12"/>
-      <c r="Q87" s="12" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="88" spans="11:18" x14ac:dyDescent="0.25">
-      <c r="K88" s="12" t="s">
-        <v>459</v>
+    </row>
+    <row r="88" spans="10:17" x14ac:dyDescent="0.25">
+      <c r="J88" s="12" t="s">
+        <v>461</v>
       </c>
       <c r="L88" s="12"/>
       <c r="M88" s="12"/>
       <c r="N88" s="12"/>
       <c r="O88" s="12"/>
-      <c r="P88" s="12"/>
-      <c r="Q88" s="12" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="89" spans="11:18" x14ac:dyDescent="0.25">
-      <c r="K89" s="12" t="s">
-        <v>460</v>
+    </row>
+    <row r="89" spans="10:17" x14ac:dyDescent="0.25">
+      <c r="J89" s="12" t="s">
+        <v>462</v>
       </c>
       <c r="L89" s="12"/>
       <c r="M89" s="12"/>
       <c r="N89" s="12"/>
       <c r="O89" s="12"/>
-      <c r="P89" s="12"/>
-      <c r="Q89" s="14" t="s">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="90" spans="11:18" x14ac:dyDescent="0.25">
-      <c r="K90" s="12" t="s">
-        <v>461</v>
+    </row>
+    <row r="90" spans="10:17" x14ac:dyDescent="0.25">
+      <c r="J90" s="12" t="s">
+        <v>463</v>
       </c>
       <c r="L90" s="12"/>
       <c r="M90" s="12"/>
       <c r="N90" s="12"/>
       <c r="O90" s="12"/>
-      <c r="P90" s="12"/>
-      <c r="Q90" s="14" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="91" spans="11:18" x14ac:dyDescent="0.25">
-      <c r="K91" s="12" t="s">
-        <v>462</v>
+    </row>
+    <row r="91" spans="10:17" x14ac:dyDescent="0.25">
+      <c r="J91" s="12" t="s">
+        <v>464</v>
       </c>
       <c r="L91" s="12"/>
       <c r="M91" s="12"/>
       <c r="N91" s="12"/>
       <c r="O91" s="12"/>
-      <c r="P91" s="12"/>
-      <c r="Q91" s="14" t="s">
-        <v>579</v>
-      </c>
-    </row>
-    <row r="92" spans="11:18" x14ac:dyDescent="0.25">
-      <c r="K92" s="12" t="s">
-        <v>463</v>
+    </row>
+    <row r="92" spans="10:17" x14ac:dyDescent="0.25">
+      <c r="J92" s="30" t="s">
+        <v>465</v>
       </c>
       <c r="L92" s="12"/>
       <c r="M92" s="12"/>
       <c r="N92" s="12"/>
       <c r="O92" s="12"/>
-      <c r="P92" s="12"/>
-      <c r="Q92" s="14" t="s">
-        <v>565</v>
-      </c>
-    </row>
-    <row r="93" spans="11:18" x14ac:dyDescent="0.25">
-      <c r="K93" s="28" t="s">
-        <v>464</v>
+    </row>
+    <row r="93" spans="10:17" x14ac:dyDescent="0.25">
+      <c r="J93" s="12" t="s">
+        <v>466</v>
       </c>
       <c r="L93" s="12"/>
       <c r="M93" s="12"/>
       <c r="N93" s="12"/>
       <c r="O93" s="12"/>
-      <c r="P93" s="12"/>
-      <c r="Q93" s="14" t="s">
-        <v>575</v>
-      </c>
-    </row>
-    <row r="94" spans="11:18" x14ac:dyDescent="0.25">
-      <c r="K94" s="12" t="s">
-        <v>465</v>
+    </row>
+    <row r="94" spans="10:17" x14ac:dyDescent="0.25">
+      <c r="J94" s="12" t="s">
+        <v>467</v>
       </c>
       <c r="L94" s="12"/>
       <c r="M94" s="12"/>
       <c r="N94" s="12"/>
       <c r="O94" s="12"/>
-      <c r="P94" s="12"/>
-      <c r="Q94" s="12" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="95" spans="11:18" x14ac:dyDescent="0.25">
-      <c r="K95" s="12" t="s">
-        <v>466</v>
+    </row>
+    <row r="95" spans="10:17" x14ac:dyDescent="0.25">
+      <c r="J95" s="30" t="s">
+        <v>468</v>
       </c>
       <c r="L95" s="12"/>
       <c r="M95" s="12"/>
       <c r="N95" s="12"/>
       <c r="O95" s="12"/>
-      <c r="P95" s="12"/>
-    </row>
-    <row r="96" spans="11:18" x14ac:dyDescent="0.25">
-      <c r="K96" s="28" t="s">
-        <v>467</v>
+    </row>
+    <row r="96" spans="10:17" x14ac:dyDescent="0.25">
+      <c r="J96" s="12" t="s">
+        <v>469</v>
       </c>
       <c r="L96" s="12"/>
       <c r="M96" s="12"/>
       <c r="N96" s="12"/>
       <c r="O96" s="12"/>
-      <c r="P96" s="12"/>
-    </row>
-    <row r="97" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="K97" s="12" t="s">
-        <v>468</v>
+    </row>
+    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J97" s="12" t="s">
+        <v>470</v>
       </c>
       <c r="L97" s="12"/>
       <c r="M97" s="12"/>
       <c r="N97" s="12"/>
       <c r="O97" s="12"/>
-      <c r="P97" s="12"/>
-    </row>
-    <row r="98" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="K98" s="12" t="s">
-        <v>469</v>
-      </c>
-      <c r="L98" s="12"/>
-    </row>
-    <row r="99" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="K99" s="28" t="s">
-        <v>470</v>
-      </c>
-      <c r="L99" s="12"/>
-    </row>
-    <row r="100" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="K100" s="12" t="s">
+    </row>
+    <row r="98" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J98" s="30" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="104" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J99" s="12" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="104" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B104" s="12" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="105" spans="1:16" x14ac:dyDescent="0.25">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="105" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A105" s="15" t="s">
         <v>143</v>
       </c>
@@ -6654,352 +6462,403 @@
         <v>361</v>
       </c>
       <c r="C105" s="21" t="s">
-        <v>416</v>
-      </c>
-      <c r="E105" s="29"/>
-      <c r="F105" s="29"/>
-    </row>
-    <row r="106" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B106" s="14" t="s">
+        <v>417</v>
+      </c>
+      <c r="E105" s="13" t="s">
+        <v>546</v>
+      </c>
+      <c r="F105" s="31" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="106" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B106" s="12" t="s">
         <v>41</v>
       </c>
       <c r="C106" s="21" t="s">
-        <v>404</v>
-      </c>
-      <c r="E106" s="29"/>
-      <c r="F106" s="29"/>
-    </row>
-    <row r="107" spans="1:16" x14ac:dyDescent="0.25">
+        <v>405</v>
+      </c>
+      <c r="E106" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="F106" s="10"/>
+    </row>
+    <row r="107" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B107" s="14" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="C107" s="21" t="s">
-        <v>405</v>
-      </c>
-      <c r="E107" s="29"/>
-      <c r="F107" s="29"/>
-    </row>
-    <row r="108" spans="1:16" x14ac:dyDescent="0.25">
+        <v>406</v>
+      </c>
+      <c r="E107" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="F107" s="10"/>
+    </row>
+    <row r="108" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B108" s="14" t="s">
         <v>50</v>
       </c>
       <c r="C108" s="21" t="s">
-        <v>406</v>
-      </c>
-      <c r="E108" s="29"/>
-      <c r="F108" s="29"/>
-    </row>
-    <row r="109" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B109" s="14" t="s">
+        <v>407</v>
+      </c>
+      <c r="E108" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="F108" s="10"/>
+    </row>
+    <row r="109" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B109" s="12" t="s">
         <v>83</v>
       </c>
       <c r="C109" s="21" t="s">
-        <v>407</v>
-      </c>
-      <c r="E109" s="29"/>
-      <c r="F109" s="29"/>
-    </row>
-    <row r="110" spans="1:16" x14ac:dyDescent="0.25">
+        <v>408</v>
+      </c>
+      <c r="E109" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="F109" s="10"/>
+    </row>
+    <row r="110" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B110" s="12" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="C110" s="21"/>
-      <c r="E110" s="29"/>
-      <c r="F110" s="29"/>
-    </row>
-    <row r="111" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="E110" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="F110" s="10"/>
+    </row>
+    <row r="111" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B111" s="14" t="s">
         <v>109</v>
       </c>
       <c r="C111" s="21"/>
-      <c r="E111" s="29"/>
-      <c r="F111" s="29"/>
-    </row>
-    <row r="112" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B112" s="14" t="s">
+      <c r="E111" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="F111" s="31" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="112" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B112" s="12" t="s">
         <v>88</v>
       </c>
       <c r="C112" s="21" t="s">
-        <v>408</v>
-      </c>
-      <c r="E112" s="29"/>
-      <c r="F112" s="29"/>
+        <v>409</v>
+      </c>
+      <c r="E112" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="F112" s="10"/>
     </row>
     <row r="113" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B113" s="12" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="C113" s="21"/>
-      <c r="E113" s="29"/>
-      <c r="F113" s="29"/>
+      <c r="E113" s="32" t="s">
+        <v>44</v>
+      </c>
+      <c r="F113" s="31" t="s">
+        <v>396</v>
+      </c>
     </row>
     <row r="114" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B114" s="14" t="s">
+      <c r="B114" s="12" t="s">
         <v>105</v>
       </c>
       <c r="C114" s="21" t="s">
-        <v>409</v>
-      </c>
-      <c r="E114" s="29"/>
-      <c r="F114" s="29"/>
+        <v>410</v>
+      </c>
+      <c r="E114" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="F114" s="31" t="s">
+        <v>397</v>
+      </c>
     </row>
     <row r="115" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B115" s="14" t="s">
+      <c r="B115" s="12" t="s">
         <v>77</v>
       </c>
       <c r="C115" s="21" t="s">
-        <v>407</v>
-      </c>
-      <c r="E115" s="29"/>
-      <c r="F115" s="29"/>
+        <v>408</v>
+      </c>
+      <c r="E115" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="F115" s="31" t="s">
+        <v>398</v>
+      </c>
     </row>
     <row r="116" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B116" s="14" t="s">
         <v>10</v>
       </c>
       <c r="C116" s="21" t="s">
-        <v>410</v>
-      </c>
-      <c r="E116" s="29"/>
-      <c r="F116" s="29"/>
+        <v>411</v>
+      </c>
+      <c r="E116" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="F116" s="10"/>
     </row>
     <row r="117" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B117" s="12" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="C117" s="21"/>
-      <c r="E117" s="29"/>
-      <c r="F117" s="29"/>
+      <c r="E117" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="F117" s="31" t="s">
+        <v>402</v>
+      </c>
     </row>
     <row r="118" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B118" s="14" t="s">
+      <c r="B118" s="12" t="s">
         <v>113</v>
       </c>
       <c r="C118" s="21" t="s">
-        <v>411</v>
-      </c>
-      <c r="E118" s="29"/>
-      <c r="F118" s="29"/>
+        <v>412</v>
+      </c>
+      <c r="E118" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="F118" s="31" t="s">
+        <v>403</v>
+      </c>
     </row>
     <row r="119" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B119" s="14" t="s">
         <v>26</v>
       </c>
       <c r="C119" s="21" t="s">
-        <v>405</v>
-      </c>
-      <c r="E119" s="29"/>
-      <c r="F119" s="29"/>
+        <v>406</v>
+      </c>
+      <c r="E119" s="10"/>
     </row>
     <row r="120" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B120" s="14" t="s">
         <v>47</v>
       </c>
       <c r="C120" s="21" t="s">
+        <v>407</v>
+      </c>
+      <c r="E120" s="13" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="121" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B121" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C121" s="21" t="s">
         <v>406</v>
       </c>
-      <c r="E120" s="29"/>
-      <c r="F120" s="29"/>
-    </row>
-    <row r="121" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B121" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="C121" s="21" t="s">
-        <v>405</v>
-      </c>
-      <c r="E121" s="29"/>
-      <c r="F121" s="29"/>
+      <c r="E121" s="13" t="s">
+        <v>400</v>
+      </c>
     </row>
     <row r="122" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B122" s="14" t="s">
         <v>81</v>
       </c>
       <c r="C122" s="21" t="s">
-        <v>407</v>
-      </c>
-      <c r="E122" s="29"/>
-      <c r="F122" s="29"/>
+        <v>408</v>
+      </c>
+      <c r="E122" s="13" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="123" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B123" s="14" t="s">
         <v>69</v>
       </c>
       <c r="C123" s="21" t="s">
-        <v>412</v>
-      </c>
-      <c r="E123" s="29"/>
-      <c r="F123" s="29"/>
+        <v>413</v>
+      </c>
+      <c r="E123" s="13" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="124" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B124" s="14" t="s">
         <v>29</v>
       </c>
       <c r="C124" s="21" t="s">
-        <v>405</v>
-      </c>
-      <c r="E124" s="29"/>
-      <c r="F124" s="29"/>
+        <v>406</v>
+      </c>
+      <c r="E124" s="13" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="125" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B125" s="12" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="C125" s="21"/>
-      <c r="E125" s="29"/>
-      <c r="F125" s="29"/>
+      <c r="E125" s="13" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="126" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B126" s="14" t="s">
+      <c r="B126" s="12" t="s">
         <v>44</v>
       </c>
       <c r="C126" s="21" t="s">
-        <v>406</v>
-      </c>
-      <c r="E126" s="29"/>
-      <c r="F126" s="29"/>
+        <v>407</v>
+      </c>
+      <c r="E126" s="13" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="127" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B127" s="14" t="s">
+      <c r="B127" s="12" t="s">
         <v>82</v>
       </c>
       <c r="C127" s="21" t="s">
-        <v>407</v>
-      </c>
-      <c r="E127" s="29"/>
-      <c r="F127" s="29"/>
+        <v>408</v>
+      </c>
+      <c r="E127" s="13" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="128" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B128" s="14" t="s">
         <v>100</v>
       </c>
       <c r="C128" s="21" t="s">
-        <v>409</v>
-      </c>
-      <c r="E128" s="29"/>
-      <c r="F128" s="29"/>
-    </row>
-    <row r="129" spans="2:6" x14ac:dyDescent="0.25">
+        <v>410</v>
+      </c>
+      <c r="E128" s="32" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="129" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B129" s="14" t="s">
         <v>53</v>
       </c>
       <c r="C129" s="21" t="s">
-        <v>413</v>
-      </c>
-      <c r="E129" s="29"/>
-      <c r="F129" s="29"/>
-    </row>
-    <row r="130" spans="2:6" x14ac:dyDescent="0.25">
+        <v>414</v>
+      </c>
+      <c r="E129" s="13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="130" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B130" s="14" t="s">
         <v>76</v>
       </c>
       <c r="C130" s="21" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="131" spans="2:6" x14ac:dyDescent="0.25">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="131" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B131" s="14" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="C131" s="21" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="132" spans="2:6" x14ac:dyDescent="0.25">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="132" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B132" s="12" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="C132" s="21"/>
     </row>
-    <row r="133" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B133" s="12" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="C133" s="21"/>
     </row>
-    <row r="134" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B134" s="12" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="C134" s="21"/>
     </row>
-    <row r="135" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B135" s="14" t="s">
+    <row r="135" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B135" s="12" t="s">
         <v>66</v>
       </c>
       <c r="C135" s="21" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="136" spans="2:6" x14ac:dyDescent="0.25">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="136" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B136" s="14" t="s">
         <v>27</v>
       </c>
       <c r="C136" s="21" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="137" spans="2:6" x14ac:dyDescent="0.25">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="137" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B137" s="12" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="C137" s="21"/>
     </row>
-    <row r="138" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B138" s="14" t="s">
+    <row r="138" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B138" s="12" t="s">
         <v>59</v>
       </c>
       <c r="C138" s="21" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="139" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B139" s="14" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="139" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B139" s="12" t="s">
         <v>79</v>
       </c>
       <c r="C139" s="21" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="140" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B140" s="14" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="140" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B140" s="12" t="s">
         <v>103</v>
       </c>
       <c r="C140" s="21" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="141" spans="2:6" x14ac:dyDescent="0.25">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="141" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B141" s="14" t="s">
         <v>108</v>
       </c>
       <c r="C141" s="21" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="142" spans="2:6" x14ac:dyDescent="0.25">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="142" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B142" s="12" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="C142" s="21"/>
     </row>
-    <row r="143" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="143" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B143" s="12" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="C143" s="21"/>
     </row>
-    <row r="144" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B144" s="12" t="s">
         <v>37</v>
       </c>
       <c r="C144" s="21" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
     </row>
     <row r="145" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B145" s="14" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="C145" s="21"/>
     </row>
@@ -7008,31 +6867,31 @@
         <v>93</v>
       </c>
       <c r="C146" s="21" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="147" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B147" s="14" t="s">
+      <c r="B147" s="12" t="s">
         <v>97</v>
       </c>
       <c r="C147" s="21" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="148" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B148" s="14" t="s">
-        <v>399</v>
+      <c r="B148" s="12" t="s">
+        <v>400</v>
       </c>
       <c r="C148" s="21" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="149" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B149" s="14" t="s">
+      <c r="B149" s="12" t="s">
         <v>94</v>
       </c>
       <c r="C149" s="21" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="150" spans="2:3" x14ac:dyDescent="0.25">
@@ -7040,29 +6899,29 @@
         <v>36</v>
       </c>
       <c r="C150" s="21" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
     </row>
     <row r="151" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B151" s="14" t="s">
+      <c r="B151" s="12" t="s">
         <v>42</v>
       </c>
       <c r="C151" s="21" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
     </row>
     <row r="152" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B152" s="12" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="C152" s="21"/>
     </row>
     <row r="153" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B153" s="14" t="s">
+      <c r="B153" s="12" t="s">
         <v>101</v>
       </c>
       <c r="C153" s="21" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="154" spans="2:3" x14ac:dyDescent="0.25">
@@ -7070,37 +6929,37 @@
         <v>107</v>
       </c>
       <c r="C154" s="21" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
     </row>
     <row r="155" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B155" s="14" t="s">
+      <c r="B155" s="12" t="s">
         <v>95</v>
       </c>
       <c r="C155" s="21" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="156" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B156" s="12" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="C156" s="21"/>
     </row>
     <row r="157" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B157" s="14" t="s">
+      <c r="B157" s="12" t="s">
         <v>102</v>
       </c>
       <c r="C157" s="21" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="158" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B158" s="14" t="s">
+      <c r="B158" s="12" t="s">
         <v>98</v>
       </c>
       <c r="C158" s="21" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="159" spans="2:3" x14ac:dyDescent="0.25">
@@ -7108,7 +6967,7 @@
         <v>96</v>
       </c>
       <c r="C159" s="21" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="160" spans="2:3" x14ac:dyDescent="0.25">
@@ -7116,7 +6975,7 @@
         <v>99</v>
       </c>
       <c r="C160" s="21" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="161" spans="2:3" x14ac:dyDescent="0.25">
@@ -7124,26 +6983,26 @@
         <v>46</v>
       </c>
       <c r="C161" s="21" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
     </row>
     <row r="162" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B162" s="14" t="s">
+      <c r="B162" s="12" t="s">
         <v>39</v>
       </c>
       <c r="C162" s="21" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
     </row>
     <row r="163" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B163" s="12" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C163" s="21"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="K57:K99">
-    <sortCondition ref="K99"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="J57:J99">
+    <sortCondition ref="J99"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>